<commit_message>
Add uncappedAmount to StakerIncentivesCalculator output, handle json writing, generic for UserRewardEntry type, 2wk config incentive, commit output json (and xlsx which is todo)
</commit_message>
<xml_diff>
--- a/staker_incentives.xlsx
+++ b/staker_incentives.xlsx
@@ -4,6 +4,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
     <sheet name="Blocks 68093124 - 68374032" sheetId="1" r:id="rId1"/>
+    <sheet name="Blocks 68093124 - 68655289" sheetId="2" r:id="rId2"/>
   </sheets>
 </workbook>
 </file>
@@ -399,7 +400,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C90"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -1397,4 +1398,975 @@
     <ignoredError numberStoredAsText="1" sqref="A1:C90"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C87"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>address</v>
+      </c>
+      <c r="B1" t="str">
+        <v>incentive - script output</v>
+      </c>
+      <c r="C1" t="str">
+        <v>incentive (TEL)</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>0xAcF543A44c24aAdF47B50e5cc05c628f3F2A5046</v>
+      </c>
+      <c r="B2">
+        <v>NaN</v>
+      </c>
+      <c r="C2">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>0xE3060D70A15f2EdFb390D66e60467Da6F5ECA1C7</v>
+      </c>
+      <c r="B3">
+        <v>NaN</v>
+      </c>
+      <c r="C3">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>0x426d787930A93314048488c4D10946FCeD265Cc7</v>
+      </c>
+      <c r="B4">
+        <v>NaN</v>
+      </c>
+      <c r="C4">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>0x096454fa85d4bD21CBB9134966c417f2e40C288C</v>
+      </c>
+      <c r="B5">
+        <v>NaN</v>
+      </c>
+      <c r="C5">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>0xaE8f06402E8e67023b13f2F132Dc34422aFA6189</v>
+      </c>
+      <c r="B6">
+        <v>NaN</v>
+      </c>
+      <c r="C6">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>0xc1c106e16cF229be127C30406c598b07986c06BA</v>
+      </c>
+      <c r="B7">
+        <v>NaN</v>
+      </c>
+      <c r="C7">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>0x5B74F5c8A2C00fea77cAED166Eb4F71BCe7d38bC</v>
+      </c>
+      <c r="B8">
+        <v>NaN</v>
+      </c>
+      <c r="C8">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>0xe05DDFB83A8b66Df42f06BfB5517Fb5d6857a8ce</v>
+      </c>
+      <c r="B9">
+        <v>NaN</v>
+      </c>
+      <c r="C9">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>0x16CaEA275D4F7cF454537b121915D92Bc5CB8C16</v>
+      </c>
+      <c r="B10">
+        <v>NaN</v>
+      </c>
+      <c r="C10">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>0x7308fC774925316052AD22Fbdc21f2a7FF4bDA49</v>
+      </c>
+      <c r="B11">
+        <v>NaN</v>
+      </c>
+      <c r="C11">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>0x721D683cBd00c78Eb2676fBA03e8c03FDF07f5dC</v>
+      </c>
+      <c r="B12">
+        <v>NaN</v>
+      </c>
+      <c r="C12">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>0x82983a034CD8811b62fbdEcDEb300b46947fCC45</v>
+      </c>
+      <c r="B13">
+        <v>NaN</v>
+      </c>
+      <c r="C13">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>0xff9aE836c989360f013A4d2F184b5f7e59aD6C11</v>
+      </c>
+      <c r="B14">
+        <v>NaN</v>
+      </c>
+      <c r="C14">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>0x9C4e5edC6A735e4AB68ef04497b64008A955A1A5</v>
+      </c>
+      <c r="B15">
+        <v>NaN</v>
+      </c>
+      <c r="C15">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>0xC090D9F71184D03568485a351456C570ff9F9Cbf</v>
+      </c>
+      <c r="B16">
+        <v>NaN</v>
+      </c>
+      <c r="C16">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>0xFb55bcB2E843Cc2dA95c48273eA89F167Faf7b93</v>
+      </c>
+      <c r="B17">
+        <v>NaN</v>
+      </c>
+      <c r="C17">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>0xb26C7c04A98eb3b92a2688ee8Fc1dA17054eF909</v>
+      </c>
+      <c r="B18">
+        <v>NaN</v>
+      </c>
+      <c r="C18">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>0xd685199C3Bfc7DD24d7E4A6bfD17dCa2bBF2F57d</v>
+      </c>
+      <c r="B19">
+        <v>NaN</v>
+      </c>
+      <c r="C19">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>0x8218E1a9D02E26E2aF124EA28b121031Cf25AaC8</v>
+      </c>
+      <c r="B20">
+        <v>NaN</v>
+      </c>
+      <c r="C20">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>0xd9C0e53199290dF3BFB223033f3eb6C16429af0e</v>
+      </c>
+      <c r="B21">
+        <v>NaN</v>
+      </c>
+      <c r="C21">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>0xdFdf143A6a12185023e01ddC61092Ac97eCB6c05</v>
+      </c>
+      <c r="B22">
+        <v>NaN</v>
+      </c>
+      <c r="C22">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>0x0603709F92A47D5367Cc93f5b587A29fA286ADbB</v>
+      </c>
+      <c r="B23">
+        <v>NaN</v>
+      </c>
+      <c r="C23">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>0xb8e441ad9cA68bf92Da52A40BFBb03Bc6454ABB4</v>
+      </c>
+      <c r="B24">
+        <v>NaN</v>
+      </c>
+      <c r="C24">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>0x9B73f16958aD4dF607E8B58aA2f407d66e9FA543</v>
+      </c>
+      <c r="B25">
+        <v>NaN</v>
+      </c>
+      <c r="C25">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>0x681ee9C08368ED5e30519f146cF3A27b24471Dc6</v>
+      </c>
+      <c r="B26">
+        <v>NaN</v>
+      </c>
+      <c r="C26">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>0xF197552b64740Ff554D2887B59CD299d7b853Df3</v>
+      </c>
+      <c r="B27">
+        <v>NaN</v>
+      </c>
+      <c r="C27">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>0xe2e039dD3206870FE6Ad4B88DDf74730c355B2e5</v>
+      </c>
+      <c r="B28">
+        <v>NaN</v>
+      </c>
+      <c r="C28">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>0x77940861e000BfC8A8f67440ad21656B9e7dbA04</v>
+      </c>
+      <c r="B29">
+        <v>NaN</v>
+      </c>
+      <c r="C29">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>0x6BF81D0d4f4e606C3cB09C45f6FA29f8743c72DE</v>
+      </c>
+      <c r="B30">
+        <v>NaN</v>
+      </c>
+      <c r="C30">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>0x74c0d21e8ffC5b83dce1A0BB6abCD061D071E85a</v>
+      </c>
+      <c r="B31">
+        <v>NaN</v>
+      </c>
+      <c r="C31">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>0xD7Be7655070f986B3E311EE04cc9aa87Cd11ab5d</v>
+      </c>
+      <c r="B32">
+        <v>NaN</v>
+      </c>
+      <c r="C32">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>0xe5C5B9C648a3e66A2A7b8a3f2dA48e76e8309A2C</v>
+      </c>
+      <c r="B33">
+        <v>NaN</v>
+      </c>
+      <c r="C33">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>0x262ba7354bA2946de8f90dCe06883FaFebB6f043</v>
+      </c>
+      <c r="B34">
+        <v>NaN</v>
+      </c>
+      <c r="C34">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>0x4DF1C6c7973f4E6e3B22149f7b8eFc4389f97C56</v>
+      </c>
+      <c r="B35">
+        <v>NaN</v>
+      </c>
+      <c r="C35">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>0x3d1F678EBd71CA033f21D6B1B5B0781a66537447</v>
+      </c>
+      <c r="B36">
+        <v>NaN</v>
+      </c>
+      <c r="C36">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>0xB6e85e12331BdEA6fF03b25d3dE68a892C99C5D4</v>
+      </c>
+      <c r="B37">
+        <v>NaN</v>
+      </c>
+      <c r="C37">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>0xE2D8A9f98072298241651a1c899907892860A1f5</v>
+      </c>
+      <c r="B38">
+        <v>NaN</v>
+      </c>
+      <c r="C38">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>0xb91406Ea49418Ff04F73231BA48930278bCef631</v>
+      </c>
+      <c r="B39">
+        <v>NaN</v>
+      </c>
+      <c r="C39">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>0x040f62A18EB5D5ca87A08E41A22D004ee7A26380</v>
+      </c>
+      <c r="B40">
+        <v>NaN</v>
+      </c>
+      <c r="C40">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>0x18fc6c299B7aA35C8f59537b4b67c23D93E782ea</v>
+      </c>
+      <c r="B41">
+        <v>NaN</v>
+      </c>
+      <c r="C41">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>0x5C9A07e59Bdc264d0579530b4e08338122833942</v>
+      </c>
+      <c r="B42">
+        <v>NaN</v>
+      </c>
+      <c r="C42">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>0x4994A7059A2921398780818c203F83613A9Bf743</v>
+      </c>
+      <c r="B43">
+        <v>NaN</v>
+      </c>
+      <c r="C43">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>0xe9052daAC8667a27B38369aD37BEE63A8CD80Fc7</v>
+      </c>
+      <c r="B44">
+        <v>NaN</v>
+      </c>
+      <c r="C44">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>0x8f437d47c7723C7AB5ab896D59549D547181BecB</v>
+      </c>
+      <c r="B45">
+        <v>NaN</v>
+      </c>
+      <c r="C45">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>0xA742150Bb2b4e5DfCC4E6df0E577237Fceb797b2</v>
+      </c>
+      <c r="B46">
+        <v>NaN</v>
+      </c>
+      <c r="C46">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>0x9D89f9451C4B7e04bd58616dbC72e924088AFF21</v>
+      </c>
+      <c r="B47">
+        <v>NaN</v>
+      </c>
+      <c r="C47">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>0x94B72396b6B40e19C2a04c28c8aE93dE08b12733</v>
+      </c>
+      <c r="B48">
+        <v>NaN</v>
+      </c>
+      <c r="C48">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>0x4CaFc8E23616346de04DE62174B1e615D8E80c70</v>
+      </c>
+      <c r="B49">
+        <v>NaN</v>
+      </c>
+      <c r="C49">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>0x6f9A5457e35FF98FCcA68b71c2D1bf7aAAeB714E</v>
+      </c>
+      <c r="B50">
+        <v>NaN</v>
+      </c>
+      <c r="C50">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>0x0b3d82e9b1D9163a1fe71DC2bc60C6Fb7fb13863</v>
+      </c>
+      <c r="B51">
+        <v>NaN</v>
+      </c>
+      <c r="C51">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>0xb12042f547d28da37E88d7Db7A2CBAaf8CD88F68</v>
+      </c>
+      <c r="B52">
+        <v>NaN</v>
+      </c>
+      <c r="C52">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>0xDF6F220E72A6320E87576c5075899Be34212f97D</v>
+      </c>
+      <c r="B53">
+        <v>NaN</v>
+      </c>
+      <c r="C53">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>0x3E3309ab5312f6875b6e9bE672b9A43EFb70D760</v>
+      </c>
+      <c r="B54">
+        <v>NaN</v>
+      </c>
+      <c r="C54">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>0x47502539673c93B2ACDC9059B36360f76D3548BB</v>
+      </c>
+      <c r="B55">
+        <v>NaN</v>
+      </c>
+      <c r="C55">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>0x0254704C23C4765496894a632ef28d6be4DCB259</v>
+      </c>
+      <c r="B56">
+        <v>NaN</v>
+      </c>
+      <c r="C56">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>0x2EeCd56c9A00E81a393Fd24F22a07C9D80336E20</v>
+      </c>
+      <c r="B57">
+        <v>NaN</v>
+      </c>
+      <c r="C57">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>0x2abf42F330c60491E8A36B73c9F3F9Ed40CDa546</v>
+      </c>
+      <c r="B58">
+        <v>NaN</v>
+      </c>
+      <c r="C58">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>0x66B6221845b9bd7A029BCCb5523168a5AcE1e013</v>
+      </c>
+      <c r="B59">
+        <v>NaN</v>
+      </c>
+      <c r="C59">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>0x331B6287b04a4Bb359C75D102a2104561BB84fe3</v>
+      </c>
+      <c r="B60">
+        <v>NaN</v>
+      </c>
+      <c r="C60">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>0x2A1Cc6c77782EA6BE6C08d61430A79E31Ea4efDf</v>
+      </c>
+      <c r="B61">
+        <v>NaN</v>
+      </c>
+      <c r="C61">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>0x417eD74e3904f2C2d2eBb4e8050bD772374bd82a</v>
+      </c>
+      <c r="B62">
+        <v>NaN</v>
+      </c>
+      <c r="C62">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>0x746F83FF7eAdA9d0fB03DbAbcAF2600ee513DCDB</v>
+      </c>
+      <c r="B63">
+        <v>NaN</v>
+      </c>
+      <c r="C63">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>0x733e103A702EACEa3189361a3b79902491FBACd1</v>
+      </c>
+      <c r="B64">
+        <v>NaN</v>
+      </c>
+      <c r="C64">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>0xE17Aa7A67B0834823F56f01260b1E0965f14Eb4c</v>
+      </c>
+      <c r="B65">
+        <v>NaN</v>
+      </c>
+      <c r="C65">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v>0x7011467e458B4cEEED928bac3E178Ce7EB892F2d</v>
+      </c>
+      <c r="B66">
+        <v>NaN</v>
+      </c>
+      <c r="C66">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="str">
+        <v>0x469E40f0854EC0E8FaC1Afd4Af2DFfD5aE5569B0</v>
+      </c>
+      <c r="B67">
+        <v>NaN</v>
+      </c>
+      <c r="C67">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="str">
+        <v>0x21a18db5749f090BB96DE151de4136866cdAC8DF</v>
+      </c>
+      <c r="B68">
+        <v>NaN</v>
+      </c>
+      <c r="C68">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="str">
+        <v>0xe6eaa2b28ce4b4064E37eF290E82de53Fd81C211</v>
+      </c>
+      <c r="B69">
+        <v>NaN</v>
+      </c>
+      <c r="C69">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="str">
+        <v>0x3010A4E7ce5c99208900c218d0375bfEfE7De269</v>
+      </c>
+      <c r="B70">
+        <v>NaN</v>
+      </c>
+      <c r="C70">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v>0x430cB4360cE341a6Ad0Dfa18b9aD1Ae2cFa9AD18</v>
+      </c>
+      <c r="B71">
+        <v>NaN</v>
+      </c>
+      <c r="C71">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>0x8fa6e6dB6B86d0Cad2fa8DeEb737BC1cB97a2bE1</v>
+      </c>
+      <c r="B72">
+        <v>NaN</v>
+      </c>
+      <c r="C72">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>0x8364044ee8062F0F6C9835f7dfC26da4CE433BB8</v>
+      </c>
+      <c r="B73">
+        <v>NaN</v>
+      </c>
+      <c r="C73">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>0x9fF7d51Cf6a3A12F2Cdd36035827037a35A4B139</v>
+      </c>
+      <c r="B74">
+        <v>NaN</v>
+      </c>
+      <c r="C74">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>0x8B66c0aEEc3a231F6e3302dBb7d351B5c7B094B0</v>
+      </c>
+      <c r="B75">
+        <v>NaN</v>
+      </c>
+      <c r="C75">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>0xD81F1cF201B68a9EA0E8f10b1864DFE925202643</v>
+      </c>
+      <c r="B76">
+        <v>NaN</v>
+      </c>
+      <c r="C76">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v>0x20944C8A17cfa6cb96556116037e3aEeB506a0b0</v>
+      </c>
+      <c r="B77">
+        <v>NaN</v>
+      </c>
+      <c r="C77">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="str">
+        <v>0x61cD23Cf91d9B6BBb4bFF28c6AD7B667C7EC6367</v>
+      </c>
+      <c r="B78">
+        <v>NaN</v>
+      </c>
+      <c r="C78">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="str">
+        <v>0xEA67438f0857e93968F50aE87db18720b9E457Ef</v>
+      </c>
+      <c r="B79">
+        <v>NaN</v>
+      </c>
+      <c r="C79">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="str">
+        <v>0x8f1928e8FEa7238b9B53A7E62AFd471b69732a66</v>
+      </c>
+      <c r="B80">
+        <v>NaN</v>
+      </c>
+      <c r="C80">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="str">
+        <v>0x5390651dd0824159FE0e82554feC7b283bCa3745</v>
+      </c>
+      <c r="B81">
+        <v>NaN</v>
+      </c>
+      <c r="C81">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="str">
+        <v>0xf33639F5c9cDB8E242c3E20Fdaf98Ae389f0e399</v>
+      </c>
+      <c r="B82">
+        <v>NaN</v>
+      </c>
+      <c r="C82">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="str">
+        <v>0x0116c14c39b5a5ecD03193E56E975064b4a405D2</v>
+      </c>
+      <c r="B83">
+        <v>NaN</v>
+      </c>
+      <c r="C83">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="str">
+        <v>0xbD73E24F927E9f1D9ce45B7e47f36711Dca35A88</v>
+      </c>
+      <c r="B84">
+        <v>NaN</v>
+      </c>
+      <c r="C84">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="str">
+        <v>0xb05822516a701573678447E6966F7eD3bdDf78C5</v>
+      </c>
+      <c r="B85">
+        <v>NaN</v>
+      </c>
+      <c r="C85">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="str">
+        <v>0xBBBA5cae882A16fEdAD9a92220C7dBF2d9Eb2313</v>
+      </c>
+      <c r="B86">
+        <v>NaN</v>
+      </c>
+      <c r="C86">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="str">
+        <v>Total</v>
+      </c>
+      <c r="B87">
+        <v>NaN</v>
+      </c>
+      <c r="C87" t="str">
+        <v>NaN</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:C87"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Excel minimalism: single source of truth excel file
</commit_message>
<xml_diff>
--- a/staker_incentives.xlsx
+++ b/staker_incentives.xlsx
@@ -3,9 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Blocks 68093124 - 68655289" sheetId="1" r:id="rId1"/>
-    <sheet name="Blocks 68093124 - 68374032" sheetId="2" r:id="rId2"/>
-    <sheet name="Blocks 68374032 - 68655289" sheetId="3" r:id="rId3"/>
+    <sheet name="Blocks 68093124 - 68374032" sheetId="1" r:id="rId1"/>
+    <sheet name="Blocks 68374032 - 68655289" sheetId="2" r:id="rId2"/>
   </sheets>
 </workbook>
 </file>
@@ -399,1499 +398,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E87"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>address</v>
-      </c>
-      <c r="B1" t="str">
-        <v>incentive - script output</v>
-      </c>
-      <c r="C1" t="str">
-        <v>incentive (TEL)</v>
-      </c>
-      <c r="D1" t="str">
-        <v>uncapped amount - script output</v>
-      </c>
-      <c r="E1" t="str">
-        <v>uncapped amount (TEL)</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>0xAcF543A44c24aAdF47B50e5cc05c628f3F2A5046</v>
-      </c>
-      <c r="B2">
-        <v>26898709</v>
-      </c>
-      <c r="C2" t="str">
-        <v>268,987.09</v>
-      </c>
-      <c r="D2">
-        <v>26898709</v>
-      </c>
-      <c r="E2" t="str">
-        <v>268,987.09</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>0xE3060D70A15f2EdFb390D66e60467Da6F5ECA1C7</v>
-      </c>
-      <c r="B3">
-        <v>140273</v>
-      </c>
-      <c r="C3" t="str">
-        <v>1,402.73</v>
-      </c>
-      <c r="D3">
-        <v>140273</v>
-      </c>
-      <c r="E3" t="str">
-        <v>1,402.73</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>0x426d787930A93314048488c4D10946FCeD265Cc7</v>
-      </c>
-      <c r="B4">
-        <v>13963745</v>
-      </c>
-      <c r="C4" t="str">
-        <v>139,637.45</v>
-      </c>
-      <c r="D4">
-        <v>13963745</v>
-      </c>
-      <c r="E4" t="str">
-        <v>139,637.45</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>0x096454fa85d4bD21CBB9134966c417f2e40C288C</v>
-      </c>
-      <c r="B5">
-        <v>2350333</v>
-      </c>
-      <c r="C5" t="str">
-        <v>23,503.33</v>
-      </c>
-      <c r="D5">
-        <v>2350333</v>
-      </c>
-      <c r="E5" t="str">
-        <v>23,503.33</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>0xaE8f06402E8e67023b13f2F132Dc34422aFA6189</v>
-      </c>
-      <c r="B6">
-        <v>1493</v>
-      </c>
-      <c r="C6" t="str">
-        <v>14.93</v>
-      </c>
-      <c r="D6">
-        <v>1493</v>
-      </c>
-      <c r="E6" t="str">
-        <v>14.93</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>0xc1c106e16cF229be127C30406c598b07986c06BA</v>
-      </c>
-      <c r="B7">
-        <v>4253163</v>
-      </c>
-      <c r="C7" t="str">
-        <v>42,531.63</v>
-      </c>
-      <c r="D7">
-        <v>4253163</v>
-      </c>
-      <c r="E7" t="str">
-        <v>42,531.63</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>0x5B74F5c8A2C00fea77cAED166Eb4F71BCe7d38bC</v>
-      </c>
-      <c r="B8">
-        <v>55495</v>
-      </c>
-      <c r="C8" t="str">
-        <v>554.95</v>
-      </c>
-      <c r="D8">
-        <v>55495</v>
-      </c>
-      <c r="E8" t="str">
-        <v>554.95</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>0xe05DDFB83A8b66Df42f06BfB5517Fb5d6857a8ce</v>
-      </c>
-      <c r="B9">
-        <v>7850777</v>
-      </c>
-      <c r="C9" t="str">
-        <v>78,507.77</v>
-      </c>
-      <c r="D9">
-        <v>7850777</v>
-      </c>
-      <c r="E9" t="str">
-        <v>78,507.77</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>0x16CaEA275D4F7cF454537b121915D92Bc5CB8C16</v>
-      </c>
-      <c r="B10">
-        <v>1292683</v>
-      </c>
-      <c r="C10" t="str">
-        <v>12,926.83</v>
-      </c>
-      <c r="D10">
-        <v>1292683</v>
-      </c>
-      <c r="E10" t="str">
-        <v>12,926.83</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>0x7308fC774925316052AD22Fbdc21f2a7FF4bDA49</v>
-      </c>
-      <c r="B11">
-        <v>6947309</v>
-      </c>
-      <c r="C11" t="str">
-        <v>69,473.09</v>
-      </c>
-      <c r="D11">
-        <v>6947309</v>
-      </c>
-      <c r="E11" t="str">
-        <v>69,473.09</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v>0x721D683cBd00c78Eb2676fBA03e8c03FDF07f5dC</v>
-      </c>
-      <c r="B12">
-        <v>4147647</v>
-      </c>
-      <c r="C12" t="str">
-        <v>41,476.47</v>
-      </c>
-      <c r="D12">
-        <v>4147647</v>
-      </c>
-      <c r="E12" t="str">
-        <v>41,476.47</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="str">
-        <v>0x82983a034CD8811b62fbdEcDEb300b46947fCC45</v>
-      </c>
-      <c r="B13">
-        <v>2115300</v>
-      </c>
-      <c r="C13" t="str">
-        <v>21,153</v>
-      </c>
-      <c r="D13">
-        <v>2115300</v>
-      </c>
-      <c r="E13" t="str">
-        <v>21,153</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="str">
-        <v>0xff9aE836c989360f013A4d2F184b5f7e59aD6C11</v>
-      </c>
-      <c r="B14">
-        <v>357739</v>
-      </c>
-      <c r="C14" t="str">
-        <v>3,577.39</v>
-      </c>
-      <c r="D14">
-        <v>6912745</v>
-      </c>
-      <c r="E14" t="str">
-        <v>69,127.45</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="str">
-        <v>0x9C4e5edC6A735e4AB68ef04497b64008A955A1A5</v>
-      </c>
-      <c r="B15">
-        <v>557554</v>
-      </c>
-      <c r="C15" t="str">
-        <v>5,575.54</v>
-      </c>
-      <c r="D15">
-        <v>557554</v>
-      </c>
-      <c r="E15" t="str">
-        <v>5,575.54</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="str">
-        <v>0xC090D9F71184D03568485a351456C570ff9F9Cbf</v>
-      </c>
-      <c r="B16">
-        <v>81515</v>
-      </c>
-      <c r="C16" t="str">
-        <v>815.15</v>
-      </c>
-      <c r="D16">
-        <v>81515</v>
-      </c>
-      <c r="E16" t="str">
-        <v>815.15</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="str">
-        <v>0xFb55bcB2E843Cc2dA95c48273eA89F167Faf7b93</v>
-      </c>
-      <c r="B17">
-        <v>20738236</v>
-      </c>
-      <c r="C17" t="str">
-        <v>207,382.36</v>
-      </c>
-      <c r="D17">
-        <v>20738236</v>
-      </c>
-      <c r="E17" t="str">
-        <v>207,382.36</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="str">
-        <v>0xb26C7c04A98eb3b92a2688ee8Fc1dA17054eF909</v>
-      </c>
-      <c r="B18">
-        <v>711874</v>
-      </c>
-      <c r="C18" t="str">
-        <v>7,118.74</v>
-      </c>
-      <c r="D18">
-        <v>711874</v>
-      </c>
-      <c r="E18" t="str">
-        <v>7,118.74</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="str">
-        <v>0xd685199C3Bfc7DD24d7E4A6bfD17dCa2bBF2F57d</v>
-      </c>
-      <c r="B19">
-        <v>13825491</v>
-      </c>
-      <c r="C19" t="str">
-        <v>138,254.91</v>
-      </c>
-      <c r="D19">
-        <v>13825491</v>
-      </c>
-      <c r="E19" t="str">
-        <v>138,254.91</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="str">
-        <v>0x8218E1a9D02E26E2aF124EA28b121031Cf25AaC8</v>
-      </c>
-      <c r="B20">
-        <v>276509</v>
-      </c>
-      <c r="C20" t="str">
-        <v>2,765.09</v>
-      </c>
-      <c r="D20">
-        <v>276509</v>
-      </c>
-      <c r="E20" t="str">
-        <v>2,765.09</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="str">
-        <v>0xd9C0e53199290dF3BFB223033f3eb6C16429af0e</v>
-      </c>
-      <c r="B21">
-        <v>414764</v>
-      </c>
-      <c r="C21" t="str">
-        <v>4,147.64</v>
-      </c>
-      <c r="D21">
-        <v>414764</v>
-      </c>
-      <c r="E21" t="str">
-        <v>4,147.64</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="str">
-        <v>0xdFdf143A6a12185023e01ddC61092Ac97eCB6c05</v>
-      </c>
-      <c r="B22">
-        <v>691274</v>
-      </c>
-      <c r="C22" t="str">
-        <v>6,912.74</v>
-      </c>
-      <c r="D22">
-        <v>691274</v>
-      </c>
-      <c r="E22" t="str">
-        <v>6,912.74</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="str">
-        <v>0x0603709F92A47D5367Cc93f5b587A29fA286ADbB</v>
-      </c>
-      <c r="B23">
-        <v>5128704</v>
-      </c>
-      <c r="C23" t="str">
-        <v>51,287.04</v>
-      </c>
-      <c r="D23">
-        <v>5128704</v>
-      </c>
-      <c r="E23" t="str">
-        <v>51,287.04</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="str">
-        <v>0xb8e441ad9cA68bf92Da52A40BFBb03Bc6454ABB4</v>
-      </c>
-      <c r="B24">
-        <v>21429511</v>
-      </c>
-      <c r="C24" t="str">
-        <v>214,295.11</v>
-      </c>
-      <c r="D24">
-        <v>21429511</v>
-      </c>
-      <c r="E24" t="str">
-        <v>214,295.11</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="str">
-        <v>0x9B73f16958aD4dF607E8B58aA2f407d66e9FA543</v>
-      </c>
-      <c r="B25">
-        <v>69127</v>
-      </c>
-      <c r="C25" t="str">
-        <v>691.27</v>
-      </c>
-      <c r="D25">
-        <v>69127</v>
-      </c>
-      <c r="E25" t="str">
-        <v>691.27</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="str">
-        <v>0x681ee9C08368ED5e30519f146cF3A27b24471Dc6</v>
-      </c>
-      <c r="B26">
-        <v>1890</v>
-      </c>
-      <c r="C26" t="str">
-        <v>18.9</v>
-      </c>
-      <c r="D26">
-        <v>69127</v>
-      </c>
-      <c r="E26" t="str">
-        <v>691.27</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="str">
-        <v>0xF197552b64740Ff554D2887B59CD299d7b853Df3</v>
-      </c>
-      <c r="B27">
-        <v>1001000</v>
-      </c>
-      <c r="C27" t="str">
-        <v>10,010</v>
-      </c>
-      <c r="D27">
-        <v>98160986</v>
-      </c>
-      <c r="E27" t="str">
-        <v>981,609.86</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="str">
-        <v>0xe2e039dD3206870FE6Ad4B88DDf74730c355B2e5</v>
-      </c>
-      <c r="B28">
-        <v>152080</v>
-      </c>
-      <c r="C28" t="str">
-        <v>1,520.8</v>
-      </c>
-      <c r="D28">
-        <v>152080</v>
-      </c>
-      <c r="E28" t="str">
-        <v>1,520.8</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="str">
-        <v>0x77940861e000BfC8A8f67440ad21656B9e7dbA04</v>
-      </c>
-      <c r="B29">
-        <v>7826201</v>
-      </c>
-      <c r="C29" t="str">
-        <v>78,262.01</v>
-      </c>
-      <c r="D29">
-        <v>28484050</v>
-      </c>
-      <c r="E29" t="str">
-        <v>284,840.5</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="str">
-        <v>0x6BF81D0d4f4e606C3cB09C45f6FA29f8743c72DE</v>
-      </c>
-      <c r="B30">
-        <v>1000000</v>
-      </c>
-      <c r="C30" t="str">
-        <v>10,000</v>
-      </c>
-      <c r="D30">
-        <v>24257128</v>
-      </c>
-      <c r="E30" t="str">
-        <v>242,571.28</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="str">
-        <v>0x74c0d21e8ffC5b83dce1A0BB6abCD061D071E85a</v>
-      </c>
-      <c r="B31">
-        <v>26898709</v>
-      </c>
-      <c r="C31" t="str">
-        <v>268,987.09</v>
-      </c>
-      <c r="D31">
-        <v>26898709</v>
-      </c>
-      <c r="E31" t="str">
-        <v>268,987.09</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="str">
-        <v>0xD7Be7655070f986B3E311EE04cc9aa87Cd11ab5d</v>
-      </c>
-      <c r="B32">
-        <v>140273</v>
-      </c>
-      <c r="C32" t="str">
-        <v>1,402.73</v>
-      </c>
-      <c r="D32">
-        <v>140273</v>
-      </c>
-      <c r="E32" t="str">
-        <v>1,402.73</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="str">
-        <v>0xe5C5B9C648a3e66A2A7b8a3f2dA48e76e8309A2C</v>
-      </c>
-      <c r="B33">
-        <v>138254</v>
-      </c>
-      <c r="C33" t="str">
-        <v>1,382.54</v>
-      </c>
-      <c r="D33">
-        <v>138254</v>
-      </c>
-      <c r="E33" t="str">
-        <v>1,382.54</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="str">
-        <v>0x262ba7354bA2946de8f90dCe06883FaFebB6f043</v>
-      </c>
-      <c r="B34">
-        <v>60845986</v>
-      </c>
-      <c r="C34" t="str">
-        <v>608,459.86</v>
-      </c>
-      <c r="D34">
-        <v>60845986</v>
-      </c>
-      <c r="E34" t="str">
-        <v>608,459.86</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="str">
-        <v>0x4DF1C6c7973f4E6e3B22149f7b8eFc4389f97C56</v>
-      </c>
-      <c r="B35">
-        <v>41490298</v>
-      </c>
-      <c r="C35" t="str">
-        <v>414,902.98</v>
-      </c>
-      <c r="D35">
-        <v>41490298</v>
-      </c>
-      <c r="E35" t="str">
-        <v>414,902.98</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="str">
-        <v>0x3d1F678EBd71CA033f21D6B1B5B0781a66537447</v>
-      </c>
-      <c r="B36">
-        <v>1479327</v>
-      </c>
-      <c r="C36" t="str">
-        <v>14,793.27</v>
-      </c>
-      <c r="D36">
-        <v>1479327</v>
-      </c>
-      <c r="E36" t="str">
-        <v>14,793.27</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="str">
-        <v>0xB6e85e12331BdEA6fF03b25d3dE68a892C99C5D4</v>
-      </c>
-      <c r="B37">
-        <v>345637</v>
-      </c>
-      <c r="C37" t="str">
-        <v>3,456.37</v>
-      </c>
-      <c r="D37">
-        <v>345637</v>
-      </c>
-      <c r="E37" t="str">
-        <v>3,456.37</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="str">
-        <v>0xE2D8A9f98072298241651a1c899907892860A1f5</v>
-      </c>
-      <c r="B38">
-        <v>100000</v>
-      </c>
-      <c r="C38" t="str">
-        <v>1,000</v>
-      </c>
-      <c r="D38">
-        <v>138254</v>
-      </c>
-      <c r="E38" t="str">
-        <v>1,382.54</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="str">
-        <v>0xb91406Ea49418Ff04F73231BA48930278bCef631</v>
-      </c>
-      <c r="B39">
-        <v>276509</v>
-      </c>
-      <c r="C39" t="str">
-        <v>2,765.09</v>
-      </c>
-      <c r="D39">
-        <v>276509</v>
-      </c>
-      <c r="E39" t="str">
-        <v>2,765.09</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="str">
-        <v>0x040f62A18EB5D5ca87A08E41A22D004ee7A26380</v>
-      </c>
-      <c r="B40">
-        <v>345637</v>
-      </c>
-      <c r="C40" t="str">
-        <v>3,456.37</v>
-      </c>
-      <c r="D40">
-        <v>345637</v>
-      </c>
-      <c r="E40" t="str">
-        <v>3,456.37</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="str">
-        <v>0x18fc6c299B7aA35C8f59537b4b67c23D93E782ea</v>
-      </c>
-      <c r="B41">
-        <v>7000094</v>
-      </c>
-      <c r="C41" t="str">
-        <v>70,000.94</v>
-      </c>
-      <c r="D41">
-        <v>7000094</v>
-      </c>
-      <c r="E41" t="str">
-        <v>70,000.94</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="str">
-        <v>0x5C9A07e59Bdc264d0579530b4e08338122833942</v>
-      </c>
-      <c r="B42">
-        <v>1451676</v>
-      </c>
-      <c r="C42" t="str">
-        <v>14,516.76</v>
-      </c>
-      <c r="D42">
-        <v>1451676</v>
-      </c>
-      <c r="E42" t="str">
-        <v>14,516.76</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="str">
-        <v>0x4994A7059A2921398780818c203F83613A9Bf743</v>
-      </c>
-      <c r="B43">
-        <v>13825491</v>
-      </c>
-      <c r="C43" t="str">
-        <v>138,254.91</v>
-      </c>
-      <c r="D43">
-        <v>13825491</v>
-      </c>
-      <c r="E43" t="str">
-        <v>138,254.91</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="str">
-        <v>0xe9052daAC8667a27B38369aD37BEE63A8CD80Fc7</v>
-      </c>
-      <c r="B44">
-        <v>20895100</v>
-      </c>
-      <c r="C44" t="str">
-        <v>208,951</v>
-      </c>
-      <c r="D44">
-        <v>20895100</v>
-      </c>
-      <c r="E44" t="str">
-        <v>208,951</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="str">
-        <v>0x8f437d47c7723C7AB5ab896D59549D547181BecB</v>
-      </c>
-      <c r="B45">
-        <v>6736194</v>
-      </c>
-      <c r="C45" t="str">
-        <v>67,361.94</v>
-      </c>
-      <c r="D45">
-        <v>6736194</v>
-      </c>
-      <c r="E45" t="str">
-        <v>67,361.94</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="str">
-        <v>0xA742150Bb2b4e5DfCC4E6df0E577237Fceb797b2</v>
-      </c>
-      <c r="B46">
-        <v>500000</v>
-      </c>
-      <c r="C46" t="str">
-        <v>5,000</v>
-      </c>
-      <c r="D46">
-        <v>6736194</v>
-      </c>
-      <c r="E46" t="str">
-        <v>67,361.94</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="str">
-        <v>0x9D89f9451C4B7e04bd58616dbC72e924088AFF21</v>
-      </c>
-      <c r="B47">
-        <v>13542151</v>
-      </c>
-      <c r="C47" t="str">
-        <v>135,421.51</v>
-      </c>
-      <c r="D47">
-        <v>13542151</v>
-      </c>
-      <c r="E47" t="str">
-        <v>135,421.51</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="str">
-        <v>0x94B72396b6B40e19C2a04c28c8aE93dE08b12733</v>
-      </c>
-      <c r="B48">
-        <v>7697535</v>
-      </c>
-      <c r="C48" t="str">
-        <v>76,975.35</v>
-      </c>
-      <c r="D48">
-        <v>7697535</v>
-      </c>
-      <c r="E48" t="str">
-        <v>76,975.35</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="str">
-        <v>0x4CaFc8E23616346de04DE62174B1e615D8E80c70</v>
-      </c>
-      <c r="B49">
-        <v>7364037</v>
-      </c>
-      <c r="C49" t="str">
-        <v>73,640.37</v>
-      </c>
-      <c r="D49">
-        <v>7364037</v>
-      </c>
-      <c r="E49" t="str">
-        <v>73,640.37</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="str">
-        <v>0x6f9A5457e35FF98FCcA68b71c2D1bf7aAAeB714E</v>
-      </c>
-      <c r="B50">
-        <v>46</v>
-      </c>
-      <c r="C50" t="str">
-        <v>0.46</v>
-      </c>
-      <c r="D50">
-        <v>189077</v>
-      </c>
-      <c r="E50" t="str">
-        <v>1,890.77</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="str">
-        <v>0x0b3d82e9b1D9163a1fe71DC2bc60C6Fb7fb13863</v>
-      </c>
-      <c r="B51">
-        <v>189077</v>
-      </c>
-      <c r="C51" t="str">
-        <v>1,890.77</v>
-      </c>
-      <c r="D51">
-        <v>189077</v>
-      </c>
-      <c r="E51" t="str">
-        <v>1,890.77</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="str">
-        <v>0xb12042f547d28da37E88d7Db7A2CBAaf8CD88F68</v>
-      </c>
-      <c r="B52">
-        <v>691274</v>
-      </c>
-      <c r="C52" t="str">
-        <v>6,912.74</v>
-      </c>
-      <c r="D52">
-        <v>691274</v>
-      </c>
-      <c r="E52" t="str">
-        <v>6,912.74</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="str">
-        <v>0xDF6F220E72A6320E87576c5075899Be34212f97D</v>
-      </c>
-      <c r="B53">
-        <v>56242</v>
-      </c>
-      <c r="C53" t="str">
-        <v>562.42</v>
-      </c>
-      <c r="D53">
-        <v>56242</v>
-      </c>
-      <c r="E53" t="str">
-        <v>562.42</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="str">
-        <v>0x3E3309ab5312f6875b6e9bE672b9A43EFb70D760</v>
-      </c>
-      <c r="B54">
-        <v>6221470</v>
-      </c>
-      <c r="C54" t="str">
-        <v>62,214.7</v>
-      </c>
-      <c r="D54">
-        <v>6221470</v>
-      </c>
-      <c r="E54" t="str">
-        <v>62,214.7</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="str">
-        <v>0x47502539673c93B2ACDC9059B36360f76D3548BB</v>
-      </c>
-      <c r="B55">
-        <v>1022560</v>
-      </c>
-      <c r="C55" t="str">
-        <v>10,225.6</v>
-      </c>
-      <c r="D55">
-        <v>1022560</v>
-      </c>
-      <c r="E55" t="str">
-        <v>10,225.6</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="str">
-        <v>0x0254704C23C4765496894a632ef28d6be4DCB259</v>
-      </c>
-      <c r="B56">
-        <v>9332206</v>
-      </c>
-      <c r="C56" t="str">
-        <v>93,322.06</v>
-      </c>
-      <c r="D56">
-        <v>9332206</v>
-      </c>
-      <c r="E56" t="str">
-        <v>93,322.06</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="str">
-        <v>0x2EeCd56c9A00E81a393Fd24F22a07C9D80336E20</v>
-      </c>
-      <c r="B57">
-        <v>1861989</v>
-      </c>
-      <c r="C57" t="str">
-        <v>18,619.89</v>
-      </c>
-      <c r="D57">
-        <v>1861989</v>
-      </c>
-      <c r="E57" t="str">
-        <v>18,619.89</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="str">
-        <v>0x2abf42F330c60491E8A36B73c9F3F9Ed40CDa546</v>
-      </c>
-      <c r="B58">
-        <v>10106433</v>
-      </c>
-      <c r="C58" t="str">
-        <v>101,064.33</v>
-      </c>
-      <c r="D58">
-        <v>10106433</v>
-      </c>
-      <c r="E58" t="str">
-        <v>101,064.33</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="str">
-        <v>0x66B6221845b9bd7A029BCCb5523168a5AcE1e013</v>
-      </c>
-      <c r="B59">
-        <v>28660242</v>
-      </c>
-      <c r="C59" t="str">
-        <v>286,602.42</v>
-      </c>
-      <c r="D59">
-        <v>28660242</v>
-      </c>
-      <c r="E59" t="str">
-        <v>286,602.42</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="str">
-        <v>0x331B6287b04a4Bb359C75D102a2104561BB84fe3</v>
-      </c>
-      <c r="B60">
-        <v>41476</v>
-      </c>
-      <c r="C60" t="str">
-        <v>414.76</v>
-      </c>
-      <c r="D60">
-        <v>41476</v>
-      </c>
-      <c r="E60" t="str">
-        <v>414.76</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="str">
-        <v>0x2A1Cc6c77782EA6BE6C08d61430A79E31Ea4efDf</v>
-      </c>
-      <c r="B61">
-        <v>670536</v>
-      </c>
-      <c r="C61" t="str">
-        <v>6,705.36</v>
-      </c>
-      <c r="D61">
-        <v>670536</v>
-      </c>
-      <c r="E61" t="str">
-        <v>6,705.36</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="str">
-        <v>0x417eD74e3904f2C2d2eBb4e8050bD772374bd82a</v>
-      </c>
-      <c r="B62">
-        <v>89865</v>
-      </c>
-      <c r="C62" t="str">
-        <v>898.65</v>
-      </c>
-      <c r="D62">
-        <v>89865</v>
-      </c>
-      <c r="E62" t="str">
-        <v>898.65</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="str">
-        <v>0x746F83FF7eAdA9d0fB03DbAbcAF2600ee513DCDB</v>
-      </c>
-      <c r="B63">
-        <v>6223130</v>
-      </c>
-      <c r="C63" t="str">
-        <v>62,231.3</v>
-      </c>
-      <c r="D63">
-        <v>6223130</v>
-      </c>
-      <c r="E63" t="str">
-        <v>62,231.3</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="str">
-        <v>0x733e103A702EACEa3189361a3b79902491FBACd1</v>
-      </c>
-      <c r="B64">
-        <v>138254</v>
-      </c>
-      <c r="C64" t="str">
-        <v>1,382.54</v>
-      </c>
-      <c r="D64">
-        <v>138254</v>
-      </c>
-      <c r="E64" t="str">
-        <v>1,382.54</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="str">
-        <v>0xE17Aa7A67B0834823F56f01260b1E0965f14Eb4c</v>
-      </c>
-      <c r="B65">
-        <v>6912745</v>
-      </c>
-      <c r="C65" t="str">
-        <v>69,127.45</v>
-      </c>
-      <c r="D65">
-        <v>6912745</v>
-      </c>
-      <c r="E65" t="str">
-        <v>69,127.45</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="str">
-        <v>0x7011467e458B4cEEED928bac3E178Ce7EB892F2d</v>
-      </c>
-      <c r="B66">
-        <v>2765098</v>
-      </c>
-      <c r="C66" t="str">
-        <v>27,650.98</v>
-      </c>
-      <c r="D66">
-        <v>2765098</v>
-      </c>
-      <c r="E66" t="str">
-        <v>27,650.98</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="str">
-        <v>0x469E40f0854EC0E8FaC1Afd4Af2DFfD5aE5569B0</v>
-      </c>
-      <c r="B67">
-        <v>110603</v>
-      </c>
-      <c r="C67" t="str">
-        <v>1,106.03</v>
-      </c>
-      <c r="D67">
-        <v>110603</v>
-      </c>
-      <c r="E67" t="str">
-        <v>1,106.03</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="str">
-        <v>0x21a18db5749f090BB96DE151de4136866cdAC8DF</v>
-      </c>
-      <c r="B68">
-        <v>81515</v>
-      </c>
-      <c r="C68" t="str">
-        <v>815.15</v>
-      </c>
-      <c r="D68">
-        <v>81515</v>
-      </c>
-      <c r="E68" t="str">
-        <v>815.15</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="str">
-        <v>0xe6eaa2b28ce4b4064E37eF290E82de53Fd81C211</v>
-      </c>
-      <c r="B69">
-        <v>1036911</v>
-      </c>
-      <c r="C69" t="str">
-        <v>10,369.11</v>
-      </c>
-      <c r="D69">
-        <v>1036911</v>
-      </c>
-      <c r="E69" t="str">
-        <v>10,369.11</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="str">
-        <v>0x3010A4E7ce5c99208900c218d0375bfEfE7De269</v>
-      </c>
-      <c r="B70">
-        <v>20738236</v>
-      </c>
-      <c r="C70" t="str">
-        <v>207,382.36</v>
-      </c>
-      <c r="D70">
-        <v>20738236</v>
-      </c>
-      <c r="E70" t="str">
-        <v>207,382.36</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="str">
-        <v>0x430cB4360cE341a6Ad0Dfa18b9aD1Ae2cFa9AD18</v>
-      </c>
-      <c r="B71">
-        <v>2765098</v>
-      </c>
-      <c r="C71" t="str">
-        <v>27,650.98</v>
-      </c>
-      <c r="D71">
-        <v>2765098</v>
-      </c>
-      <c r="E71" t="str">
-        <v>27,650.98</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="str">
-        <v>0x8fa6e6dB6B86d0Cad2fa8DeEb737BC1cB97a2bE1</v>
-      </c>
-      <c r="B72">
-        <v>691274</v>
-      </c>
-      <c r="C72" t="str">
-        <v>6,912.74</v>
-      </c>
-      <c r="D72">
-        <v>691274</v>
-      </c>
-      <c r="E72" t="str">
-        <v>6,912.74</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="str">
-        <v>0x8364044ee8062F0F6C9835f7dfC26da4CE433BB8</v>
-      </c>
-      <c r="B73">
-        <v>691274</v>
-      </c>
-      <c r="C73" t="str">
-        <v>6,912.74</v>
-      </c>
-      <c r="D73">
-        <v>691274</v>
-      </c>
-      <c r="E73" t="str">
-        <v>6,912.74</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="str">
-        <v>0x9fF7d51Cf6a3A12F2Cdd36035827037a35A4B139</v>
-      </c>
-      <c r="B74">
-        <v>23613</v>
-      </c>
-      <c r="C74" t="str">
-        <v>236.13</v>
-      </c>
-      <c r="D74">
-        <v>23613</v>
-      </c>
-      <c r="E74" t="str">
-        <v>236.13</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="str">
-        <v>0x8B66c0aEEc3a231F6e3302dBb7d351B5c7B094B0</v>
-      </c>
-      <c r="B75">
-        <v>276509</v>
-      </c>
-      <c r="C75" t="str">
-        <v>2,765.09</v>
-      </c>
-      <c r="D75">
-        <v>276509</v>
-      </c>
-      <c r="E75" t="str">
-        <v>2,765.09</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="str">
-        <v>0xD81F1cF201B68a9EA0E8f10b1864DFE925202643</v>
-      </c>
-      <c r="B76">
-        <v>317986</v>
-      </c>
-      <c r="C76" t="str">
-        <v>3,179.86</v>
-      </c>
-      <c r="D76">
-        <v>317986</v>
-      </c>
-      <c r="E76" t="str">
-        <v>3,179.86</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="str">
-        <v>0x20944C8A17cfa6cb96556116037e3aEeB506a0b0</v>
-      </c>
-      <c r="B77">
-        <v>317986</v>
-      </c>
-      <c r="C77" t="str">
-        <v>3,179.86</v>
-      </c>
-      <c r="D77">
-        <v>317986</v>
-      </c>
-      <c r="E77" t="str">
-        <v>3,179.86</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="str">
-        <v>0x61cD23Cf91d9B6BBb4bFF28c6AD7B667C7EC6367</v>
-      </c>
-      <c r="B78">
-        <v>2500000</v>
-      </c>
-      <c r="C78" t="str">
-        <v>25,000</v>
-      </c>
-      <c r="D78">
-        <v>8986569</v>
-      </c>
-      <c r="E78" t="str">
-        <v>89,865.69</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="str">
-        <v>0xEA67438f0857e93968F50aE87db18720b9E457Ef</v>
-      </c>
-      <c r="B79">
-        <v>417391</v>
-      </c>
-      <c r="C79" t="str">
-        <v>4,173.91</v>
-      </c>
-      <c r="D79">
-        <v>417391</v>
-      </c>
-      <c r="E79" t="str">
-        <v>4,173.91</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="str">
-        <v>0x8f1928e8FEa7238b9B53A7E62AFd471b69732a66</v>
-      </c>
-      <c r="B80">
-        <v>4147647</v>
-      </c>
-      <c r="C80" t="str">
-        <v>41,476.47</v>
-      </c>
-      <c r="D80">
-        <v>4147647</v>
-      </c>
-      <c r="E80" t="str">
-        <v>41,476.47</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="str">
-        <v>0x5390651dd0824159FE0e82554feC7b283bCa3745</v>
-      </c>
-      <c r="B81">
-        <v>4147647</v>
-      </c>
-      <c r="C81" t="str">
-        <v>41,476.47</v>
-      </c>
-      <c r="D81">
-        <v>4147647</v>
-      </c>
-      <c r="E81" t="str">
-        <v>41,476.47</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="str">
-        <v>0xf33639F5c9cDB8E242c3E20Fdaf98Ae389f0e399</v>
-      </c>
-      <c r="B82">
-        <v>414764</v>
-      </c>
-      <c r="C82" t="str">
-        <v>4,147.64</v>
-      </c>
-      <c r="D82">
-        <v>414764</v>
-      </c>
-      <c r="E82" t="str">
-        <v>4,147.64</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="str">
-        <v>0x0116c14c39b5a5ecD03193E56E975064b4a405D2</v>
-      </c>
-      <c r="B83">
-        <v>414764</v>
-      </c>
-      <c r="C83" t="str">
-        <v>4,147.64</v>
-      </c>
-      <c r="D83">
-        <v>414764</v>
-      </c>
-      <c r="E83" t="str">
-        <v>4,147.64</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="str">
-        <v>0xbD73E24F927E9f1D9ce45B7e47f36711Dca35A88</v>
-      </c>
-      <c r="B84">
-        <v>5530196</v>
-      </c>
-      <c r="C84" t="str">
-        <v>55,301.96</v>
-      </c>
-      <c r="D84">
-        <v>5530196</v>
-      </c>
-      <c r="E84" t="str">
-        <v>55,301.96</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="str">
-        <v>0xb05822516a701573678447E6966F7eD3bdDf78C5</v>
-      </c>
-      <c r="B85">
-        <v>2653885</v>
-      </c>
-      <c r="C85" t="str">
-        <v>26,538.85</v>
-      </c>
-      <c r="D85">
-        <v>2653885</v>
-      </c>
-      <c r="E85" t="str">
-        <v>26,538.85</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="str">
-        <v>0xBBBA5cae882A16fEdAD9a92220C7dBF2d9Eb2313</v>
-      </c>
-      <c r="B86">
-        <v>2765098</v>
-      </c>
-      <c r="C86" t="str">
-        <v>27,650.98</v>
-      </c>
-      <c r="D86">
-        <v>2765098</v>
-      </c>
-      <c r="E86" t="str">
-        <v>27,650.98</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="str">
-        <v>Total</v>
-      </c>
-      <c r="B87">
-        <v>480378344</v>
-      </c>
-      <c r="C87" t="str">
-        <v>4,803,783.44</v>
-      </c>
-      <c r="D87">
-        <v>641025598</v>
-      </c>
-      <c r="E87" t="str">
-        <v>6,410,255.98</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E87"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
@@ -2873,7 +1379,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E58"/>
   <sheetViews>

</xml_diff>

<commit_message>
Publish TANIP-1 Period 9 rewards
</commit_message>
<xml_diff>
--- a/staker_incentives.xlsx
+++ b/staker_incentives.xlsx
@@ -12,6 +12,7 @@
     <sheet name="Blocks 69783960 - 70067138" sheetId="7" r:id="rId7"/>
     <sheet name="Blocks 70067139 - 70350763" sheetId="8" r:id="rId8"/>
     <sheet name="Blocks 70350764 - 70634063" sheetId="9" r:id="rId9"/>
+    <sheet name="Blocks 70634064 - 70917849" sheetId="10" r:id="rId10"/>
   </sheets>
 </workbook>
 </file>
@@ -7064,6 +7065,3886 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E227"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" width="20.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Staker Address</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Reward (ERC20 TEL)</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Uncapped Reward (ERC20 TEL)</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Staker Fees</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Referee Fees</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>0xA0De99feED77A3f228F9e6Bfe3B8333c2fc1D0f9</v>
+      </c>
+      <c r="B2" t="str">
+        <v>1,997.25</v>
+      </c>
+      <c r="C2" t="str">
+        <v>1,997.25</v>
+      </c>
+      <c r="D2" t="str">
+        <v>309.92</v>
+      </c>
+      <c r="E2" t="str">
+        <v>1,410.09</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>0xDdF9E0547714839685900403611875EbB18C6236</v>
+      </c>
+      <c r="B3" t="str">
+        <v>2,202.23</v>
+      </c>
+      <c r="C3" t="str">
+        <v>2,202.23</v>
+      </c>
+      <c r="D3" t="str">
+        <v>831.4</v>
+      </c>
+      <c r="E3" t="str">
+        <v>1,065.14</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>0x76cf73e99947E31e951416E3859F3cFB07f9Fd3B</v>
+      </c>
+      <c r="B4" t="str">
+        <v>2,202.23</v>
+      </c>
+      <c r="C4" t="str">
+        <v>2,202.23</v>
+      </c>
+      <c r="D4" t="str">
+        <v>1,065.14</v>
+      </c>
+      <c r="E4" t="str">
+        <v>831.4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>0x1f21AdB9fe6A088B4F5411eEd543BEA954A15F56</v>
+      </c>
+      <c r="B5" t="str">
+        <v>79,719.08</v>
+      </c>
+      <c r="C5" t="str">
+        <v>79,719.08</v>
+      </c>
+      <c r="D5" t="str">
+        <v>3,582.7</v>
+      </c>
+      <c r="E5" t="str">
+        <v>65,070.4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>0x77Fb1AeEEC6e3F3Cfe3a1f3aB87E7cB74872Db5D</v>
+      </c>
+      <c r="B6" t="str">
+        <v>1,926.5</v>
+      </c>
+      <c r="C6" t="str">
+        <v>1,926.5</v>
+      </c>
+      <c r="D6" t="str">
+        <v>1.06</v>
+      </c>
+      <c r="E6" t="str">
+        <v>1,658.02</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>0xF68784ce085df3b5d3493A29F3Be8Bc971c3C87A</v>
+      </c>
+      <c r="B7" t="str">
+        <v>11,951.61</v>
+      </c>
+      <c r="C7" t="str">
+        <v>11,951.61</v>
+      </c>
+      <c r="D7" t="str">
+        <v>10,292.58</v>
+      </c>
+      <c r="E7" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>0x4B3D17974c2F79fEf5D495F082e9eC7d1FD95a06</v>
+      </c>
+      <c r="B8" t="str">
+        <v>947.01</v>
+      </c>
+      <c r="C8" t="str">
+        <v>947.01</v>
+      </c>
+      <c r="D8" t="str">
+        <v>815.56</v>
+      </c>
+      <c r="E8" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>0x096454fa85d4bD21CBB9134966c417f2e40C288C</v>
+      </c>
+      <c r="B9" t="str">
+        <v>947.01</v>
+      </c>
+      <c r="C9" t="str">
+        <v>947.01</v>
+      </c>
+      <c r="D9" t="str">
+        <v>0</v>
+      </c>
+      <c r="E9" t="str">
+        <v>815.56</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>0x9195C770DCe41eC211353afD92c8a0f0b28fB011</v>
+      </c>
+      <c r="B10" t="str">
+        <v>5,465.27</v>
+      </c>
+      <c r="C10" t="str">
+        <v>5,465.27</v>
+      </c>
+      <c r="D10" t="str">
+        <v>1,164.33</v>
+      </c>
+      <c r="E10" t="str">
+        <v>3,542.3</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>0xf78D0cdFB459eD9CC19eEb7c22B5F193d7662fcC</v>
+      </c>
+      <c r="B11" t="str">
+        <v>906.01</v>
+      </c>
+      <c r="C11" t="str">
+        <v>906.01</v>
+      </c>
+      <c r="D11" t="str">
+        <v>780.25</v>
+      </c>
+      <c r="E11" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>0xAD5c21611Ea4790991c40BFD8e0888e012D7162E</v>
+      </c>
+      <c r="B12" t="str">
+        <v>1,138</v>
+      </c>
+      <c r="C12" t="str">
+        <v>1,138</v>
+      </c>
+      <c r="D12" t="str">
+        <v>980.04</v>
+      </c>
+      <c r="E12" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>0x3F3Cb523ce45c048c07081925CBd588a6C601b72</v>
+      </c>
+      <c r="B13" t="str">
+        <v>90.2</v>
+      </c>
+      <c r="C13" t="str">
+        <v>90.2</v>
+      </c>
+      <c r="D13" t="str">
+        <v>0</v>
+      </c>
+      <c r="E13" t="str">
+        <v>77.68</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>0x143A47CAF24904a750242e138F31ADd7F6999Cb5</v>
+      </c>
+      <c r="B14" t="str">
+        <v>8.99</v>
+      </c>
+      <c r="C14" t="str">
+        <v>8.99</v>
+      </c>
+      <c r="D14" t="str">
+        <v>7.75</v>
+      </c>
+      <c r="E14" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>0xE233390f362B1dC22F621feead135D828a39781A</v>
+      </c>
+      <c r="B15" t="str">
+        <v>17.73</v>
+      </c>
+      <c r="C15" t="str">
+        <v>17.73</v>
+      </c>
+      <c r="D15" t="str">
+        <v>15.27</v>
+      </c>
+      <c r="E15" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>0x25E9eA1a93D9e505cd7d056C1e1bA16789537EAb</v>
+      </c>
+      <c r="B16" t="str">
+        <v>9,195.33</v>
+      </c>
+      <c r="C16" t="str">
+        <v>9,195.33</v>
+      </c>
+      <c r="D16" t="str">
+        <v>0</v>
+      </c>
+      <c r="E16" t="str">
+        <v>7,918.91</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>0xBBF6951084154eB73b77f9A9BA943e478bFa06c4</v>
+      </c>
+      <c r="B17" t="str">
+        <v>1,707.65</v>
+      </c>
+      <c r="C17" t="str">
+        <v>1,707.65</v>
+      </c>
+      <c r="D17" t="str">
+        <v>1,470.61</v>
+      </c>
+      <c r="E17" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>0x5Fc4faF3934548c57d66f1179C2991cEd028E61F</v>
+      </c>
+      <c r="B18" t="str">
+        <v>290.29</v>
+      </c>
+      <c r="C18" t="str">
+        <v>290.29</v>
+      </c>
+      <c r="D18" t="str">
+        <v>0</v>
+      </c>
+      <c r="E18" t="str">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>0x9D89f9451C4B7e04bd58616dbC72e924088AFF21</v>
+      </c>
+      <c r="B19" t="str">
+        <v>108,672.83</v>
+      </c>
+      <c r="C19" t="str">
+        <v>108,672.83</v>
+      </c>
+      <c r="D19" t="str">
+        <v>18,501.95</v>
+      </c>
+      <c r="E19" t="str">
+        <v>75,085.76</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>0x426d787930A93314048488c4D10946FCeD265Cc7</v>
+      </c>
+      <c r="B20" t="str">
+        <v>12,278.97</v>
+      </c>
+      <c r="C20" t="str">
+        <v>12,278.97</v>
+      </c>
+      <c r="D20" t="str">
+        <v>4,092.1</v>
+      </c>
+      <c r="E20" t="str">
+        <v>6,482.4</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>0xc1c106e16cF229be127C30406c598b07986c06BA</v>
+      </c>
+      <c r="B21" t="str">
+        <v>72,480.52</v>
+      </c>
+      <c r="C21" t="str">
+        <v>72,480.52</v>
+      </c>
+      <c r="D21" t="str">
+        <v>4,601.73</v>
+      </c>
+      <c r="E21" t="str">
+        <v>57,817.61</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>0x16eE201E4fD4418f47A6c7f45fB0Aaf8a61011Df</v>
+      </c>
+      <c r="B22" t="str">
+        <v>2,858.79</v>
+      </c>
+      <c r="C22" t="str">
+        <v>2,858.79</v>
+      </c>
+      <c r="D22" t="str">
+        <v>2,461.96</v>
+      </c>
+      <c r="E22" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>0xB34C5F08ff67cF102D31055ba5Fc517eDeD517BC</v>
+      </c>
+      <c r="B23" t="str">
+        <v>9,775.49</v>
+      </c>
+      <c r="C23" t="str">
+        <v>9,775.49</v>
+      </c>
+      <c r="D23" t="str">
+        <v>8,111.53</v>
+      </c>
+      <c r="E23" t="str">
+        <v>307.01</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>0xd2938A7fCa560A5b6630aaf12d817E5f146cddA4</v>
+      </c>
+      <c r="B24" t="str">
+        <v>310.87</v>
+      </c>
+      <c r="C24" t="str">
+        <v>310.87</v>
+      </c>
+      <c r="D24" t="str">
+        <v>267.72</v>
+      </c>
+      <c r="E24" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>0x721D683cBd00c78Eb2676fBA03e8c03FDF07f5dC</v>
+      </c>
+      <c r="B25" t="str">
+        <v>3,753.37</v>
+      </c>
+      <c r="C25" t="str">
+        <v>3,753.37</v>
+      </c>
+      <c r="D25" t="str">
+        <v>2,922.44</v>
+      </c>
+      <c r="E25" t="str">
+        <v>309.92</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>0xDe113Cfea35386619bB00AD4B84130b22222c742</v>
+      </c>
+      <c r="B26" t="str">
+        <v>788.88</v>
+      </c>
+      <c r="C26" t="str">
+        <v>788.88</v>
+      </c>
+      <c r="D26" t="str">
+        <v>679.38</v>
+      </c>
+      <c r="E26" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>0xCdDca3b68166cB76442B5D69cB6B800fD7fc67c0</v>
+      </c>
+      <c r="B27" t="str">
+        <v>1,275.99</v>
+      </c>
+      <c r="C27" t="str">
+        <v>1,275.99</v>
+      </c>
+      <c r="D27" t="str">
+        <v>0</v>
+      </c>
+      <c r="E27" t="str">
+        <v>1,098.87</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>0x72d20dcB42DC91D2Dc1DB60375e1945e23708130</v>
+      </c>
+      <c r="B28" t="str">
+        <v>480.71</v>
+      </c>
+      <c r="C28" t="str">
+        <v>480.71</v>
+      </c>
+      <c r="D28" t="str">
+        <v>413.99</v>
+      </c>
+      <c r="E28" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>0xaB851DBd7b470252D76C725411143d12aCd2adCB</v>
+      </c>
+      <c r="B29" t="str">
+        <v>480.71</v>
+      </c>
+      <c r="C29" t="str">
+        <v>480.71</v>
+      </c>
+      <c r="D29" t="str">
+        <v>0</v>
+      </c>
+      <c r="E29" t="str">
+        <v>413.99</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>0x893b99952A101ea504E2DA3d44164858b11a58a1</v>
+      </c>
+      <c r="B30" t="str">
+        <v>118.8</v>
+      </c>
+      <c r="C30" t="str">
+        <v>118.8</v>
+      </c>
+      <c r="D30" t="str">
+        <v>102.31</v>
+      </c>
+      <c r="E30" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>0xc790596C713f906Bc24beEC6da941AC5DDD92800</v>
+      </c>
+      <c r="B31" t="str">
+        <v>0</v>
+      </c>
+      <c r="C31" t="str">
+        <v>21,514.21</v>
+      </c>
+      <c r="D31" t="str">
+        <v>17.99</v>
+      </c>
+      <c r="E31" t="str">
+        <v>18,509.79</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>0x964087989Df5D5e89cF7527b72A3949367a337bA</v>
+      </c>
+      <c r="B32" t="str">
+        <v>9,669.08</v>
+      </c>
+      <c r="C32" t="str">
+        <v>9,669.08</v>
+      </c>
+      <c r="D32" t="str">
+        <v>8,326.9</v>
+      </c>
+      <c r="E32" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>0x65ED1e1351640D112aeAc04d4988B6916a5f62dc</v>
+      </c>
+      <c r="B33" t="str">
+        <v>249.73</v>
+      </c>
+      <c r="C33" t="str">
+        <v>249.73</v>
+      </c>
+      <c r="D33" t="str">
+        <v>215.07</v>
+      </c>
+      <c r="E33" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>0x883c4BF5F45e8E75C59DdeA8B2ba3Cd40e81047D</v>
+      </c>
+      <c r="B34" t="str">
+        <v>249.73</v>
+      </c>
+      <c r="C34" t="str">
+        <v>249.73</v>
+      </c>
+      <c r="D34" t="str">
+        <v>0</v>
+      </c>
+      <c r="E34" t="str">
+        <v>215.07</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>0x8218E1a9D02E26E2aF124EA28b121031Cf25AaC8</v>
+      </c>
+      <c r="B35" t="str">
+        <v>3,442.5</v>
+      </c>
+      <c r="C35" t="str">
+        <v>3,442.5</v>
+      </c>
+      <c r="D35" t="str">
+        <v>2,964.64</v>
+      </c>
+      <c r="E35" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>0x64d564A6A6003a9fcb44f8F50b9A3C7bBea2a7E7</v>
+      </c>
+      <c r="B36" t="str">
+        <v>119.46</v>
+      </c>
+      <c r="C36" t="str">
+        <v>119.46</v>
+      </c>
+      <c r="D36" t="str">
+        <v>102.88</v>
+      </c>
+      <c r="E36" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>0xf0a8596541F839EBcC9f0A9d1442c15f43A2836E</v>
+      </c>
+      <c r="B37" t="str">
+        <v>119.46</v>
+      </c>
+      <c r="C37" t="str">
+        <v>119.46</v>
+      </c>
+      <c r="D37" t="str">
+        <v>0</v>
+      </c>
+      <c r="E37" t="str">
+        <v>102.88</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>0x20944C8A17cfa6cb96556116037e3aEeB506a0b0</v>
+      </c>
+      <c r="B38" t="str">
+        <v>1,888.71</v>
+      </c>
+      <c r="C38" t="str">
+        <v>1,888.71</v>
+      </c>
+      <c r="D38" t="str">
+        <v>1,626.54</v>
+      </c>
+      <c r="E38" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>0x5099ccbB5FC14BF6ea516EE6CC3e6B209a7aA8C6</v>
+      </c>
+      <c r="B39" t="str">
+        <v>603.43</v>
+      </c>
+      <c r="C39" t="str">
+        <v>603.43</v>
+      </c>
+      <c r="D39" t="str">
+        <v>519.67</v>
+      </c>
+      <c r="E39" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>0x033047D46C9dD342b21274a0f328DD04c3ABa9b7</v>
+      </c>
+      <c r="B40" t="str">
+        <v>15,946.55</v>
+      </c>
+      <c r="C40" t="str">
+        <v>15,946.55</v>
+      </c>
+      <c r="D40" t="str">
+        <v>590.78</v>
+      </c>
+      <c r="E40" t="str">
+        <v>13,142.2</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>0xfC433E52b109b00c9e9f9532Da4a1B94a873A3a8</v>
+      </c>
+      <c r="B41" t="str">
+        <v>686</v>
+      </c>
+      <c r="C41" t="str">
+        <v>686</v>
+      </c>
+      <c r="D41" t="str">
+        <v>0</v>
+      </c>
+      <c r="E41" t="str">
+        <v>590.78</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>0xdd61cabccEa7933D2372606963D66F0924831D29</v>
+      </c>
+      <c r="B42" t="str">
+        <v>20.4</v>
+      </c>
+      <c r="C42" t="str">
+        <v>20.4</v>
+      </c>
+      <c r="D42" t="str">
+        <v>17.57</v>
+      </c>
+      <c r="E42" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>0x70a358970c122dE0ebb3f9c0b8704E71c2f69352</v>
+      </c>
+      <c r="B43" t="str">
+        <v>20.4</v>
+      </c>
+      <c r="C43" t="str">
+        <v>20.4</v>
+      </c>
+      <c r="D43" t="str">
+        <v>0</v>
+      </c>
+      <c r="E43" t="str">
+        <v>17.57</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>0xb51D1dC8c04786ec6B47570619bBa8f6D0B7bcbc</v>
+      </c>
+      <c r="B44" t="str">
+        <v>1,436.73</v>
+      </c>
+      <c r="C44" t="str">
+        <v>1,436.73</v>
+      </c>
+      <c r="D44" t="str">
+        <v>1,237.3</v>
+      </c>
+      <c r="E44" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>0x8f26838FF9A288727088F10968Ea663A424509F4</v>
+      </c>
+      <c r="B45" t="str">
+        <v>44,560.21</v>
+      </c>
+      <c r="C45" t="str">
+        <v>44,560.21</v>
+      </c>
+      <c r="D45" t="str">
+        <v>0</v>
+      </c>
+      <c r="E45" t="str">
+        <v>38,374.71</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>0xF336C5e15E672F6606CA8CDe3D4FaF95fE1C63Bb</v>
+      </c>
+      <c r="B46" t="str">
+        <v>275.77</v>
+      </c>
+      <c r="C46" t="str">
+        <v>275.77</v>
+      </c>
+      <c r="D46" t="str">
+        <v>237.49</v>
+      </c>
+      <c r="E46" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>0x04d9f35C7c292ca2c75C498563b48123C0662e19</v>
+      </c>
+      <c r="B47" t="str">
+        <v>2,909.13</v>
+      </c>
+      <c r="C47" t="str">
+        <v>2,909.13</v>
+      </c>
+      <c r="D47" t="str">
+        <v>2,505.31</v>
+      </c>
+      <c r="E47" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>0x7B82007d91312Bb84E57A79c6df7Fa3928beD152</v>
+      </c>
+      <c r="B48" t="str">
+        <v>18.97</v>
+      </c>
+      <c r="C48" t="str">
+        <v>18.97</v>
+      </c>
+      <c r="D48" t="str">
+        <v>0</v>
+      </c>
+      <c r="E48" t="str">
+        <v>16.34</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>0xaE8f06402E8e67023b13f2F132Dc34422aFA6189</v>
+      </c>
+      <c r="B49" t="str">
+        <v>18.81</v>
+      </c>
+      <c r="C49" t="str">
+        <v>18.81</v>
+      </c>
+      <c r="D49" t="str">
+        <v>16.2</v>
+      </c>
+      <c r="E49" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>0xEbbabF54e68354253E41f2D0F1C543FEc5Bcfffa</v>
+      </c>
+      <c r="B50" t="str">
+        <v>577,271.42</v>
+      </c>
+      <c r="C50" t="str">
+        <v>577,271.42</v>
+      </c>
+      <c r="D50" t="str">
+        <v>248,690.08</v>
+      </c>
+      <c r="E50" t="str">
+        <v>248,448.98</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>0x3C7c8Ae12872dCbcF52B450FADB323810B9f5a94</v>
+      </c>
+      <c r="B51" t="str">
+        <v>284.49</v>
+      </c>
+      <c r="C51" t="str">
+        <v>284.49</v>
+      </c>
+      <c r="D51" t="str">
+        <v>245</v>
+      </c>
+      <c r="E51" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>0x413Af536E3D18D259A9b71B42AC66faC5aBa0Fbf</v>
+      </c>
+      <c r="B52" t="str">
+        <v>9.87</v>
+      </c>
+      <c r="C52" t="str">
+        <v>9.87</v>
+      </c>
+      <c r="D52" t="str">
+        <v>8.5</v>
+      </c>
+      <c r="E52" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>0x5a46E444528E8f72897FE6C08AB2bbCC11E69096</v>
+      </c>
+      <c r="B53" t="str">
+        <v>54.32</v>
+      </c>
+      <c r="C53" t="str">
+        <v>54.32</v>
+      </c>
+      <c r="D53" t="str">
+        <v>46.78</v>
+      </c>
+      <c r="E53" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>0x4e50BEF218F0Db065F4EE833D3679712A74F21F2</v>
+      </c>
+      <c r="B54" t="str">
+        <v>50.47</v>
+      </c>
+      <c r="C54" t="str">
+        <v>50.47</v>
+      </c>
+      <c r="D54" t="str">
+        <v>43.47</v>
+      </c>
+      <c r="E54" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>0xc3E8E2045564533F6a31ec05b3BD9BCFc5C9f76D</v>
+      </c>
+      <c r="B55" t="str">
+        <v>44.84</v>
+      </c>
+      <c r="C55" t="str">
+        <v>44.84</v>
+      </c>
+      <c r="D55" t="str">
+        <v>38.62</v>
+      </c>
+      <c r="E55" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>0x98Bf5dA74530B21130C029663a25A32066b9913b</v>
+      </c>
+      <c r="B56" t="str">
+        <v>32.72</v>
+      </c>
+      <c r="C56" t="str">
+        <v>32.72</v>
+      </c>
+      <c r="D56" t="str">
+        <v>28.18</v>
+      </c>
+      <c r="E56" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>0x4E2069d03340c94A9C79e31dd93D577d82C83b22</v>
+      </c>
+      <c r="B57" t="str">
+        <v>25.41</v>
+      </c>
+      <c r="C57" t="str">
+        <v>25.41</v>
+      </c>
+      <c r="D57" t="str">
+        <v>21.89</v>
+      </c>
+      <c r="E57" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>0xa755B0E03b0C0411c64749C64F063a6600a24D8c</v>
+      </c>
+      <c r="B58" t="str">
+        <v>721.32</v>
+      </c>
+      <c r="C58" t="str">
+        <v>721.32</v>
+      </c>
+      <c r="D58" t="str">
+        <v>621.2</v>
+      </c>
+      <c r="E58" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>0x357cDa2237d31e618ba3A39dD4691429E7cDD107</v>
+      </c>
+      <c r="B59" t="str">
+        <v>1,391.03</v>
+      </c>
+      <c r="C59" t="str">
+        <v>1,391.03</v>
+      </c>
+      <c r="D59" t="str">
+        <v>1,197.94</v>
+      </c>
+      <c r="E59" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>0x24EC4345706a30747bA16dCA3e9751B73b72C78a</v>
+      </c>
+      <c r="B60" t="str">
+        <v>466.69</v>
+      </c>
+      <c r="C60" t="str">
+        <v>466.69</v>
+      </c>
+      <c r="D60" t="str">
+        <v>401.91</v>
+      </c>
+      <c r="E60" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>0xE5d3b6737c87c922A0D6D4Abe4C76A8D6C70C628</v>
+      </c>
+      <c r="B61" t="str">
+        <v>472.33</v>
+      </c>
+      <c r="C61" t="str">
+        <v>472.33</v>
+      </c>
+      <c r="D61" t="str">
+        <v>406.77</v>
+      </c>
+      <c r="E61" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>0x2731b9BC4c6AC6287996741A5A87D6E51D18B2EB</v>
+      </c>
+      <c r="B62" t="str">
+        <v>368.39</v>
+      </c>
+      <c r="C62" t="str">
+        <v>368.39</v>
+      </c>
+      <c r="D62" t="str">
+        <v>317.26</v>
+      </c>
+      <c r="E62" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>0x942E746C384bec88Dfa6164e8d699858E9988FeB</v>
+      </c>
+      <c r="B63" t="str">
+        <v>270.81</v>
+      </c>
+      <c r="C63" t="str">
+        <v>270.81</v>
+      </c>
+      <c r="D63" t="str">
+        <v>233.22</v>
+      </c>
+      <c r="E63" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>0x8f956317B24CA7CB331BdfC3ECB21864f7dF731E</v>
+      </c>
+      <c r="B64" t="str">
+        <v>32.95</v>
+      </c>
+      <c r="C64" t="str">
+        <v>32.95</v>
+      </c>
+      <c r="D64" t="str">
+        <v>28.38</v>
+      </c>
+      <c r="E64" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>0xB51e05e0F9b9a22D714fC181aBA3a43d79d728bB</v>
+      </c>
+      <c r="B65" t="str">
+        <v>15,260.55</v>
+      </c>
+      <c r="C65" t="str">
+        <v>15,260.55</v>
+      </c>
+      <c r="D65" t="str">
+        <v>13,142.2</v>
+      </c>
+      <c r="E65" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v>0xcC333A0d55395f7cABD42793850D4ea5B32E1D78</v>
+      </c>
+      <c r="B66" t="str">
+        <v>6,070.82</v>
+      </c>
+      <c r="C66" t="str">
+        <v>6,070.82</v>
+      </c>
+      <c r="D66" t="str">
+        <v>0</v>
+      </c>
+      <c r="E66" t="str">
+        <v>5,228.12</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="str">
+        <v>0x7229aE5d9fa64DAe6C47d360023FfE683f0517F0</v>
+      </c>
+      <c r="B67" t="str">
+        <v>878.04</v>
+      </c>
+      <c r="C67" t="str">
+        <v>878.04</v>
+      </c>
+      <c r="D67" t="str">
+        <v>0</v>
+      </c>
+      <c r="E67" t="str">
+        <v>756.16</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="str">
+        <v>0xb4120A72ad3778E123da74F3C09c1272521C8b7e</v>
+      </c>
+      <c r="B68" t="str">
+        <v>74,795.79</v>
+      </c>
+      <c r="C68" t="str">
+        <v>74,795.79</v>
+      </c>
+      <c r="D68" t="str">
+        <v>64,413.22</v>
+      </c>
+      <c r="E68" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="str">
+        <v>0xa8f881849583f2dBC55f04433C62Edbc79f46286</v>
+      </c>
+      <c r="B69" t="str">
+        <v>23.35</v>
+      </c>
+      <c r="C69" t="str">
+        <v>23.35</v>
+      </c>
+      <c r="D69" t="str">
+        <v>20.11</v>
+      </c>
+      <c r="E69" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="str">
+        <v>0x3E19a28308585b842974317f2198A1f4f720EF85</v>
+      </c>
+      <c r="B70" t="str">
+        <v>51.92</v>
+      </c>
+      <c r="C70" t="str">
+        <v>51.92</v>
+      </c>
+      <c r="D70" t="str">
+        <v>0</v>
+      </c>
+      <c r="E70" t="str">
+        <v>44.72</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v>0x7e729b21005cF2FDda685bA7Bef04c6Dc3DcD444</v>
+      </c>
+      <c r="B71" t="str">
+        <v>4.81</v>
+      </c>
+      <c r="C71" t="str">
+        <v>4.81</v>
+      </c>
+      <c r="D71" t="str">
+        <v>4.15</v>
+      </c>
+      <c r="E71" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>0x18fc6c299B7aA35C8f59537b4b67c23D93E782ea</v>
+      </c>
+      <c r="B72" t="str">
+        <v>44,765.14</v>
+      </c>
+      <c r="C72" t="str">
+        <v>44,765.14</v>
+      </c>
+      <c r="D72" t="str">
+        <v>0</v>
+      </c>
+      <c r="E72" t="str">
+        <v>38,551.19</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>0xBBBA5cae882A16fEdAD9a92220C7dBF2d9Eb2313</v>
+      </c>
+      <c r="B73" t="str">
+        <v>1,989.25</v>
+      </c>
+      <c r="C73" t="str">
+        <v>1,989.25</v>
+      </c>
+      <c r="D73" t="str">
+        <v>0</v>
+      </c>
+      <c r="E73" t="str">
+        <v>1,713.12</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>0x430cB4360cE341a6Ad0Dfa18b9aD1Ae2cFa9AD18</v>
+      </c>
+      <c r="B74" t="str">
+        <v>1,697.43</v>
+      </c>
+      <c r="C74" t="str">
+        <v>1,697.43</v>
+      </c>
+      <c r="D74" t="str">
+        <v>0</v>
+      </c>
+      <c r="E74" t="str">
+        <v>1,461.81</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>0x494700b98fE1F432EeF0F5Ca8262D6d903F8a5Ab</v>
+      </c>
+      <c r="B75" t="str">
+        <v>1,211.72</v>
+      </c>
+      <c r="C75" t="str">
+        <v>1,211.72</v>
+      </c>
+      <c r="D75" t="str">
+        <v>0</v>
+      </c>
+      <c r="E75" t="str">
+        <v>1,043.52</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>0x889f1F09b491711013cA6787E29e07a04FDf42a4</v>
+      </c>
+      <c r="B76" t="str">
+        <v>237,594.93</v>
+      </c>
+      <c r="C76" t="str">
+        <v>237,594.93</v>
+      </c>
+      <c r="D76" t="str">
+        <v>25,974.89</v>
+      </c>
+      <c r="E76" t="str">
+        <v>178,638.95</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v>0x94B72396b6B40e19C2a04c28c8aE93dE08b12733</v>
+      </c>
+      <c r="B77" t="str">
+        <v>194,482.46</v>
+      </c>
+      <c r="C77" t="str">
+        <v>194,482.46</v>
+      </c>
+      <c r="D77" t="str">
+        <v>0</v>
+      </c>
+      <c r="E77" t="str">
+        <v>167,485.91</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="str">
+        <v>0xe9052daAC8667a27B38369aD37BEE63A8CD80Fc7</v>
+      </c>
+      <c r="B78" t="str">
+        <v>1,714.38</v>
+      </c>
+      <c r="C78" t="str">
+        <v>1,714.38</v>
+      </c>
+      <c r="D78" t="str">
+        <v>0</v>
+      </c>
+      <c r="E78" t="str">
+        <v>1,476.41</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="str">
+        <v>0x5eE2FC3425b4e3C908C6d6BcaDf3dce444BE8617</v>
+      </c>
+      <c r="B79" t="str">
+        <v>634.9</v>
+      </c>
+      <c r="C79" t="str">
+        <v>634.9</v>
+      </c>
+      <c r="D79" t="str">
+        <v>546.77</v>
+      </c>
+      <c r="E79" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="str">
+        <v>0xA53aFB483Fa417B9491C3a7AEAeDF463Ab687E29</v>
+      </c>
+      <c r="B80" t="str">
+        <v>13,743.43</v>
+      </c>
+      <c r="C80" t="str">
+        <v>13,743.43</v>
+      </c>
+      <c r="D80" t="str">
+        <v>11,835.68</v>
+      </c>
+      <c r="E80" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="str">
+        <v>0x126f38D7Dda782e2a33f2061556524C3aA9cE30B</v>
+      </c>
+      <c r="B81" t="str">
+        <v>13,743.43</v>
+      </c>
+      <c r="C81" t="str">
+        <v>13,743.43</v>
+      </c>
+      <c r="D81" t="str">
+        <v>0</v>
+      </c>
+      <c r="E81" t="str">
+        <v>11,835.68</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="str">
+        <v>0x387c310a3cC65aa12BC11CAF67a17b4a8693ed5e</v>
+      </c>
+      <c r="B82" t="str">
+        <v>11,129.75</v>
+      </c>
+      <c r="C82" t="str">
+        <v>11,129.75</v>
+      </c>
+      <c r="D82" t="str">
+        <v>9,584.81</v>
+      </c>
+      <c r="E82" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="str">
+        <v>0x9860C142d59D2d4cBE43c20a7F072A8C5Aac2057</v>
+      </c>
+      <c r="B83" t="str">
+        <v>8,390.06</v>
+      </c>
+      <c r="C83" t="str">
+        <v>8,390.06</v>
+      </c>
+      <c r="D83" t="str">
+        <v>7,225.42</v>
+      </c>
+      <c r="E83" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="str">
+        <v>0xFb286C7ca309a0B72885Fa2022633440C6334D6e</v>
+      </c>
+      <c r="B84" t="str">
+        <v>8,390.06</v>
+      </c>
+      <c r="C84" t="str">
+        <v>8,390.06</v>
+      </c>
+      <c r="D84" t="str">
+        <v>0</v>
+      </c>
+      <c r="E84" t="str">
+        <v>7,225.42</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="str">
+        <v>0x0fA1AfF9540786DCad9196e0676e2e4423317FAf</v>
+      </c>
+      <c r="B85" t="str">
+        <v>9,596.35</v>
+      </c>
+      <c r="C85" t="str">
+        <v>9,596.35</v>
+      </c>
+      <c r="D85" t="str">
+        <v>8,264.26</v>
+      </c>
+      <c r="E85" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="str">
+        <v>0x7011467e458B4cEEED928bac3E178Ce7EB892F2d</v>
+      </c>
+      <c r="B86" t="str">
+        <v>9,730.6</v>
+      </c>
+      <c r="C86" t="str">
+        <v>9,730.6</v>
+      </c>
+      <c r="D86" t="str">
+        <v>115.62</v>
+      </c>
+      <c r="E86" t="str">
+        <v>8,264.26</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="str">
+        <v>0x44dDf2A9375EF552A77973588E3964b9BBBe8191</v>
+      </c>
+      <c r="B87" t="str">
+        <v>3,232.73</v>
+      </c>
+      <c r="C87" t="str">
+        <v>3,232.73</v>
+      </c>
+      <c r="D87" t="str">
+        <v>2,783.99</v>
+      </c>
+      <c r="E87" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="str">
+        <v>0x681ee9C08368ED5e30519f146cF3A27b24471Dc6</v>
+      </c>
+      <c r="B88" t="str">
+        <v>0</v>
+      </c>
+      <c r="C88" t="str">
+        <v>3,232.73</v>
+      </c>
+      <c r="D88" t="str">
+        <v>0</v>
+      </c>
+      <c r="E88" t="str">
+        <v>2,783.99</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="str">
+        <v>0x0603709F92A47D5367Cc93f5b587A29fA286ADbB</v>
+      </c>
+      <c r="B89" t="str">
+        <v>6,739.71</v>
+      </c>
+      <c r="C89" t="str">
+        <v>6,739.71</v>
+      </c>
+      <c r="D89" t="str">
+        <v>0</v>
+      </c>
+      <c r="E89" t="str">
+        <v>5,804.16</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="str">
+        <v>0x778Ba6B5ca859F7c72df96Bf13D274e35a78a356</v>
+      </c>
+      <c r="B90" t="str">
+        <v>59.22</v>
+      </c>
+      <c r="C90" t="str">
+        <v>59.22</v>
+      </c>
+      <c r="D90" t="str">
+        <v>51</v>
+      </c>
+      <c r="E90" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="str">
+        <v>0xCf54bb8C360FB4Ec47AE0c31Bc8864B163651277</v>
+      </c>
+      <c r="B91" t="str">
+        <v>0</v>
+      </c>
+      <c r="C91" t="str">
+        <v>140.1</v>
+      </c>
+      <c r="D91" t="str">
+        <v>120.66</v>
+      </c>
+      <c r="E91" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="str">
+        <v>0x26763e975D773f46E8bA6AF80C09D9C90A07E14D</v>
+      </c>
+      <c r="B92" t="str">
+        <v>643.82</v>
+      </c>
+      <c r="C92" t="str">
+        <v>643.82</v>
+      </c>
+      <c r="D92" t="str">
+        <v>500</v>
+      </c>
+      <c r="E92" t="str">
+        <v>54.45</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="str">
+        <v>0x71c951E44E3D907dfa99D590cd7e6A235190dff4</v>
+      </c>
+      <c r="B93" t="str">
+        <v>580.59</v>
+      </c>
+      <c r="C93" t="str">
+        <v>580.59</v>
+      </c>
+      <c r="D93" t="str">
+        <v>0</v>
+      </c>
+      <c r="E93" t="str">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="str">
+        <v>0x4CaFc8E23616346de04DE62174B1e615D8E80c70</v>
+      </c>
+      <c r="B94" t="str">
+        <v>321.43</v>
+      </c>
+      <c r="C94" t="str">
+        <v>321.43</v>
+      </c>
+      <c r="D94" t="str">
+        <v>0</v>
+      </c>
+      <c r="E94" t="str">
+        <v>276.82</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="str">
+        <v>0x77940861e000BfC8A8f67440ad21656B9e7dbA04</v>
+      </c>
+      <c r="B95" t="str">
+        <v>35,222.79</v>
+      </c>
+      <c r="C95" t="str">
+        <v>35,222.79</v>
+      </c>
+      <c r="D95" t="str">
+        <v>30,333.44</v>
+      </c>
+      <c r="E95" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="str">
+        <v>0x6BF81D0d4f4e606C3cB09C45f6FA29f8743c72DE</v>
+      </c>
+      <c r="B96" t="str">
+        <v>0</v>
+      </c>
+      <c r="C96" t="str">
+        <v>35,222.79</v>
+      </c>
+      <c r="D96" t="str">
+        <v>0</v>
+      </c>
+      <c r="E96" t="str">
+        <v>30,333.44</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="str">
+        <v>0xe05DDFB83A8b66Df42f06BfB5517Fb5d6857a8ce</v>
+      </c>
+      <c r="B97" t="str">
+        <v>8,204.03</v>
+      </c>
+      <c r="C97" t="str">
+        <v>8,204.03</v>
+      </c>
+      <c r="D97" t="str">
+        <v>2,321.52</v>
+      </c>
+      <c r="E97" t="str">
+        <v>4,743.69</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="str">
+        <v>0x61c17C2EbD2647F82F7450b9956f1EE9357eA4B1</v>
+      </c>
+      <c r="B98" t="str">
+        <v>55,063.92</v>
+      </c>
+      <c r="C98" t="str">
+        <v>60,372.84</v>
+      </c>
+      <c r="D98" t="str">
+        <v>51,992.35</v>
+      </c>
+      <c r="E98" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="str">
+        <v>0xA66ABB96cC791CFD157CFcd404B27A0920824B35</v>
+      </c>
+      <c r="B99" t="str">
+        <v>0</v>
+      </c>
+      <c r="C99" t="str">
+        <v>267,806.07</v>
+      </c>
+      <c r="D99" t="str">
+        <v>178,638.95</v>
+      </c>
+      <c r="E99" t="str">
+        <v>51,992.35</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="str">
+        <v>0x531B206B50567FDF5029ae8bBc03d4C236ce185d</v>
+      </c>
+      <c r="B100" t="str">
+        <v>46.93</v>
+      </c>
+      <c r="C100" t="str">
+        <v>46.93</v>
+      </c>
+      <c r="D100" t="str">
+        <v>40.42</v>
+      </c>
+      <c r="E100" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="str">
+        <v>0x41382710CB3320194F0fb9Ef8e8531e0E291D740</v>
+      </c>
+      <c r="B101" t="str">
+        <v>233.45</v>
+      </c>
+      <c r="C101" t="str">
+        <v>233.45</v>
+      </c>
+      <c r="D101" t="str">
+        <v>201.05</v>
+      </c>
+      <c r="E101" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="str">
+        <v>0xAa00788779C2bB3C012BA6914A26cA5B23E02371</v>
+      </c>
+      <c r="B102" t="str">
+        <v>233.45</v>
+      </c>
+      <c r="C102" t="str">
+        <v>233.45</v>
+      </c>
+      <c r="D102" t="str">
+        <v>0</v>
+      </c>
+      <c r="E102" t="str">
+        <v>201.05</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="str">
+        <v>0x7B7e4eEA4BE17A75d0c2E72fcEe2c91DcfeACC45</v>
+      </c>
+      <c r="B103" t="str">
+        <v>3,530</v>
+      </c>
+      <c r="C103" t="str">
+        <v>3,530</v>
+      </c>
+      <c r="D103" t="str">
+        <v>3,040</v>
+      </c>
+      <c r="E103" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="str">
+        <v>0xd9C0e53199290dF3BFB223033f3eb6C16429af0e</v>
+      </c>
+      <c r="B104" t="str">
+        <v>3,530</v>
+      </c>
+      <c r="C104" t="str">
+        <v>3,530</v>
+      </c>
+      <c r="D104" t="str">
+        <v>0</v>
+      </c>
+      <c r="E104" t="str">
+        <v>3,040</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="str">
+        <v>0xc5f85e44C65783b4f1fD18D81CDA4e0Eb0eBb77d</v>
+      </c>
+      <c r="B105" t="str">
+        <v>93.54</v>
+      </c>
+      <c r="C105" t="str">
+        <v>93.54</v>
+      </c>
+      <c r="D105" t="str">
+        <v>80.56</v>
+      </c>
+      <c r="E105" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="str">
+        <v>0xAcF543A44c24aAdF47B50e5cc05c628f3F2A5046</v>
+      </c>
+      <c r="B106" t="str">
+        <v>18,968.52</v>
+      </c>
+      <c r="C106" t="str">
+        <v>18,968.52</v>
+      </c>
+      <c r="D106" t="str">
+        <v>9,967.11</v>
+      </c>
+      <c r="E106" t="str">
+        <v>6,368.35</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="str">
+        <v>0xe1cE7bDEae6757E29008f2ECA572b6208E23a822</v>
+      </c>
+      <c r="B107" t="str">
+        <v>3,499.42</v>
+      </c>
+      <c r="C107" t="str">
+        <v>3,499.42</v>
+      </c>
+      <c r="D107" t="str">
+        <v>3,013.66</v>
+      </c>
+      <c r="E107" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="str">
+        <v>0xb8D8066d1EE9D03800B7600d2807b7749B9F6899</v>
+      </c>
+      <c r="B108" t="str">
+        <v>290.29</v>
+      </c>
+      <c r="C108" t="str">
+        <v>290.29</v>
+      </c>
+      <c r="D108" t="str">
+        <v>250</v>
+      </c>
+      <c r="E108" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="str">
+        <v>0xD465Ffa5efAdF5cF1Dd6c45c3C305f58279A2140</v>
+      </c>
+      <c r="B109" t="str">
+        <v>0</v>
+      </c>
+      <c r="C109" t="str">
+        <v>290.29</v>
+      </c>
+      <c r="D109" t="str">
+        <v>0</v>
+      </c>
+      <c r="E109" t="str">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="str">
+        <v>0xd4e63B2004b55E2aE3c84451951D28dE1C5226Af</v>
+      </c>
+      <c r="B110" t="str">
+        <v>39.96</v>
+      </c>
+      <c r="C110" t="str">
+        <v>39.96</v>
+      </c>
+      <c r="D110" t="str">
+        <v>0</v>
+      </c>
+      <c r="E110" t="str">
+        <v>34.42</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="str">
+        <v>0xcFffD6F1C52280f46A0f32212150CbCaF50bBfb9</v>
+      </c>
+      <c r="B111" t="str">
+        <v>71.19</v>
+      </c>
+      <c r="C111" t="str">
+        <v>71.19</v>
+      </c>
+      <c r="D111" t="str">
+        <v>61.31</v>
+      </c>
+      <c r="E111" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="str">
+        <v>0x4f4EEe1b009725Bd92EF4368C3E69ca5Ee614541</v>
+      </c>
+      <c r="B112" t="str">
+        <v>28.29</v>
+      </c>
+      <c r="C112" t="str">
+        <v>28.29</v>
+      </c>
+      <c r="D112" t="str">
+        <v>0</v>
+      </c>
+      <c r="E112" t="str">
+        <v>24.37</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="str">
+        <v>0xC53Fa15adE563291bF8ba8d7E62a9B0959e6aE30</v>
+      </c>
+      <c r="B113" t="str">
+        <v>67.11</v>
+      </c>
+      <c r="C113" t="str">
+        <v>67.11</v>
+      </c>
+      <c r="D113" t="str">
+        <v>57.8</v>
+      </c>
+      <c r="E113" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="str">
+        <v>0xcE1290F5457067497EAd8Aea22515d52ca94357E</v>
+      </c>
+      <c r="B114" t="str">
+        <v>165</v>
+      </c>
+      <c r="C114" t="str">
+        <v>165</v>
+      </c>
+      <c r="D114" t="str">
+        <v>0</v>
+      </c>
+      <c r="E114" t="str">
+        <v>142.1</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="str">
+        <v>0x0254704C23C4765496894a632ef28d6be4DCB259</v>
+      </c>
+      <c r="B115" t="str">
+        <v>4,630.54</v>
+      </c>
+      <c r="C115" t="str">
+        <v>4,630.54</v>
+      </c>
+      <c r="D115" t="str">
+        <v>3,987.77</v>
+      </c>
+      <c r="E115" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="str">
+        <v>0x4994A7059A2921398780818c203F83613A9Bf743</v>
+      </c>
+      <c r="B116" t="str">
+        <v>86,038.08</v>
+      </c>
+      <c r="C116" t="str">
+        <v>86,038.08</v>
+      </c>
+      <c r="D116" t="str">
+        <v>70,000</v>
+      </c>
+      <c r="E116" t="str">
+        <v>4,094.94</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="str">
+        <v>0x425F2F1287045bC9d04C0f933E7FdEdA4A2e5765</v>
+      </c>
+      <c r="B117" t="str">
+        <v>2,858.79</v>
+      </c>
+      <c r="C117" t="str">
+        <v>2,858.79</v>
+      </c>
+      <c r="D117" t="str">
+        <v>0</v>
+      </c>
+      <c r="E117" t="str">
+        <v>2,461.96</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="str">
+        <v>0x358e444fFb60A1Cc82A6E412C6720f110dc1E921</v>
+      </c>
+      <c r="B118" t="str">
+        <v>0</v>
+      </c>
+      <c r="C118" t="str">
+        <v>4,222.52</v>
+      </c>
+      <c r="D118" t="str">
+        <v>0</v>
+      </c>
+      <c r="E118" t="str">
+        <v>3,636.39</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="str">
+        <v>0xFeD4972A2Ee597c587C1b0643849845544c17C2F</v>
+      </c>
+      <c r="B119" t="str">
+        <v>1,071.24</v>
+      </c>
+      <c r="C119" t="str">
+        <v>1,071.24</v>
+      </c>
+      <c r="D119" t="str">
+        <v>0</v>
+      </c>
+      <c r="E119" t="str">
+        <v>922.54</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="str">
+        <v>0x212172E536d6c24f46D64F57f8FA64E201882146</v>
+      </c>
+      <c r="B120" t="str">
+        <v>293.46</v>
+      </c>
+      <c r="C120" t="str">
+        <v>293.46</v>
+      </c>
+      <c r="D120" t="str">
+        <v>252.73</v>
+      </c>
+      <c r="E120" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="str">
+        <v>0x2A1Cc6c77782EA6BE6C08d61430A79E31Ea4efDf</v>
+      </c>
+      <c r="B121" t="str">
+        <v>149.95</v>
+      </c>
+      <c r="C121" t="str">
+        <v>149.95</v>
+      </c>
+      <c r="D121" t="str">
+        <v>0</v>
+      </c>
+      <c r="E121" t="str">
+        <v>129.14</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="str">
+        <v>0x233680379B54D12357711b431Be3B8a4cdfBe6bD</v>
+      </c>
+      <c r="B122" t="str">
+        <v>107.1</v>
+      </c>
+      <c r="C122" t="str">
+        <v>107.1</v>
+      </c>
+      <c r="D122" t="str">
+        <v>92.24</v>
+      </c>
+      <c r="E122" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="str">
+        <v>0x9342fD3f10101019Cf9e6774640957fa1d7A78B2</v>
+      </c>
+      <c r="B123" t="str">
+        <v>827.83</v>
+      </c>
+      <c r="C123" t="str">
+        <v>827.83</v>
+      </c>
+      <c r="D123" t="str">
+        <v>362.27</v>
+      </c>
+      <c r="E123" t="str">
+        <v>350.65</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="str">
+        <v>0xDbfd080A579b7DFc5D99834C86ffd543b688c864</v>
+      </c>
+      <c r="B124" t="str">
+        <v>1,916.74</v>
+      </c>
+      <c r="C124" t="str">
+        <v>1,916.74</v>
+      </c>
+      <c r="D124" t="str">
+        <v>1,650.68</v>
+      </c>
+      <c r="E124" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="str">
+        <v>0x69f96f2A5Cdd84E574dB2a353880095988243417</v>
+      </c>
+      <c r="B125" t="str">
+        <v>0</v>
+      </c>
+      <c r="C125" t="str">
+        <v>5,246.88</v>
+      </c>
+      <c r="D125" t="str">
+        <v>4,518.55</v>
+      </c>
+      <c r="E125" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="str">
+        <v>0xEA67438f0857e93968F50aE87db18720b9E457Ef</v>
+      </c>
+      <c r="B126" t="str">
+        <v>11,331.51</v>
+      </c>
+      <c r="C126" t="str">
+        <v>11,331.51</v>
+      </c>
+      <c r="D126" t="str">
+        <v>0</v>
+      </c>
+      <c r="E126" t="str">
+        <v>9,758.56</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="str">
+        <v>0x9AFd15a40275947bDD6824ba0eAfE1cCe4143a2F</v>
+      </c>
+      <c r="B127" t="str">
+        <v>378.04</v>
+      </c>
+      <c r="C127" t="str">
+        <v>378.04</v>
+      </c>
+      <c r="D127" t="str">
+        <v>325.57</v>
+      </c>
+      <c r="E127" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="str">
+        <v>0xF473Ea7dc6E82C348530FDE410bFF035bCe0B269</v>
+      </c>
+      <c r="B128" t="str">
+        <v>958.64</v>
+      </c>
+      <c r="C128" t="str">
+        <v>958.64</v>
+      </c>
+      <c r="D128" t="str">
+        <v>0</v>
+      </c>
+      <c r="E128" t="str">
+        <v>825.57</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="str">
+        <v>0xb78b932C7FA6f818D2c46aD42B38c4E9289660E4</v>
+      </c>
+      <c r="B129" t="str">
+        <v>4,716.57</v>
+      </c>
+      <c r="C129" t="str">
+        <v>4,716.57</v>
+      </c>
+      <c r="D129" t="str">
+        <v>0</v>
+      </c>
+      <c r="E129" t="str">
+        <v>4,061.86</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="str">
+        <v>0x88852100b52867c80eaa3b5eA0500F4bFB7E5899</v>
+      </c>
+      <c r="B130" t="str">
+        <v>7.91</v>
+      </c>
+      <c r="C130" t="str">
+        <v>7.91</v>
+      </c>
+      <c r="D130" t="str">
+        <v>6.82</v>
+      </c>
+      <c r="E130" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="str">
+        <v>0x5284F4d83AFBF50c661169FC50376aec49a2eEC4</v>
+      </c>
+      <c r="B131" t="str">
+        <v>7.91</v>
+      </c>
+      <c r="C131" t="str">
+        <v>7.91</v>
+      </c>
+      <c r="D131" t="str">
+        <v>0</v>
+      </c>
+      <c r="E131" t="str">
+        <v>6.82</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="str">
+        <v>0x9C19FE52c5b04d39EF89d58fCDef24A55CfDA4a7</v>
+      </c>
+      <c r="B132" t="str">
+        <v>98.35</v>
+      </c>
+      <c r="C132" t="str">
+        <v>98.35</v>
+      </c>
+      <c r="D132" t="str">
+        <v>84.7</v>
+      </c>
+      <c r="E132" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="str">
+        <v>0x73A4386890268E835d8d01598D06A44d47A489d8</v>
+      </c>
+      <c r="B133" t="str">
+        <v>245.33</v>
+      </c>
+      <c r="C133" t="str">
+        <v>245.33</v>
+      </c>
+      <c r="D133" t="str">
+        <v>0</v>
+      </c>
+      <c r="E133" t="str">
+        <v>211.28</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="str">
+        <v>0xe2e039dD3206870FE6Ad4B88DDf74730c355B2e5</v>
+      </c>
+      <c r="B134" t="str">
+        <v>21,795.09</v>
+      </c>
+      <c r="C134" t="str">
+        <v>21,795.09</v>
+      </c>
+      <c r="D134" t="str">
+        <v>0</v>
+      </c>
+      <c r="E134" t="str">
+        <v>18,769.67</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="str">
+        <v>0xBcb9C22A0b6479E1519fC26a9499FE12AeA0c848</v>
+      </c>
+      <c r="B135" t="str">
+        <v>1,533.09</v>
+      </c>
+      <c r="C135" t="str">
+        <v>1,533.09</v>
+      </c>
+      <c r="D135" t="str">
+        <v>235.01</v>
+      </c>
+      <c r="E135" t="str">
+        <v>1,085.27</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="str">
+        <v>0x240e0289a4d0D6B1b412ad1A4fD04711656A29ee</v>
+      </c>
+      <c r="B136" t="str">
+        <v>201.67</v>
+      </c>
+      <c r="C136" t="str">
+        <v>201.67</v>
+      </c>
+      <c r="D136" t="str">
+        <v>173.68</v>
+      </c>
+      <c r="E136" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="str">
+        <v>0x262ba7354bA2946de8f90dCe06883FaFebB6f043</v>
+      </c>
+      <c r="B137" t="str">
+        <v>26,905.19</v>
+      </c>
+      <c r="C137" t="str">
+        <v>26,905.19</v>
+      </c>
+      <c r="D137" t="str">
+        <v>0</v>
+      </c>
+      <c r="E137" t="str">
+        <v>23,170.42</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="str">
+        <v>0x3636D15fa9BBE63B1e67494f4604eD13E224F405</v>
+      </c>
+      <c r="B138" t="str">
+        <v>31.53</v>
+      </c>
+      <c r="C138" t="str">
+        <v>31.53</v>
+      </c>
+      <c r="D138" t="str">
+        <v>27.16</v>
+      </c>
+      <c r="E138" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="str">
+        <v>0xfDbb14D0A9a2f85663134F16BF006c08e2918B6a</v>
+      </c>
+      <c r="B139" t="str">
+        <v>118.8</v>
+      </c>
+      <c r="C139" t="str">
+        <v>118.8</v>
+      </c>
+      <c r="D139" t="str">
+        <v>0</v>
+      </c>
+      <c r="E139" t="str">
+        <v>102.31</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="str">
+        <v>0x74c0d21e8ffC5b83dce1A0BB6abCD061D071E85a</v>
+      </c>
+      <c r="B140" t="str">
+        <v>17,260.87</v>
+      </c>
+      <c r="C140" t="str">
+        <v>17,260.87</v>
+      </c>
+      <c r="D140" t="str">
+        <v>4,897.74</v>
+      </c>
+      <c r="E140" t="str">
+        <v>9,967.11</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="str">
+        <v>0xB19c1b3cEc4c5bD6DCA220A4f59de9EC681e9211</v>
+      </c>
+      <c r="B141" t="str">
+        <v>0</v>
+      </c>
+      <c r="C141" t="str">
+        <v>180.95</v>
+      </c>
+      <c r="D141" t="str">
+        <v>12.73</v>
+      </c>
+      <c r="E141" t="str">
+        <v>143.11</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="str">
+        <v>0x175780bC4d0A1bc28c46C3E71130C092790E7576</v>
+      </c>
+      <c r="B142" t="str">
+        <v>166.17</v>
+      </c>
+      <c r="C142" t="str">
+        <v>166.17</v>
+      </c>
+      <c r="D142" t="str">
+        <v>143.11</v>
+      </c>
+      <c r="E142" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="str">
+        <v>0x19d4dEce6C48d99F0Ec4bE4258f26fdA9a7Ad4e5</v>
+      </c>
+      <c r="B143" t="str">
+        <v>350.87</v>
+      </c>
+      <c r="C143" t="str">
+        <v>350.87</v>
+      </c>
+      <c r="D143" t="str">
+        <v>302.17</v>
+      </c>
+      <c r="E143" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="str">
+        <v>0x0c9168A60476c84DeD650f13837892725D25DeB1</v>
+      </c>
+      <c r="B144" t="str">
+        <v>20.88</v>
+      </c>
+      <c r="C144" t="str">
+        <v>20.88</v>
+      </c>
+      <c r="D144" t="str">
+        <v>0</v>
+      </c>
+      <c r="E144" t="str">
+        <v>17.99</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="str">
+        <v>0xb76c661bad5bbc54F1D4a7BF7663211aa34455D8</v>
+      </c>
+      <c r="B145" t="str">
+        <v>3,193.26</v>
+      </c>
+      <c r="C145" t="str">
+        <v>3,193.26</v>
+      </c>
+      <c r="D145" t="str">
+        <v>2,750</v>
+      </c>
+      <c r="E145" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="str">
+        <v>0x746F83FF7eAdA9d0fB03DbAbcAF2600ee513DCDB</v>
+      </c>
+      <c r="B146" t="str">
+        <v>7,257.41</v>
+      </c>
+      <c r="C146" t="str">
+        <v>7,257.41</v>
+      </c>
+      <c r="D146" t="str">
+        <v>0</v>
+      </c>
+      <c r="E146" t="str">
+        <v>6,250</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="str">
+        <v>0x8538330Cd197d24CDdF7DEe46309c2ad9428FACc</v>
+      </c>
+      <c r="B147" t="str">
+        <v>32.82</v>
+      </c>
+      <c r="C147" t="str">
+        <v>32.82</v>
+      </c>
+      <c r="D147" t="str">
+        <v>28.27</v>
+      </c>
+      <c r="E147" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="str">
+        <v>0x4922dc29D2d0c725F542f5021D9353F3872F2dFF</v>
+      </c>
+      <c r="B148" t="str">
+        <v>580.59</v>
+      </c>
+      <c r="C148" t="str">
+        <v>580.59</v>
+      </c>
+      <c r="D148" t="str">
+        <v>500</v>
+      </c>
+      <c r="E148" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="str">
+        <v>0x4e0F1063F13d020B1316791Ae56ea5a826aba501</v>
+      </c>
+      <c r="B149" t="str">
+        <v>62.26</v>
+      </c>
+      <c r="C149" t="str">
+        <v>62.26</v>
+      </c>
+      <c r="D149" t="str">
+        <v>0</v>
+      </c>
+      <c r="E149" t="str">
+        <v>53.62</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="str">
+        <v>0xdC2F100fCabBa1660d8714E2F15664488Ab4F25D</v>
+      </c>
+      <c r="B150" t="str">
+        <v>102.11</v>
+      </c>
+      <c r="C150" t="str">
+        <v>102.11</v>
+      </c>
+      <c r="D150" t="str">
+        <v>87.94</v>
+      </c>
+      <c r="E150" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="str">
+        <v>0xc003A6Dab5463E71667324fe7F50F36199B22674</v>
+      </c>
+      <c r="B151" t="str">
+        <v>357.77</v>
+      </c>
+      <c r="C151" t="str">
+        <v>357.77</v>
+      </c>
+      <c r="D151" t="str">
+        <v>0</v>
+      </c>
+      <c r="E151" t="str">
+        <v>308.11</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="str">
+        <v>0x96f194Cf1c9e5eE23B4D96785791F468F6A9C98e</v>
+      </c>
+      <c r="B152" t="str">
+        <v>81,283.09</v>
+      </c>
+      <c r="C152" t="str">
+        <v>81,283.09</v>
+      </c>
+      <c r="D152" t="str">
+        <v>0</v>
+      </c>
+      <c r="E152" t="str">
+        <v>70,000</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="str">
+        <v>0x09aFEC89b908C2cbD220942f3788530C195Ba894</v>
+      </c>
+      <c r="B153" t="str">
+        <v>597.46</v>
+      </c>
+      <c r="C153" t="str">
+        <v>597.46</v>
+      </c>
+      <c r="D153" t="str">
+        <v>0</v>
+      </c>
+      <c r="E153" t="str">
+        <v>514.53</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="str">
+        <v>0x23ac940D8098674DE7D2d86B4264C1eB892Fe4AD</v>
+      </c>
+      <c r="B154" t="str">
+        <v>777.13</v>
+      </c>
+      <c r="C154" t="str">
+        <v>777.13</v>
+      </c>
+      <c r="D154" t="str">
+        <v>0</v>
+      </c>
+      <c r="E154" t="str">
+        <v>669.26</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="str">
+        <v>0xF6a52cb99b772d46C736F6F90Be792A1d4159414</v>
+      </c>
+      <c r="B155" t="str">
+        <v>49.4</v>
+      </c>
+      <c r="C155" t="str">
+        <v>49.4</v>
+      </c>
+      <c r="D155" t="str">
+        <v>42.55</v>
+      </c>
+      <c r="E155" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="str">
+        <v>0xdFdf143A6a12185023e01ddC61092Ac97eCB6c05</v>
+      </c>
+      <c r="B156" t="str">
+        <v>119.45</v>
+      </c>
+      <c r="C156" t="str">
+        <v>119.45</v>
+      </c>
+      <c r="D156" t="str">
+        <v>102.87</v>
+      </c>
+      <c r="E156" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="str">
+        <v>0x16CaEA275D4F7cF454537b121915D92Bc5CB8C16</v>
+      </c>
+      <c r="B157" t="str">
+        <v>67,137.05</v>
+      </c>
+      <c r="C157" t="str">
+        <v>67,137.05</v>
+      </c>
+      <c r="D157" t="str">
+        <v>57,817.61</v>
+      </c>
+      <c r="E157" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="str">
+        <v>0x47502539673c93B2ACDC9059B36360f76D3548BB</v>
+      </c>
+      <c r="B158" t="str">
+        <v>2,616.15</v>
+      </c>
+      <c r="C158" t="str">
+        <v>2,616.15</v>
+      </c>
+      <c r="D158" t="str">
+        <v>0</v>
+      </c>
+      <c r="E158" t="str">
+        <v>2,253</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="str">
+        <v>0xBc7b31dFbEd762841AC646961C887B49e3f625d5</v>
+      </c>
+      <c r="B159" t="str">
+        <v>356.49</v>
+      </c>
+      <c r="C159" t="str">
+        <v>356.49</v>
+      </c>
+      <c r="D159" t="str">
+        <v>307.01</v>
+      </c>
+      <c r="E159" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="str">
+        <v>0xc4b88bff8D047576eC693EaFA72482A5e8f0fd7A</v>
+      </c>
+      <c r="B160" t="str">
+        <v>100</v>
+      </c>
+      <c r="C160" t="str">
+        <v>100</v>
+      </c>
+      <c r="D160" t="str">
+        <v>86.12</v>
+      </c>
+      <c r="E160" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="str">
+        <v>0xD44E29759A73d29F7887702F864406b16612BF5e</v>
+      </c>
+      <c r="B161" t="str">
+        <v>0</v>
+      </c>
+      <c r="C161" t="str">
+        <v>2,695.71</v>
+      </c>
+      <c r="D161" t="str">
+        <v>0</v>
+      </c>
+      <c r="E161" t="str">
+        <v>2,321.52</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="str">
+        <v>0x886049Df7a8010a7e3c21A32b74e41402986ae37</v>
+      </c>
+      <c r="B162" t="str">
+        <v>133.07</v>
+      </c>
+      <c r="C162" t="str">
+        <v>133.07</v>
+      </c>
+      <c r="D162" t="str">
+        <v>114.6</v>
+      </c>
+      <c r="E162" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="str">
+        <v>0x9f0bE4E742e7d98a8837388b83d508d4A483AECF</v>
+      </c>
+      <c r="B163" t="str">
+        <v>8,092.05</v>
+      </c>
+      <c r="C163" t="str">
+        <v>8,092.05</v>
+      </c>
+      <c r="D163" t="str">
+        <v>6,968.78</v>
+      </c>
+      <c r="E163" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="str">
+        <v>0x9A4dbCDE63b55273DC51BeA546A7ba6456f059D0</v>
+      </c>
+      <c r="B164" t="str">
+        <v>2,043.32</v>
+      </c>
+      <c r="C164" t="str">
+        <v>2,043.32</v>
+      </c>
+      <c r="D164" t="str">
+        <v>0</v>
+      </c>
+      <c r="E164" t="str">
+        <v>1,759.69</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="str">
+        <v>0x5C9A07e59Bdc264d0579530b4e08338122833942</v>
+      </c>
+      <c r="B165" t="str">
+        <v>1,436.73</v>
+      </c>
+      <c r="C165" t="str">
+        <v>1,436.73</v>
+      </c>
+      <c r="D165" t="str">
+        <v>0</v>
+      </c>
+      <c r="E165" t="str">
+        <v>1,237.3</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="str">
+        <v>0xfA9FBD6360692a1b23b84A9dDFf63ed77faF58c9</v>
+      </c>
+      <c r="B166" t="str">
+        <v>17.68</v>
+      </c>
+      <c r="C166" t="str">
+        <v>17.68</v>
+      </c>
+      <c r="D166" t="str">
+        <v>0</v>
+      </c>
+      <c r="E166" t="str">
+        <v>15.23</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="str">
+        <v>0x88d6B2Cdb0fEf078621De5308aD787CC147C76C0</v>
+      </c>
+      <c r="B167" t="str">
+        <v>50.59</v>
+      </c>
+      <c r="C167" t="str">
+        <v>50.59</v>
+      </c>
+      <c r="D167" t="str">
+        <v>0</v>
+      </c>
+      <c r="E167" t="str">
+        <v>43.57</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="str">
+        <v>0x9C4e5edC6A735e4AB68ef04497b64008A955A1A5</v>
+      </c>
+      <c r="B168" t="str">
+        <v>715.26</v>
+      </c>
+      <c r="C168" t="str">
+        <v>715.26</v>
+      </c>
+      <c r="D168" t="str">
+        <v>0</v>
+      </c>
+      <c r="E168" t="str">
+        <v>615.98</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="str">
+        <v>0x1DA42d0A3108af9D1f8eB3bFd80bD26FBE2d911d</v>
+      </c>
+      <c r="B169" t="str">
+        <v>44,560.21</v>
+      </c>
+      <c r="C169" t="str">
+        <v>44,560.21</v>
+      </c>
+      <c r="D169" t="str">
+        <v>38,374.71</v>
+      </c>
+      <c r="E169" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="str">
+        <v>0xbdAb516d352Adf142207EA2F7749c4a7e0543a55</v>
+      </c>
+      <c r="B170" t="str">
+        <v>11,449.64</v>
+      </c>
+      <c r="C170" t="str">
+        <v>11,449.64</v>
+      </c>
+      <c r="D170" t="str">
+        <v>9,860.29</v>
+      </c>
+      <c r="E170" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="str">
+        <v>0x53ca313FFDcAADAd0CCa71b3eEf7fDc57d83Bfed</v>
+      </c>
+      <c r="B171" t="str">
+        <v>70.01</v>
+      </c>
+      <c r="C171" t="str">
+        <v>70.01</v>
+      </c>
+      <c r="D171" t="str">
+        <v>60.3</v>
+      </c>
+      <c r="E171" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="str">
+        <v>0x555D98207F3Cb7fdB6fB7217A081A365ca45c135</v>
+      </c>
+      <c r="B172" t="str">
+        <v>70.01</v>
+      </c>
+      <c r="C172" t="str">
+        <v>70.01</v>
+      </c>
+      <c r="D172" t="str">
+        <v>0</v>
+      </c>
+      <c r="E172" t="str">
+        <v>60.3</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="str">
+        <v>0x89c7eF9CE8c8B7C683f8051f355B5f6B55acA4De</v>
+      </c>
+      <c r="B173" t="str">
+        <v>94.81</v>
+      </c>
+      <c r="C173" t="str">
+        <v>94.81</v>
+      </c>
+      <c r="D173" t="str">
+        <v>81.65</v>
+      </c>
+      <c r="E173" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="str">
+        <v>0x2848A658c1097a8639d2fb62a977b23903200b53</v>
+      </c>
+      <c r="B174" t="str">
+        <v>94.81</v>
+      </c>
+      <c r="C174" t="str">
+        <v>94.81</v>
+      </c>
+      <c r="D174" t="str">
+        <v>0</v>
+      </c>
+      <c r="E174" t="str">
+        <v>81.65</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="str">
+        <v>0xC023483Fa22d037EC5f056FC31C8f40751722aD5</v>
+      </c>
+      <c r="B175" t="str">
+        <v>58.05</v>
+      </c>
+      <c r="C175" t="str">
+        <v>58.05</v>
+      </c>
+      <c r="D175" t="str">
+        <v>0</v>
+      </c>
+      <c r="E175" t="str">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="str">
+        <v>0xeBB36F543A6c3E09a06c937E86fB0930a6EdA151</v>
+      </c>
+      <c r="B176" t="str">
+        <v>174.17</v>
+      </c>
+      <c r="C176" t="str">
+        <v>174.17</v>
+      </c>
+      <c r="D176" t="str">
+        <v>0</v>
+      </c>
+      <c r="E176" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="str">
+        <v>0xFb9Fa9E9276D1631fc4f72c32c19628a8d8a3935</v>
+      </c>
+      <c r="B177" t="str">
+        <v>2,888.92</v>
+      </c>
+      <c r="C177" t="str">
+        <v>2,888.92</v>
+      </c>
+      <c r="D177" t="str">
+        <v>2,487.91</v>
+      </c>
+      <c r="E177" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="str">
+        <v>0xd0bC9CB19A72c6DDE6206d302E049D6E0496a453</v>
+      </c>
+      <c r="B178" t="str">
+        <v>2,888.92</v>
+      </c>
+      <c r="C178" t="str">
+        <v>2,888.92</v>
+      </c>
+      <c r="D178" t="str">
+        <v>0</v>
+      </c>
+      <c r="E178" t="str">
+        <v>2,487.91</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="str">
+        <v>0x1A24A8CDa46ACac40606af1D233dAfF9AEe66e2f</v>
+      </c>
+      <c r="B179" t="str">
+        <v>95.7</v>
+      </c>
+      <c r="C179" t="str">
+        <v>95.7</v>
+      </c>
+      <c r="D179" t="str">
+        <v>0</v>
+      </c>
+      <c r="E179" t="str">
+        <v>82.42</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="str">
+        <v>0xFa544d034dC07aD4Fa185ba769031a29Fbef5e36</v>
+      </c>
+      <c r="B180" t="str">
+        <v>18.81</v>
+      </c>
+      <c r="C180" t="str">
+        <v>18.81</v>
+      </c>
+      <c r="D180" t="str">
+        <v>0</v>
+      </c>
+      <c r="E180" t="str">
+        <v>16.2</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="str">
+        <v>0xd5d071b3A56381308F4B9Fa560AAd7876Df292c7</v>
+      </c>
+      <c r="B181" t="str">
+        <v>577,271.42</v>
+      </c>
+      <c r="C181" t="str">
+        <v>577,271.42</v>
+      </c>
+      <c r="D181" t="str">
+        <v>248,448.98</v>
+      </c>
+      <c r="E181" t="str">
+        <v>248,690.08</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="str">
+        <v>0x1B5f7cBb775f11BC5CFC4ac9dC1406Ef613F7A63</v>
+      </c>
+      <c r="B182" t="str">
+        <v>19.84</v>
+      </c>
+      <c r="C182" t="str">
+        <v>19.84</v>
+      </c>
+      <c r="D182" t="str">
+        <v>17.09</v>
+      </c>
+      <c r="E182" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="str">
+        <v>0xb26C7c04A98eb3b92a2688ee8Fc1dA17054eF909</v>
+      </c>
+      <c r="B183" t="str">
+        <v>284.49</v>
+      </c>
+      <c r="C183" t="str">
+        <v>284.49</v>
+      </c>
+      <c r="D183" t="str">
+        <v>0</v>
+      </c>
+      <c r="E183" t="str">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="str">
+        <v>0x27e0D3A0D88BACaD8720aa9c6Bf7e0d099f3bCEa</v>
+      </c>
+      <c r="B184" t="str">
+        <v>510</v>
+      </c>
+      <c r="C184" t="str">
+        <v>697.01</v>
+      </c>
+      <c r="D184" t="str">
+        <v>600.26</v>
+      </c>
+      <c r="E184" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="str">
+        <v>0xa427746a2606c82afaa69cE757E0705c2c8081a1</v>
+      </c>
+      <c r="B185" t="str">
+        <v>54.32</v>
+      </c>
+      <c r="C185" t="str">
+        <v>54.32</v>
+      </c>
+      <c r="D185" t="str">
+        <v>0</v>
+      </c>
+      <c r="E185" t="str">
+        <v>46.78</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="str">
+        <v>0xf6FE07aC323c53d2445C06566F040056a31B0612</v>
+      </c>
+      <c r="B186" t="str">
+        <v>20,996.02</v>
+      </c>
+      <c r="C186" t="str">
+        <v>20,996.02</v>
+      </c>
+      <c r="D186" t="str">
+        <v>18,081.52</v>
+      </c>
+      <c r="E186" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="str">
+        <v>0x4CEbE974145E6796dB356F3689082D2d1eEf02Bf</v>
+      </c>
+      <c r="B187" t="str">
+        <v>116.11</v>
+      </c>
+      <c r="C187" t="str">
+        <v>116.11</v>
+      </c>
+      <c r="D187" t="str">
+        <v>100</v>
+      </c>
+      <c r="E187" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="str">
+        <v>0x9137e3E86cFf5736277B418E41449CC3428F5317</v>
+      </c>
+      <c r="B188" t="str">
+        <v>116.11</v>
+      </c>
+      <c r="C188" t="str">
+        <v>116.11</v>
+      </c>
+      <c r="D188" t="str">
+        <v>0</v>
+      </c>
+      <c r="E188" t="str">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="str">
+        <v>0x880cd618B4cA66bBb8862558954d8473d7b0C867</v>
+      </c>
+      <c r="B189" t="str">
+        <v>1,285.92</v>
+      </c>
+      <c r="C189" t="str">
+        <v>1,285.92</v>
+      </c>
+      <c r="D189" t="str">
+        <v>1,107.42</v>
+      </c>
+      <c r="E189" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="str">
+        <v>0x9ff812DfE804e2BF400Fd6fD22293203674DDdEe</v>
+      </c>
+      <c r="B190" t="str">
+        <v>50.47</v>
+      </c>
+      <c r="C190" t="str">
+        <v>50.47</v>
+      </c>
+      <c r="D190" t="str">
+        <v>0</v>
+      </c>
+      <c r="E190" t="str">
+        <v>43.47</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="str">
+        <v>0x2728c19586e1eB6b2AA599c15fA1456426C7CC7C</v>
+      </c>
+      <c r="B191" t="str">
+        <v>2,800.28</v>
+      </c>
+      <c r="C191" t="str">
+        <v>2,800.28</v>
+      </c>
+      <c r="D191" t="str">
+        <v>2,407.06</v>
+      </c>
+      <c r="E191" t="str">
+        <v>4.51</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="str">
+        <v>0x1893c5D2fb92D2AD0990943E952D8370bfBD9463</v>
+      </c>
+      <c r="B192" t="str">
+        <v>44.84</v>
+      </c>
+      <c r="C192" t="str">
+        <v>44.84</v>
+      </c>
+      <c r="D192" t="str">
+        <v>0</v>
+      </c>
+      <c r="E192" t="str">
+        <v>38.62</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="str">
+        <v>0xe5C5B9C648a3e66A2A7b8a3f2dA48e76e8309A2C</v>
+      </c>
+      <c r="B193" t="str">
+        <v>2,802.21</v>
+      </c>
+      <c r="C193" t="str">
+        <v>2,802.21</v>
+      </c>
+      <c r="D193" t="str">
+        <v>2,403.63</v>
+      </c>
+      <c r="E193" t="str">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="str">
+        <v>0x48A7209DD07Bc7409bF3f61820E1Ee9409F462e9</v>
+      </c>
+      <c r="B194" t="str">
+        <v>219.48</v>
+      </c>
+      <c r="C194" t="str">
+        <v>219.48</v>
+      </c>
+      <c r="D194" t="str">
+        <v>0</v>
+      </c>
+      <c r="E194" t="str">
+        <v>189.02</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="str">
+        <v>0xAE1aD5B0Cb04CFe479E9308006F2e0063Ab8E845</v>
+      </c>
+      <c r="B195" t="str">
+        <v>138.13</v>
+      </c>
+      <c r="C195" t="str">
+        <v>138.13</v>
+      </c>
+      <c r="D195" t="str">
+        <v>0</v>
+      </c>
+      <c r="E195" t="str">
+        <v>118.96</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="str">
+        <v>0xf85F765B52C7c319287d669D8682eC33eA52Bca9</v>
+      </c>
+      <c r="B196" t="str">
+        <v>63.22</v>
+      </c>
+      <c r="C196" t="str">
+        <v>63.22</v>
+      </c>
+      <c r="D196" t="str">
+        <v>54.45</v>
+      </c>
+      <c r="E196" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="str">
+        <v>0x040f62A18EB5D5ca87A08E41A22D004ee7A26380</v>
+      </c>
+      <c r="B197" t="str">
+        <v>1,465.48</v>
+      </c>
+      <c r="C197" t="str">
+        <v>1,465.48</v>
+      </c>
+      <c r="D197" t="str">
+        <v>0</v>
+      </c>
+      <c r="E197" t="str">
+        <v>1,262.06</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="str">
+        <v>0xC8a3B31C5d3Ba95Eec7377887a445BE34AfEE3BD</v>
+      </c>
+      <c r="B198" t="str">
+        <v>870.89</v>
+      </c>
+      <c r="C198" t="str">
+        <v>870.89</v>
+      </c>
+      <c r="D198" t="str">
+        <v>750</v>
+      </c>
+      <c r="E198" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="str">
+        <v>0xBe1f72dA08102c8B54EbCde91c68f07f759f2712</v>
+      </c>
+      <c r="B199" t="str">
+        <v>1,384.56</v>
+      </c>
+      <c r="C199" t="str">
+        <v>1,384.56</v>
+      </c>
+      <c r="D199" t="str">
+        <v>0</v>
+      </c>
+      <c r="E199" t="str">
+        <v>1,192.37</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="str">
+        <v>0xE2D8A9f98072298241651a1c899907892860A1f5</v>
+      </c>
+      <c r="B200" t="str">
+        <v>0</v>
+      </c>
+      <c r="C200" t="str">
+        <v>8.17</v>
+      </c>
+      <c r="D200" t="str">
+        <v>7.04</v>
+      </c>
+      <c r="E200" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="str">
+        <v>0x231E89f21Da8d752262D42ad835B30D0Ee0aF8c5</v>
+      </c>
+      <c r="B201" t="str">
+        <v>25.41</v>
+      </c>
+      <c r="C201" t="str">
+        <v>25.41</v>
+      </c>
+      <c r="D201" t="str">
+        <v>0</v>
+      </c>
+      <c r="E201" t="str">
+        <v>21.89</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="str">
+        <v>0xB6e85e12331BdEA6fF03b25d3dE68a892C99C5D4</v>
+      </c>
+      <c r="B202" t="str">
+        <v>158.33</v>
+      </c>
+      <c r="C202" t="str">
+        <v>158.33</v>
+      </c>
+      <c r="D202" t="str">
+        <v>0</v>
+      </c>
+      <c r="E202" t="str">
+        <v>136.36</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="str">
+        <v>0xa7B320Ea5368EC4990Ec76E1C1719aFddeE876d6</v>
+      </c>
+      <c r="B203" t="str">
+        <v>4,086.86</v>
+      </c>
+      <c r="C203" t="str">
+        <v>4,086.86</v>
+      </c>
+      <c r="D203" t="str">
+        <v>0</v>
+      </c>
+      <c r="E203" t="str">
+        <v>3,519.56</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="str">
+        <v>0xedaa63C95A0faB8e7Dc7A710f8b9Aa6ee461dAC7</v>
+      </c>
+      <c r="B204" t="str">
+        <v>1,051.88</v>
+      </c>
+      <c r="C204" t="str">
+        <v>1,051.88</v>
+      </c>
+      <c r="D204" t="str">
+        <v>905.87</v>
+      </c>
+      <c r="E204" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="str">
+        <v>0xd19d505d3618A142E85bd1A2A8C0878cD2b1089d</v>
+      </c>
+      <c r="B205" t="str">
+        <v>1,051.88</v>
+      </c>
+      <c r="C205" t="str">
+        <v>1,051.88</v>
+      </c>
+      <c r="D205" t="str">
+        <v>0</v>
+      </c>
+      <c r="E205" t="str">
+        <v>905.87</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="str">
+        <v>0x361631d54F49b6a4C19F033Ef507D67aC6BA1c0a</v>
+      </c>
+      <c r="B206" t="str">
+        <v>470.31</v>
+      </c>
+      <c r="C206" t="str">
+        <v>470.31</v>
+      </c>
+      <c r="D206" t="str">
+        <v>405.03</v>
+      </c>
+      <c r="E206" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="str">
+        <v>0x9f65AE97F174c6849297dF848651C520cC145A69</v>
+      </c>
+      <c r="B207" t="str">
+        <v>1,527.44</v>
+      </c>
+      <c r="C207" t="str">
+        <v>1,527.44</v>
+      </c>
+      <c r="D207" t="str">
+        <v>0</v>
+      </c>
+      <c r="E207" t="str">
+        <v>1,315.42</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="str">
+        <v>0xa8CE35A87d51EaC37675c1Cf7C5d6435a3b2079A</v>
+      </c>
+      <c r="B208" t="str">
+        <v>2,813.1</v>
+      </c>
+      <c r="C208" t="str">
+        <v>2,813.1</v>
+      </c>
+      <c r="D208" t="str">
+        <v>0</v>
+      </c>
+      <c r="E208" t="str">
+        <v>2,422.61</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="str">
+        <v>0x46d47D232d27bdF83FEA707ffd9Ce3e175B2D1dE</v>
+      </c>
+      <c r="B209" t="str">
+        <v>1,161.18</v>
+      </c>
+      <c r="C209" t="str">
+        <v>1,161.18</v>
+      </c>
+      <c r="D209" t="str">
+        <v>0</v>
+      </c>
+      <c r="E209" t="str">
+        <v>1,000</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="str">
+        <v>0xb4903c3b44dA26bf38cD923C64c6Cdad18ED280E</v>
+      </c>
+      <c r="B210" t="str">
+        <v>1,910.1</v>
+      </c>
+      <c r="C210" t="str">
+        <v>1,910.1</v>
+      </c>
+      <c r="D210" t="str">
+        <v>1,644.96</v>
+      </c>
+      <c r="E210" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="str">
+        <v>0x9c6E23aC65D33b747B8c56C04db77d836c41Faf5</v>
+      </c>
+      <c r="B211" t="str">
+        <v>3,407.24</v>
+      </c>
+      <c r="C211" t="str">
+        <v>3,407.24</v>
+      </c>
+      <c r="D211" t="str">
+        <v>0</v>
+      </c>
+      <c r="E211" t="str">
+        <v>2,934.28</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="str">
+        <v>0xa5086DeBa52099aDAe5c7f70b56ea494AACdfCa1</v>
+      </c>
+      <c r="B212" t="str">
+        <v>472.33</v>
+      </c>
+      <c r="C212" t="str">
+        <v>472.33</v>
+      </c>
+      <c r="D212" t="str">
+        <v>0</v>
+      </c>
+      <c r="E212" t="str">
+        <v>406.77</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="str">
+        <v>0x60E7Ff2154093f10d619e1ed30EDd11e8f1DDcAc</v>
+      </c>
+      <c r="B213" t="str">
+        <v>58.05</v>
+      </c>
+      <c r="C213" t="str">
+        <v>58.05</v>
+      </c>
+      <c r="D213" t="str">
+        <v>0</v>
+      </c>
+      <c r="E213" t="str">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="str">
+        <v>0xa235aF3C12D4A0b91EB6Fd836da45464141a21e8</v>
+      </c>
+      <c r="B214" t="str">
+        <v>216.03</v>
+      </c>
+      <c r="C214" t="str">
+        <v>216.03</v>
+      </c>
+      <c r="D214" t="str">
+        <v>0</v>
+      </c>
+      <c r="E214" t="str">
+        <v>186.05</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="str">
+        <v>0xf74f5cF53A6746b1eddD9C7ea8Ab7447797c3D74</v>
+      </c>
+      <c r="B215" t="str">
+        <v>6,538.66</v>
+      </c>
+      <c r="C215" t="str">
+        <v>6,538.66</v>
+      </c>
+      <c r="D215" t="str">
+        <v>0</v>
+      </c>
+      <c r="E215" t="str">
+        <v>5,631.02</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="str">
+        <v>0x36413818a988749f40de4877B51f782126282a89</v>
+      </c>
+      <c r="B216" t="str">
+        <v>1,175.19</v>
+      </c>
+      <c r="C216" t="str">
+        <v>1,175.19</v>
+      </c>
+      <c r="D216" t="str">
+        <v>1,012.06</v>
+      </c>
+      <c r="E216" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="str">
+        <v>0x48682644c1e8529338e46e7DdabA4383C1fceBb1</v>
+      </c>
+      <c r="B217" t="str">
+        <v>2,128.64</v>
+      </c>
+      <c r="C217" t="str">
+        <v>2,128.64</v>
+      </c>
+      <c r="D217" t="str">
+        <v>0</v>
+      </c>
+      <c r="E217" t="str">
+        <v>1,833.16</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="str">
+        <v>0x9B275D3580D7db9613e14308C978e27134365828</v>
+      </c>
+      <c r="B218" t="str">
+        <v>410.52</v>
+      </c>
+      <c r="C218" t="str">
+        <v>410.52</v>
+      </c>
+      <c r="D218" t="str">
+        <v>353.54</v>
+      </c>
+      <c r="E218" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="str">
+        <v>0xf0eeE0837e8F4feaC444412991f7005B8dFFa305</v>
+      </c>
+      <c r="B219" t="str">
+        <v>270.81</v>
+      </c>
+      <c r="C219" t="str">
+        <v>270.81</v>
+      </c>
+      <c r="D219" t="str">
+        <v>0</v>
+      </c>
+      <c r="E219" t="str">
+        <v>233.22</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="str">
+        <v>0x3f80b42ae4B6a8701329682B5C66a2780917E5D0</v>
+      </c>
+      <c r="B220" t="str">
+        <v>32.95</v>
+      </c>
+      <c r="C220" t="str">
+        <v>32.95</v>
+      </c>
+      <c r="D220" t="str">
+        <v>0</v>
+      </c>
+      <c r="E220" t="str">
+        <v>28.38</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="str">
+        <v>0x041BbF8dAEE68Bc5D306B7775b8299b0026416b3</v>
+      </c>
+      <c r="B221" t="str">
+        <v>205.06</v>
+      </c>
+      <c r="C221" t="str">
+        <v>205.06</v>
+      </c>
+      <c r="D221" t="str">
+        <v>176.6</v>
+      </c>
+      <c r="E221" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="str">
+        <v>0x260250876501b886EB540553d1f5306FAce6E393</v>
+      </c>
+      <c r="B222" t="str">
+        <v>136.41</v>
+      </c>
+      <c r="C222" t="str">
+        <v>136.41</v>
+      </c>
+      <c r="D222" t="str">
+        <v>117.48</v>
+      </c>
+      <c r="E222" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="str">
+        <v>0x75f87A0070d3710DA45A39D9d8D4bc9435d6287b</v>
+      </c>
+      <c r="B223" t="str">
+        <v>54.56</v>
+      </c>
+      <c r="C223" t="str">
+        <v>54.56</v>
+      </c>
+      <c r="D223" t="str">
+        <v>46.99</v>
+      </c>
+      <c r="E223" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="str">
+        <v>0x9fF7d51Cf6a3A12F2Cdd36035827037a35A4B139</v>
+      </c>
+      <c r="B224" t="str">
+        <v>17.58</v>
+      </c>
+      <c r="C224" t="str">
+        <v>17.58</v>
+      </c>
+      <c r="D224" t="str">
+        <v>0</v>
+      </c>
+      <c r="E224" t="str">
+        <v>15.14</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="str">
+        <v>0xdaf24dd4c9c7888b4f31937f99A869721E1E276c</v>
+      </c>
+      <c r="B225" t="str">
+        <v>1,102.89</v>
+      </c>
+      <c r="C225" t="str">
+        <v>1,102.89</v>
+      </c>
+      <c r="D225" t="str">
+        <v>0</v>
+      </c>
+      <c r="E225" t="str">
+        <v>949.8</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="str">
+        <v>0x4279DFA3c1fE5c16337f173f13D3BCBAA508a4C0</v>
+      </c>
+      <c r="B226" t="str">
+        <v>11.14</v>
+      </c>
+      <c r="C226" t="str">
+        <v>11.14</v>
+      </c>
+      <c r="D226" t="str">
+        <v>9.6</v>
+      </c>
+      <c r="E226" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="str">
+        <v>Total</v>
+      </c>
+      <c r="B227" t="str">
+        <v>2,859,070.7</v>
+      </c>
+      <c r="C227" t="str">
+        <v>3,205,127.05</v>
+      </c>
+      <c r="D227" t="str">
+        <v>1,244,153.33</v>
+      </c>
+      <c r="E227" t="str">
+        <v>1,516,063.72</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:E227"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E1000"/>
@@ -43735,13 +47616,6 @@
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
-  <cols>
-    <col min="1" max="1" width="20.83203125" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" customWidth="1"/>
-    <col min="5" max="5" width="15.83203125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">

</xml_diff>

<commit_message>
publish period 19 rewards
</commit_message>
<xml_diff>
--- a/staker_incentives.xlsx
+++ b/staker_incentives.xlsx
@@ -22,6 +22,7 @@
     <sheet name="Blocks 72615455 - 72898666" sheetId="17" r:id="rId17"/>
     <sheet name="Blocks 72898667 - 73182217" sheetId="18" r:id="rId18"/>
     <sheet name="Blocks 73182218 - 73465198" sheetId="19" r:id="rId19"/>
+    <sheet name="Blocks 73465199 - 73749236" sheetId="20" r:id="rId20"/>
   </sheets>
 </workbook>
 </file>
@@ -41359,13 +41360,6 @@
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
-  <cols>
-    <col min="1" max="1" width="20.83203125" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" customWidth="1"/>
-    <col min="5" max="5" width="15.83203125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
@@ -50874,6 +50868,3410 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E199"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" width="20.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Staker Address</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Reward (ERC20 TEL)</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Uncapped Reward (ERC20 TEL)</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Staker Fees</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Referee Fees</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>0x9195C770DCe41eC211353afD92c8a0f0b28fB011</v>
+      </c>
+      <c r="B2" t="str">
+        <v>627,379.96</v>
+      </c>
+      <c r="C2" t="str">
+        <v>627,379.96</v>
+      </c>
+      <c r="D2" t="str">
+        <v>648.87</v>
+      </c>
+      <c r="E2" t="str">
+        <v>655,048.68</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>0xAD5c21611Ea4790991c40BFD8e0888e012D7162E</v>
+      </c>
+      <c r="B3" t="str">
+        <v>3,621.77</v>
+      </c>
+      <c r="C3" t="str">
+        <v>3,621.77</v>
+      </c>
+      <c r="D3" t="str">
+        <v>3,785.25</v>
+      </c>
+      <c r="E3" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>0x30eE4B629Abe95d3383e4522dC3bCE84f2D28554</v>
+      </c>
+      <c r="B4" t="str">
+        <v>181.97</v>
+      </c>
+      <c r="C4" t="str">
+        <v>181.97</v>
+      </c>
+      <c r="D4" t="str">
+        <v>190.19</v>
+      </c>
+      <c r="E4" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>0x033047D46C9dD342b21274a0f328DD04c3ABa9b7</v>
+      </c>
+      <c r="B5" t="str">
+        <v>12,918.88</v>
+      </c>
+      <c r="C5" t="str">
+        <v>12,918.88</v>
+      </c>
+      <c r="D5" t="str">
+        <v>660.99</v>
+      </c>
+      <c r="E5" t="str">
+        <v>12,841</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>0xfC433E52b109b00c9e9f9532Da4a1B94a873A3a8</v>
+      </c>
+      <c r="B6" t="str">
+        <v>632.44</v>
+      </c>
+      <c r="C6" t="str">
+        <v>632.44</v>
+      </c>
+      <c r="D6" t="str">
+        <v>0</v>
+      </c>
+      <c r="E6" t="str">
+        <v>660.99</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>0x82983a034CD8811b62fbdEcDEb300b46947fCC45</v>
+      </c>
+      <c r="B7" t="str">
+        <v>403.79</v>
+      </c>
+      <c r="C7" t="str">
+        <v>403.79</v>
+      </c>
+      <c r="D7" t="str">
+        <v>422.02</v>
+      </c>
+      <c r="E7" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>0x24EC4345706a30747bA16dCA3e9751B73b72C78a</v>
+      </c>
+      <c r="B8" t="str">
+        <v>2,076.49</v>
+      </c>
+      <c r="C8" t="str">
+        <v>2,076.49</v>
+      </c>
+      <c r="D8" t="str">
+        <v>2,170.22</v>
+      </c>
+      <c r="E8" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>0x886049Df7a8010a7e3c21A32b74e41402986ae37</v>
+      </c>
+      <c r="B9" t="str">
+        <v>147.24</v>
+      </c>
+      <c r="C9" t="str">
+        <v>147.24</v>
+      </c>
+      <c r="D9" t="str">
+        <v>153.89</v>
+      </c>
+      <c r="E9" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>0xEE9688E9CBa96c56ad91c9899507580415a47795</v>
+      </c>
+      <c r="B10" t="str">
+        <v>1,538.16</v>
+      </c>
+      <c r="C10" t="str">
+        <v>1,538.16</v>
+      </c>
+      <c r="D10" t="str">
+        <v>1,607.59</v>
+      </c>
+      <c r="E10" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>0x1f21AdB9fe6A088B4F5411eEd543BEA954A15F56</v>
+      </c>
+      <c r="B11" t="str">
+        <v>1,538.16</v>
+      </c>
+      <c r="C11" t="str">
+        <v>1,538.16</v>
+      </c>
+      <c r="D11" t="str">
+        <v>0</v>
+      </c>
+      <c r="E11" t="str">
+        <v>1,607.59</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>0xd685199C3Bfc7DD24d7E4A6bfD17dCa2bBF2F57d</v>
+      </c>
+      <c r="B12" t="str">
+        <v>6,955.69</v>
+      </c>
+      <c r="C12" t="str">
+        <v>6,955.69</v>
+      </c>
+      <c r="D12" t="str">
+        <v>148.49</v>
+      </c>
+      <c r="E12" t="str">
+        <v>7,121.16</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>0x20944C8A17cfa6cb96556116037e3aEeB506a0b0</v>
+      </c>
+      <c r="B13" t="str">
+        <v>6,633.06</v>
+      </c>
+      <c r="C13" t="str">
+        <v>6,633.06</v>
+      </c>
+      <c r="D13" t="str">
+        <v>6,807.46</v>
+      </c>
+      <c r="E13" t="str">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>0x5fBC9150Df7FDf49Cd4C6BF2a2649259Ad3Ca0Bc</v>
+      </c>
+      <c r="B14" t="str">
+        <v>3.11</v>
+      </c>
+      <c r="C14" t="str">
+        <v>3.11</v>
+      </c>
+      <c r="D14" t="str">
+        <v>3.26</v>
+      </c>
+      <c r="E14" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>0x37cB7396A901E73B0f490F98E708933684263456</v>
+      </c>
+      <c r="B15" t="str">
+        <v>5,428.45</v>
+      </c>
+      <c r="C15" t="str">
+        <v>5,428.45</v>
+      </c>
+      <c r="D15" t="str">
+        <v>5,673.47</v>
+      </c>
+      <c r="E15" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>0xF68784ce085df3b5d3493A29F3Be8Bc971c3C87A</v>
+      </c>
+      <c r="B16" t="str">
+        <v>27,709.2</v>
+      </c>
+      <c r="C16" t="str">
+        <v>27,709.2</v>
+      </c>
+      <c r="D16" t="str">
+        <v>28,959.89</v>
+      </c>
+      <c r="E16" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>0xdC7A5B88f099B3385a9a714e679B0a511E9071bf</v>
+      </c>
+      <c r="B17" t="str">
+        <v>28.31</v>
+      </c>
+      <c r="C17" t="str">
+        <v>28.31</v>
+      </c>
+      <c r="D17" t="str">
+        <v>29.59</v>
+      </c>
+      <c r="E17" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>0xe2e039dD3206870FE6Ad4B88DDf74730c355B2e5</v>
+      </c>
+      <c r="B18" t="str">
+        <v>406.1</v>
+      </c>
+      <c r="C18" t="str">
+        <v>406.1</v>
+      </c>
+      <c r="D18" t="str">
+        <v>0</v>
+      </c>
+      <c r="E18" t="str">
+        <v>424.43</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>0x2Cb57c4f35be11e63395E6b9920c5Ac2754d417E</v>
+      </c>
+      <c r="B19" t="str">
+        <v>64.34</v>
+      </c>
+      <c r="C19" t="str">
+        <v>64.34</v>
+      </c>
+      <c r="D19" t="str">
+        <v>67.25</v>
+      </c>
+      <c r="E19" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>0xb51D1dC8c04786ec6B47570619bBa8f6D0B7bcbc</v>
+      </c>
+      <c r="B20" t="str">
+        <v>1,892.57</v>
+      </c>
+      <c r="C20" t="str">
+        <v>1,892.57</v>
+      </c>
+      <c r="D20" t="str">
+        <v>1,978</v>
+      </c>
+      <c r="E20" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>0x721D683cBd00c78Eb2676fBA03e8c03FDF07f5dC</v>
+      </c>
+      <c r="B21" t="str">
+        <v>1,909.1</v>
+      </c>
+      <c r="C21" t="str">
+        <v>1,909.1</v>
+      </c>
+      <c r="D21" t="str">
+        <v>1,128.37</v>
+      </c>
+      <c r="E21" t="str">
+        <v>866.91</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>0x1174EaB7a553690130EC76fa1E950df457b930a5</v>
+      </c>
+      <c r="B22" t="str">
+        <v>234,788.88</v>
+      </c>
+      <c r="C22" t="str">
+        <v>234,788.88</v>
+      </c>
+      <c r="D22" t="str">
+        <v>245,386.38</v>
+      </c>
+      <c r="E22" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>0x5eE2FC3425b4e3C908C6d6BcaDf3dce444BE8617</v>
+      </c>
+      <c r="B23" t="str">
+        <v>72,429.1</v>
+      </c>
+      <c r="C23" t="str">
+        <v>72,429.1</v>
+      </c>
+      <c r="D23" t="str">
+        <v>75,698.28</v>
+      </c>
+      <c r="E23" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>0xF336C5e15E672F6606CA8CDe3D4FaF95fE1C63Bb</v>
+      </c>
+      <c r="B24" t="str">
+        <v>93,505.24</v>
+      </c>
+      <c r="C24" t="str">
+        <v>93,505.24</v>
+      </c>
+      <c r="D24" t="str">
+        <v>92,453.4</v>
+      </c>
+      <c r="E24" t="str">
+        <v>5,272.32</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>0xB51e05e0F9b9a22D714fC181aBA3a43d79d728bB</v>
+      </c>
+      <c r="B25" t="str">
+        <v>132.52</v>
+      </c>
+      <c r="C25" t="str">
+        <v>132.52</v>
+      </c>
+      <c r="D25" t="str">
+        <v>138.51</v>
+      </c>
+      <c r="E25" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>0x426d787930A93314048488c4D10946FCeD265Cc7</v>
+      </c>
+      <c r="B26" t="str">
+        <v>24,038.93</v>
+      </c>
+      <c r="C26" t="str">
+        <v>24,038.93</v>
+      </c>
+      <c r="D26" t="str">
+        <v>25,107.86</v>
+      </c>
+      <c r="E26" t="str">
+        <v>16.1</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>0xa36AA3562dA79a0a0Fbbd7a210131f3d705537F2</v>
+      </c>
+      <c r="B27" t="str">
+        <v>131,015.5</v>
+      </c>
+      <c r="C27" t="str">
+        <v>131,015.5</v>
+      </c>
+      <c r="D27" t="str">
+        <v>136,929.05</v>
+      </c>
+      <c r="E27" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>0x76cf73e99947E31e951416E3859F3cFB07f9Fd3B</v>
+      </c>
+      <c r="B28" t="str">
+        <v>0</v>
+      </c>
+      <c r="C28" t="str">
+        <v>54.09</v>
+      </c>
+      <c r="D28" t="str">
+        <v>56.54</v>
+      </c>
+      <c r="E28" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>0x436aCB00107faBb69b486e2C7F4654bB37b02c41</v>
+      </c>
+      <c r="B29" t="str">
+        <v>12,153.9</v>
+      </c>
+      <c r="C29" t="str">
+        <v>12,153.9</v>
+      </c>
+      <c r="D29" t="str">
+        <v>12,702.49</v>
+      </c>
+      <c r="E29" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>0x11C3498d0D70BBfCdAa8dA275d7dDEb7BF977137</v>
+      </c>
+      <c r="B30" t="str">
+        <v>1,077.86</v>
+      </c>
+      <c r="C30" t="str">
+        <v>1,077.86</v>
+      </c>
+      <c r="D30" t="str">
+        <v>626.13</v>
+      </c>
+      <c r="E30" t="str">
+        <v>500.39</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>0x27dF802924227b28Ad0Bec076Bd7f1D223441bF5</v>
+      </c>
+      <c r="B31" t="str">
+        <v>1,077.86</v>
+      </c>
+      <c r="C31" t="str">
+        <v>1,077.86</v>
+      </c>
+      <c r="D31" t="str">
+        <v>500.39</v>
+      </c>
+      <c r="E31" t="str">
+        <v>626.13</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>0x9f39dD592Fc405A08eB7730D9FA4CF2e37cB5862</v>
+      </c>
+      <c r="B32" t="str">
+        <v>10.7</v>
+      </c>
+      <c r="C32" t="str">
+        <v>10.7</v>
+      </c>
+      <c r="D32" t="str">
+        <v>11.19</v>
+      </c>
+      <c r="E32" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>0x77940861e000BfC8A8f67440ad21656B9e7dbA04</v>
+      </c>
+      <c r="B33" t="str">
+        <v>3,652.3</v>
+      </c>
+      <c r="C33" t="str">
+        <v>3,652.3</v>
+      </c>
+      <c r="D33" t="str">
+        <v>3,817.16</v>
+      </c>
+      <c r="E33" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>0x8C96f8c87Ea3015953f18852eBaB2c3D2139d73b</v>
+      </c>
+      <c r="B34" t="str">
+        <v>119.5</v>
+      </c>
+      <c r="C34" t="str">
+        <v>119.5</v>
+      </c>
+      <c r="D34" t="str">
+        <v>124.9</v>
+      </c>
+      <c r="E34" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>0x2731b9BC4c6AC6287996741A5A87D6E51D18B2EB</v>
+      </c>
+      <c r="B35" t="str">
+        <v>1,235.36</v>
+      </c>
+      <c r="C35" t="str">
+        <v>1,235.36</v>
+      </c>
+      <c r="D35" t="str">
+        <v>1,291.12</v>
+      </c>
+      <c r="E35" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>0xA0De99feED77A3f228F9e6Bfe3B8333c2fc1D0f9</v>
+      </c>
+      <c r="B36" t="str">
+        <v>62.01</v>
+      </c>
+      <c r="C36" t="str">
+        <v>62.01</v>
+      </c>
+      <c r="D36" t="str">
+        <v>0</v>
+      </c>
+      <c r="E36" t="str">
+        <v>64.81</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>0x096454fa85d4bD21CBB9134966c417f2e40C288C</v>
+      </c>
+      <c r="B37" t="str">
+        <v>368.14</v>
+      </c>
+      <c r="C37" t="str">
+        <v>368.14</v>
+      </c>
+      <c r="D37" t="str">
+        <v>384.76</v>
+      </c>
+      <c r="E37" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>0x1DA42d0A3108af9D1f8eB3bFd80bD26FBE2d911d</v>
+      </c>
+      <c r="B38" t="str">
+        <v>148,089.2</v>
+      </c>
+      <c r="C38" t="str">
+        <v>148,089.2</v>
+      </c>
+      <c r="D38" t="str">
+        <v>154,773.4</v>
+      </c>
+      <c r="E38" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>0x8f26838FF9A288727088F10968Ea663A424509F4</v>
+      </c>
+      <c r="B39" t="str">
+        <v>148,089.2</v>
+      </c>
+      <c r="C39" t="str">
+        <v>148,089.2</v>
+      </c>
+      <c r="D39" t="str">
+        <v>0</v>
+      </c>
+      <c r="E39" t="str">
+        <v>154,773.4</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>0x33dE4E1bE024FeD529b5af917955DBa1951FfE26</v>
+      </c>
+      <c r="B40" t="str">
+        <v>28,427.29</v>
+      </c>
+      <c r="C40" t="str">
+        <v>28,427.29</v>
+      </c>
+      <c r="D40" t="str">
+        <v>29,710.4</v>
+      </c>
+      <c r="E40" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>0x6468eF36F4375A0bB4f18eEB3aA114C8D69066eF</v>
+      </c>
+      <c r="B41" t="str">
+        <v>1,285.62</v>
+      </c>
+      <c r="C41" t="str">
+        <v>1,285.62</v>
+      </c>
+      <c r="D41" t="str">
+        <v>1,317.45</v>
+      </c>
+      <c r="E41" t="str">
+        <v>26.2</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>0xEED1ea5dFDB1D4e9c9Bc0826fbCA66f5f5660886</v>
+      </c>
+      <c r="B42" t="str">
+        <v>262.96</v>
+      </c>
+      <c r="C42" t="str">
+        <v>262.96</v>
+      </c>
+      <c r="D42" t="str">
+        <v>274.83</v>
+      </c>
+      <c r="E42" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>0x04d9f35C7c292ca2c75C498563b48123C0662e19</v>
+      </c>
+      <c r="B43" t="str">
+        <v>71,371.85</v>
+      </c>
+      <c r="C43" t="str">
+        <v>71,371.85</v>
+      </c>
+      <c r="D43" t="str">
+        <v>74,593.31</v>
+      </c>
+      <c r="E43" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>0xd63c4fE2E52948079b40d0eFd5FBa8a5F54aB32b</v>
+      </c>
+      <c r="B44" t="str">
+        <v>5,120.59</v>
+      </c>
+      <c r="C44" t="str">
+        <v>5,120.59</v>
+      </c>
+      <c r="D44" t="str">
+        <v>5,351.72</v>
+      </c>
+      <c r="E44" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>0x01Bf02ECf2aa5f2E824a64Fba6A0DC3Ee46D775B</v>
+      </c>
+      <c r="B45" t="str">
+        <v>256,910.89</v>
+      </c>
+      <c r="C45" t="str">
+        <v>256,910.89</v>
+      </c>
+      <c r="D45" t="str">
+        <v>268,506.89</v>
+      </c>
+      <c r="E45" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>0xA7258aeA0F44A7fe4a4933a1434e2fc8217891C0</v>
+      </c>
+      <c r="B46" t="str">
+        <v>256,910.89</v>
+      </c>
+      <c r="C46" t="str">
+        <v>256,910.89</v>
+      </c>
+      <c r="D46" t="str">
+        <v>0</v>
+      </c>
+      <c r="E46" t="str">
+        <v>268,506.89</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>0xB6324b4410036C4C307255dE5E44AE8D6D4474CA</v>
+      </c>
+      <c r="B47" t="str">
+        <v>124.39</v>
+      </c>
+      <c r="C47" t="str">
+        <v>124.39</v>
+      </c>
+      <c r="D47" t="str">
+        <v>130.01</v>
+      </c>
+      <c r="E47" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>0x3ce8daA3F14F9ED56F0dbfe04daf6A6EE5aA7187</v>
+      </c>
+      <c r="B48" t="str">
+        <v>81.68</v>
+      </c>
+      <c r="C48" t="str">
+        <v>81.68</v>
+      </c>
+      <c r="D48" t="str">
+        <v>85.37</v>
+      </c>
+      <c r="E48" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>0x8364044ee8062F0F6C9835f7dfC26da4CE433BB8</v>
+      </c>
+      <c r="B49" t="str">
+        <v>310.36</v>
+      </c>
+      <c r="C49" t="str">
+        <v>310.36</v>
+      </c>
+      <c r="D49" t="str">
+        <v>0</v>
+      </c>
+      <c r="E49" t="str">
+        <v>324.37</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>0x425F2F1287045bC9d04C0f933E7FdEdA4A2e5765</v>
+      </c>
+      <c r="B50" t="str">
+        <v>916.65</v>
+      </c>
+      <c r="C50" t="str">
+        <v>916.65</v>
+      </c>
+      <c r="D50" t="str">
+        <v>958.03</v>
+      </c>
+      <c r="E50" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>0xc790596C713f906Bc24beEC6da941AC5DDD92800</v>
+      </c>
+      <c r="B51" t="str">
+        <v>210.46</v>
+      </c>
+      <c r="C51" t="str">
+        <v>210.46</v>
+      </c>
+      <c r="D51" t="str">
+        <v>0</v>
+      </c>
+      <c r="E51" t="str">
+        <v>219.96</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>0x8087C1A1Be0B5c51B35DdC49aa1C65d0C3B24038</v>
+      </c>
+      <c r="B52" t="str">
+        <v>1.4</v>
+      </c>
+      <c r="C52" t="str">
+        <v>1.4</v>
+      </c>
+      <c r="D52" t="str">
+        <v>1.47</v>
+      </c>
+      <c r="E52" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>0x880cd618B4cA66bBb8862558954d8473d7b0C867</v>
+      </c>
+      <c r="B53" t="str">
+        <v>257.95</v>
+      </c>
+      <c r="C53" t="str">
+        <v>257.95</v>
+      </c>
+      <c r="D53" t="str">
+        <v>269.6</v>
+      </c>
+      <c r="E53" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>0x7D350424B120fA3C454484fe2DEE04fA0315b336</v>
+      </c>
+      <c r="B54" t="str">
+        <v>40.15</v>
+      </c>
+      <c r="C54" t="str">
+        <v>40.15</v>
+      </c>
+      <c r="D54" t="str">
+        <v>41.97</v>
+      </c>
+      <c r="E54" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>0xC8a3B31C5d3Ba95Eec7377887a445BE34AfEE3BD</v>
+      </c>
+      <c r="B55" t="str">
+        <v>721.24</v>
+      </c>
+      <c r="C55" t="str">
+        <v>721.24</v>
+      </c>
+      <c r="D55" t="str">
+        <v>753.8</v>
+      </c>
+      <c r="E55" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>0xcFf9490e51524c67555C6f6896bB5ccF09751F06</v>
+      </c>
+      <c r="B56" t="str">
+        <v>5,044.62</v>
+      </c>
+      <c r="C56" t="str">
+        <v>5,044.62</v>
+      </c>
+      <c r="D56" t="str">
+        <v>5,272.32</v>
+      </c>
+      <c r="E56" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>0xD602189e5A2C76fb8Cd054c72e984b32997538d2</v>
+      </c>
+      <c r="B57" t="str">
+        <v>588.03</v>
+      </c>
+      <c r="C57" t="str">
+        <v>588.03</v>
+      </c>
+      <c r="D57" t="str">
+        <v>614.58</v>
+      </c>
+      <c r="E57" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>0x8f437d47c7723C7AB5ab896D59549D547181BecB</v>
+      </c>
+      <c r="B58" t="str">
+        <v>42.9</v>
+      </c>
+      <c r="C58" t="str">
+        <v>42.9</v>
+      </c>
+      <c r="D58" t="str">
+        <v>44.84</v>
+      </c>
+      <c r="E58" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>0xd3e2D6e79E0B7511813641B4FDb26E6EB6dFa66f</v>
+      </c>
+      <c r="B59" t="str">
+        <v>160.49</v>
+      </c>
+      <c r="C59" t="str">
+        <v>160.49</v>
+      </c>
+      <c r="D59" t="str">
+        <v>167.74</v>
+      </c>
+      <c r="E59" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>0x375bE33B63Ad8204eb4FB2CaCa325126d1eC6f19</v>
+      </c>
+      <c r="B60" t="str">
+        <v>3.76</v>
+      </c>
+      <c r="C60" t="str">
+        <v>3.76</v>
+      </c>
+      <c r="D60" t="str">
+        <v>3.93</v>
+      </c>
+      <c r="E60" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>0xDe113Cfea35386619bB00AD4B84130b22222c742</v>
+      </c>
+      <c r="B61" t="str">
+        <v>117.15</v>
+      </c>
+      <c r="C61" t="str">
+        <v>117.15</v>
+      </c>
+      <c r="D61" t="str">
+        <v>122.44</v>
+      </c>
+      <c r="E61" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>0x392377C45797a725667bd47C315462cF82550BcC</v>
+      </c>
+      <c r="B62" t="str">
+        <v>979.99</v>
+      </c>
+      <c r="C62" t="str">
+        <v>979.99</v>
+      </c>
+      <c r="D62" t="str">
+        <v>1,024.23</v>
+      </c>
+      <c r="E62" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>0xE02A23F9DA0971f65a548e3Da4F247a5ed6Fc82d</v>
+      </c>
+      <c r="B63" t="str">
+        <v>201.82</v>
+      </c>
+      <c r="C63" t="str">
+        <v>201.82</v>
+      </c>
+      <c r="D63" t="str">
+        <v>210.93</v>
+      </c>
+      <c r="E63" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>0xe05DDFB83A8b66Df42f06BfB5517Fb5d6857a8ce</v>
+      </c>
+      <c r="B64" t="str">
+        <v>21,741.6</v>
+      </c>
+      <c r="C64" t="str">
+        <v>21,741.6</v>
+      </c>
+      <c r="D64" t="str">
+        <v>1,594.79</v>
+      </c>
+      <c r="E64" t="str">
+        <v>21,128.15</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>0x4994A7059A2921398780818c203F83613A9Bf743</v>
+      </c>
+      <c r="B65" t="str">
+        <v>41,328.75</v>
+      </c>
+      <c r="C65" t="str">
+        <v>41,328.75</v>
+      </c>
+      <c r="D65" t="str">
+        <v>5,000</v>
+      </c>
+      <c r="E65" t="str">
+        <v>38,194.18</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v>0xDd7e4E36199cC322cb61758F13708b3bC95A688c</v>
+      </c>
+      <c r="B66" t="str">
+        <v>835.55</v>
+      </c>
+      <c r="C66" t="str">
+        <v>835.55</v>
+      </c>
+      <c r="D66" t="str">
+        <v>873.27</v>
+      </c>
+      <c r="E66" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="str">
+        <v>0xdC2F100fCabBa1660d8714E2F15664488Ab4F25D</v>
+      </c>
+      <c r="B67" t="str">
+        <v>94.6</v>
+      </c>
+      <c r="C67" t="str">
+        <v>94.6</v>
+      </c>
+      <c r="D67" t="str">
+        <v>98.88</v>
+      </c>
+      <c r="E67" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="str">
+        <v>0xf90518CBcd4ef086891cb22C87bd4F80B61a7081</v>
+      </c>
+      <c r="B68" t="str">
+        <v>367.65</v>
+      </c>
+      <c r="C68" t="str">
+        <v>367.65</v>
+      </c>
+      <c r="D68" t="str">
+        <v>0</v>
+      </c>
+      <c r="E68" t="str">
+        <v>384.25</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="str">
+        <v>0x746F83FF7eAdA9d0fB03DbAbcAF2600ee513DCDB</v>
+      </c>
+      <c r="B69" t="str">
+        <v>4,888.01</v>
+      </c>
+      <c r="C69" t="str">
+        <v>4,888.01</v>
+      </c>
+      <c r="D69" t="str">
+        <v>0</v>
+      </c>
+      <c r="E69" t="str">
+        <v>5,108.64</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="str">
+        <v>0x61cD23Cf91d9B6BBb4bFF28c6AD7B667C7EC6367</v>
+      </c>
+      <c r="B70" t="str">
+        <v>0</v>
+      </c>
+      <c r="C70" t="str">
+        <v>1,841.86</v>
+      </c>
+      <c r="D70" t="str">
+        <v>1,925</v>
+      </c>
+      <c r="E70" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v>0x1D712193A96B4d9D4eC32108cfcde704AC9CCC9C</v>
+      </c>
+      <c r="B71" t="str">
+        <v>246.22</v>
+      </c>
+      <c r="C71" t="str">
+        <v>246.22</v>
+      </c>
+      <c r="D71" t="str">
+        <v>257.34</v>
+      </c>
+      <c r="E71" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>0xBb3123adaa39aA9b0Bf8c0374eab50353F479c97</v>
+      </c>
+      <c r="B72" t="str">
+        <v>1,004.42</v>
+      </c>
+      <c r="C72" t="str">
+        <v>1,004.42</v>
+      </c>
+      <c r="D72" t="str">
+        <v>1,049.76</v>
+      </c>
+      <c r="E72" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>0xF1D275F804a6b3d3f75B7C08150178836E56dE8B</v>
+      </c>
+      <c r="B73" t="str">
+        <v>1,004.42</v>
+      </c>
+      <c r="C73" t="str">
+        <v>1,004.42</v>
+      </c>
+      <c r="D73" t="str">
+        <v>0</v>
+      </c>
+      <c r="E73" t="str">
+        <v>1,049.76</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>0xBC3f8985F75c8628C3a6687EB91e21f50C961a5D</v>
+      </c>
+      <c r="B74" t="str">
+        <v>116.75</v>
+      </c>
+      <c r="C74" t="str">
+        <v>116.75</v>
+      </c>
+      <c r="D74" t="str">
+        <v>122.03</v>
+      </c>
+      <c r="E74" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>0xd19d505d3618A142E85bd1A2A8C0878cD2b1089d</v>
+      </c>
+      <c r="B75" t="str">
+        <v>1,312.77</v>
+      </c>
+      <c r="C75" t="str">
+        <v>1,312.77</v>
+      </c>
+      <c r="D75" t="str">
+        <v>0</v>
+      </c>
+      <c r="E75" t="str">
+        <v>1,372.03</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>0x0603709F92A47D5367Cc93f5b587A29fA286ADbB</v>
+      </c>
+      <c r="B76" t="str">
+        <v>3,864.72</v>
+      </c>
+      <c r="C76" t="str">
+        <v>3,864.72</v>
+      </c>
+      <c r="D76" t="str">
+        <v>0</v>
+      </c>
+      <c r="E76" t="str">
+        <v>4,039.16</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v>0x94B72396b6B40e19C2a04c28c8aE93dE08b12733</v>
+      </c>
+      <c r="B77" t="str">
+        <v>0</v>
+      </c>
+      <c r="C77" t="str">
+        <v>4,934.14</v>
+      </c>
+      <c r="D77" t="str">
+        <v>0</v>
+      </c>
+      <c r="E77" t="str">
+        <v>5,156.85</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="str">
+        <v>0xa6A4BE6499cfdd7E94Cd1BF5498533FdCbb6CE5d</v>
+      </c>
+      <c r="B78" t="str">
+        <v>61,735.76</v>
+      </c>
+      <c r="C78" t="str">
+        <v>61,735.76</v>
+      </c>
+      <c r="D78" t="str">
+        <v>62,182.53</v>
+      </c>
+      <c r="E78" t="str">
+        <v>2,339.76</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="str">
+        <v>0xcC333A0d55395f7cABD42793850D4ea5B32E1D78</v>
+      </c>
+      <c r="B79" t="str">
+        <v>59,497.05</v>
+      </c>
+      <c r="C79" t="str">
+        <v>59,497.05</v>
+      </c>
+      <c r="D79" t="str">
+        <v>0</v>
+      </c>
+      <c r="E79" t="str">
+        <v>62,182.53</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="str">
+        <v>0x231E89f21Da8d752262D42ad835B30D0Ee0aF8c5</v>
+      </c>
+      <c r="B80" t="str">
+        <v>246.43</v>
+      </c>
+      <c r="C80" t="str">
+        <v>246.43</v>
+      </c>
+      <c r="D80" t="str">
+        <v>0</v>
+      </c>
+      <c r="E80" t="str">
+        <v>257.56</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="str">
+        <v>0xf33639F5c9cDB8E242c3E20Fdaf98Ae389f0e399</v>
+      </c>
+      <c r="B81" t="str">
+        <v>29.9</v>
+      </c>
+      <c r="C81" t="str">
+        <v>29.9</v>
+      </c>
+      <c r="D81" t="str">
+        <v>31.25</v>
+      </c>
+      <c r="E81" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="str">
+        <v>0x0116c14c39b5a5ecD03193E56E975064b4a405D2</v>
+      </c>
+      <c r="B82" t="str">
+        <v>29.9</v>
+      </c>
+      <c r="C82" t="str">
+        <v>29.9</v>
+      </c>
+      <c r="D82" t="str">
+        <v>0</v>
+      </c>
+      <c r="E82" t="str">
+        <v>31.25</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="str">
+        <v>0x47502539673c93B2ACDC9059B36360f76D3548BB</v>
+      </c>
+      <c r="B83" t="str">
+        <v>9,229.33</v>
+      </c>
+      <c r="C83" t="str">
+        <v>9,229.33</v>
+      </c>
+      <c r="D83" t="str">
+        <v>219.96</v>
+      </c>
+      <c r="E83" t="str">
+        <v>9,425.95</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="str">
+        <v>0xbD73E24F927E9f1D9ce45B7e47f36711Dca35A88</v>
+      </c>
+      <c r="B84" t="str">
+        <v>13.11</v>
+      </c>
+      <c r="C84" t="str">
+        <v>13.11</v>
+      </c>
+      <c r="D84" t="str">
+        <v>0</v>
+      </c>
+      <c r="E84" t="str">
+        <v>13.71</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="str">
+        <v>0x0D9692C297c0C72dD94a8614141B4bF8A2398d3E</v>
+      </c>
+      <c r="B85" t="str">
+        <v>4,815.2</v>
+      </c>
+      <c r="C85" t="str">
+        <v>4,815.2</v>
+      </c>
+      <c r="D85" t="str">
+        <v>5,032.55</v>
+      </c>
+      <c r="E85" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="str">
+        <v>0x62Ff55e86d95A460a661929d6D125139bB7DCF7b</v>
+      </c>
+      <c r="B86" t="str">
+        <v>9,627.57</v>
+      </c>
+      <c r="C86" t="str">
+        <v>9,627.57</v>
+      </c>
+      <c r="D86" t="str">
+        <v>0</v>
+      </c>
+      <c r="E86" t="str">
+        <v>10,062.13</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="str">
+        <v>0xb9311fa41ABE8b7eb4c962113664749CED864748</v>
+      </c>
+      <c r="B87" t="str">
+        <v>4,812.36</v>
+      </c>
+      <c r="C87" t="str">
+        <v>4,812.36</v>
+      </c>
+      <c r="D87" t="str">
+        <v>5,029.58</v>
+      </c>
+      <c r="E87" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="str">
+        <v>0xcFffD6F1C52280f46A0f32212150CbCaF50bBfb9</v>
+      </c>
+      <c r="B88" t="str">
+        <v>959.85</v>
+      </c>
+      <c r="C88" t="str">
+        <v>959.85</v>
+      </c>
+      <c r="D88" t="str">
+        <v>1,003.18</v>
+      </c>
+      <c r="E88" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="str">
+        <v>0x44dDf2A9375EF552A77973588E3964b9BBBe8191</v>
+      </c>
+      <c r="B89" t="str">
+        <v>1,272.76</v>
+      </c>
+      <c r="C89" t="str">
+        <v>1,272.76</v>
+      </c>
+      <c r="D89" t="str">
+        <v>1,330.21</v>
+      </c>
+      <c r="E89" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="str">
+        <v>0x681ee9C08368ED5e30519f146cF3A27b24471Dc6</v>
+      </c>
+      <c r="B90" t="str">
+        <v>0</v>
+      </c>
+      <c r="C90" t="str">
+        <v>1,272.76</v>
+      </c>
+      <c r="D90" t="str">
+        <v>0</v>
+      </c>
+      <c r="E90" t="str">
+        <v>1,330.21</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="str">
+        <v>0xe5E0B4E52743E5A1E53162d38eAAF6DE05B9a4bF</v>
+      </c>
+      <c r="B91" t="str">
+        <v>481.67</v>
+      </c>
+      <c r="C91" t="str">
+        <v>481.67</v>
+      </c>
+      <c r="D91" t="str">
+        <v>503.42</v>
+      </c>
+      <c r="E91" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="str">
+        <v>0x7229aE5d9fa64DAe6C47d360023FfE683f0517F0</v>
+      </c>
+      <c r="B92" t="str">
+        <v>2,873.71</v>
+      </c>
+      <c r="C92" t="str">
+        <v>2,873.71</v>
+      </c>
+      <c r="D92" t="str">
+        <v>0</v>
+      </c>
+      <c r="E92" t="str">
+        <v>3,003.42</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="str">
+        <v>0xA53aFB483Fa417B9491C3a7AEAeDF463Ab687E29</v>
+      </c>
+      <c r="B93" t="str">
+        <v>23.53</v>
+      </c>
+      <c r="C93" t="str">
+        <v>23.53</v>
+      </c>
+      <c r="D93" t="str">
+        <v>24.6</v>
+      </c>
+      <c r="E93" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="str">
+        <v>0x126f38D7Dda782e2a33f2061556524C3aA9cE30B</v>
+      </c>
+      <c r="B94" t="str">
+        <v>23.53</v>
+      </c>
+      <c r="C94" t="str">
+        <v>23.53</v>
+      </c>
+      <c r="D94" t="str">
+        <v>0</v>
+      </c>
+      <c r="E94" t="str">
+        <v>24.6</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="str">
+        <v>0xCdDca3b68166cB76442B5D69cB6B800fD7fc67c0</v>
+      </c>
+      <c r="B95" t="str">
+        <v>353.47</v>
+      </c>
+      <c r="C95" t="str">
+        <v>353.47</v>
+      </c>
+      <c r="D95" t="str">
+        <v>0</v>
+      </c>
+      <c r="E95" t="str">
+        <v>369.43</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="str">
+        <v>0x0254704C23C4765496894a632ef28d6be4DCB259</v>
+      </c>
+      <c r="B96" t="str">
+        <v>0.83</v>
+      </c>
+      <c r="C96" t="str">
+        <v>0.83</v>
+      </c>
+      <c r="D96" t="str">
+        <v>0</v>
+      </c>
+      <c r="E96" t="str">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="str">
+        <v>0xF5515DFf13e55c0B219fB8B56BD18B2A8dC7bF33</v>
+      </c>
+      <c r="B97" t="str">
+        <v>184.33</v>
+      </c>
+      <c r="C97" t="str">
+        <v>184.33</v>
+      </c>
+      <c r="D97" t="str">
+        <v>0</v>
+      </c>
+      <c r="E97" t="str">
+        <v>192.66</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="str">
+        <v>0x4E2069d03340c94A9C79e31dd93D577d82C83b22</v>
+      </c>
+      <c r="B98" t="str">
+        <v>28.84</v>
+      </c>
+      <c r="C98" t="str">
+        <v>28.84</v>
+      </c>
+      <c r="D98" t="str">
+        <v>30.15</v>
+      </c>
+      <c r="E98" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="str">
+        <v>0xA6F3eb75fa915C7Bf8a6987710511070D97E2a75</v>
+      </c>
+      <c r="B99" t="str">
+        <v>389.27</v>
+      </c>
+      <c r="C99" t="str">
+        <v>389.27</v>
+      </c>
+      <c r="D99" t="str">
+        <v>406.85</v>
+      </c>
+      <c r="E99" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="str">
+        <v>0xE34bBD8d72B7Ffe5ad2e84CE93e3A07581De2e50</v>
+      </c>
+      <c r="B100" t="str">
+        <v>0</v>
+      </c>
+      <c r="C100" t="str">
+        <v>350.69</v>
+      </c>
+      <c r="D100" t="str">
+        <v>0</v>
+      </c>
+      <c r="E100" t="str">
+        <v>366.52</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="str">
+        <v>0x4CaFc8E23616346de04DE62174B1e615D8E80c70</v>
+      </c>
+      <c r="B101" t="str">
+        <v>3,179.53</v>
+      </c>
+      <c r="C101" t="str">
+        <v>3,179.53</v>
+      </c>
+      <c r="D101" t="str">
+        <v>0</v>
+      </c>
+      <c r="E101" t="str">
+        <v>3,323.05</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="str">
+        <v>0x88852100b52867c80eaa3b5eA0500F4bFB7E5899</v>
+      </c>
+      <c r="B102" t="str">
+        <v>2,387.41</v>
+      </c>
+      <c r="C102" t="str">
+        <v>2,387.41</v>
+      </c>
+      <c r="D102" t="str">
+        <v>0</v>
+      </c>
+      <c r="E102" t="str">
+        <v>2,495.17</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="str">
+        <v>0x753AA7A72763f8C3Dc7791cC938fAd954bc34842</v>
+      </c>
+      <c r="B103" t="str">
+        <v>582.12</v>
+      </c>
+      <c r="C103" t="str">
+        <v>582.12</v>
+      </c>
+      <c r="D103" t="str">
+        <v>608.4</v>
+      </c>
+      <c r="E103" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="str">
+        <v>0x73A4386890268E835d8d01598D06A44d47A489d8</v>
+      </c>
+      <c r="B104" t="str">
+        <v>582.12</v>
+      </c>
+      <c r="C104" t="str">
+        <v>582.12</v>
+      </c>
+      <c r="D104" t="str">
+        <v>0</v>
+      </c>
+      <c r="E104" t="str">
+        <v>608.4</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="str">
+        <v>0x16CaEA275D4F7cF454537b121915D92Bc5CB8C16</v>
+      </c>
+      <c r="B105" t="str">
+        <v>3.11</v>
+      </c>
+      <c r="C105" t="str">
+        <v>3.11</v>
+      </c>
+      <c r="D105" t="str">
+        <v>0</v>
+      </c>
+      <c r="E105" t="str">
+        <v>3.26</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="str">
+        <v>0x7011467e458B4cEEED928bac3E178Ce7EB892F2d</v>
+      </c>
+      <c r="B106" t="str">
+        <v>2,420.61</v>
+      </c>
+      <c r="C106" t="str">
+        <v>2,420.61</v>
+      </c>
+      <c r="D106" t="str">
+        <v>24.44</v>
+      </c>
+      <c r="E106" t="str">
+        <v>2,505.43</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="str">
+        <v>0xe9052daAC8667a27B38369aD37BEE63A8CD80Fc7</v>
+      </c>
+      <c r="B107" t="str">
+        <v>6,663.81</v>
+      </c>
+      <c r="C107" t="str">
+        <v>6,663.81</v>
+      </c>
+      <c r="D107" t="str">
+        <v>0</v>
+      </c>
+      <c r="E107" t="str">
+        <v>6,964.59</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="str">
+        <v>0x18fc6c299B7aA35C8f59537b4b67c23D93E782ea</v>
+      </c>
+      <c r="B108" t="str">
+        <v>39,478.54</v>
+      </c>
+      <c r="C108" t="str">
+        <v>39,478.54</v>
+      </c>
+      <c r="D108" t="str">
+        <v>0</v>
+      </c>
+      <c r="E108" t="str">
+        <v>41,260.46</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="str">
+        <v>0x98085d3327429Fc85f875e6baE8498EbC336eD97</v>
+      </c>
+      <c r="B109" t="str">
+        <v>1,913.62</v>
+      </c>
+      <c r="C109" t="str">
+        <v>1,913.62</v>
+      </c>
+      <c r="D109" t="str">
+        <v>2,000</v>
+      </c>
+      <c r="E109" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="str">
+        <v>0xF56A7C0C4f08356F9987Ef2C02f2034FD7F8608C</v>
+      </c>
+      <c r="B110" t="str">
+        <v>1,913.62</v>
+      </c>
+      <c r="C110" t="str">
+        <v>1,913.62</v>
+      </c>
+      <c r="D110" t="str">
+        <v>0</v>
+      </c>
+      <c r="E110" t="str">
+        <v>2,000</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="str">
+        <v>0x9D6B1E57daaE9A80411481801733B750d58782c0</v>
+      </c>
+      <c r="B111" t="str">
+        <v>299.32</v>
+      </c>
+      <c r="C111" t="str">
+        <v>299.32</v>
+      </c>
+      <c r="D111" t="str">
+        <v>312.84</v>
+      </c>
+      <c r="E111" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="str">
+        <v>0x094CAE95AB3744453Cf7Ce9251dFDD816C3C810E</v>
+      </c>
+      <c r="B112" t="str">
+        <v>257.88</v>
+      </c>
+      <c r="C112" t="str">
+        <v>257.88</v>
+      </c>
+      <c r="D112" t="str">
+        <v>132.67</v>
+      </c>
+      <c r="E112" t="str">
+        <v>136.86</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="str">
+        <v>0x74c0d21e8ffC5b83dce1A0BB6abCD061D071E85a</v>
+      </c>
+      <c r="B113" t="str">
+        <v>65,863.45</v>
+      </c>
+      <c r="C113" t="str">
+        <v>65,863.45</v>
+      </c>
+      <c r="D113" t="str">
+        <v>42,987.44</v>
+      </c>
+      <c r="E113" t="str">
+        <v>25,848.84</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="str">
+        <v>0xAcF543A44c24aAdF47B50e5cc05c628f3F2A5046</v>
+      </c>
+      <c r="B114" t="str">
+        <v>67,177.32</v>
+      </c>
+      <c r="C114" t="str">
+        <v>67,177.32</v>
+      </c>
+      <c r="D114" t="str">
+        <v>25,848.84</v>
+      </c>
+      <c r="E114" t="str">
+        <v>44,360.62</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="str">
+        <v>0xBBF6951084154eB73b77f9A9BA943e478bFa06c4</v>
+      </c>
+      <c r="B115" t="str">
+        <v>1,313.87</v>
+      </c>
+      <c r="C115" t="str">
+        <v>1,313.87</v>
+      </c>
+      <c r="D115" t="str">
+        <v>1,373.18</v>
+      </c>
+      <c r="E115" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="str">
+        <v>0x0fB3b0892619aF19B0a8016783f84EED26CfAE1E</v>
+      </c>
+      <c r="B116" t="str">
+        <v>139.38</v>
+      </c>
+      <c r="C116" t="str">
+        <v>139.38</v>
+      </c>
+      <c r="D116" t="str">
+        <v>145.68</v>
+      </c>
+      <c r="E116" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="str">
+        <v>0x4e300F965ACE7aBF11A53662419F9A2D27dE3B1d</v>
+      </c>
+      <c r="B117" t="str">
+        <v>139.38</v>
+      </c>
+      <c r="C117" t="str">
+        <v>139.38</v>
+      </c>
+      <c r="D117" t="str">
+        <v>0</v>
+      </c>
+      <c r="E117" t="str">
+        <v>145.68</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="str">
+        <v>0xD51a57fa53a22A063088950FfB92ddAFFa214141</v>
+      </c>
+      <c r="B118" t="str">
+        <v>24.26</v>
+      </c>
+      <c r="C118" t="str">
+        <v>24.26</v>
+      </c>
+      <c r="D118" t="str">
+        <v>25.36</v>
+      </c>
+      <c r="E118" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="str">
+        <v>0x04BA03baabB1e9221520fD9c31505a0d4c073167</v>
+      </c>
+      <c r="B119" t="str">
+        <v>24.26</v>
+      </c>
+      <c r="C119" t="str">
+        <v>24.26</v>
+      </c>
+      <c r="D119" t="str">
+        <v>0</v>
+      </c>
+      <c r="E119" t="str">
+        <v>25.36</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="str">
+        <v>0x5C9A07e59Bdc264d0579530b4e08338122833942</v>
+      </c>
+      <c r="B120" t="str">
+        <v>1,892.57</v>
+      </c>
+      <c r="C120" t="str">
+        <v>1,892.57</v>
+      </c>
+      <c r="D120" t="str">
+        <v>0</v>
+      </c>
+      <c r="E120" t="str">
+        <v>1,978</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="str">
+        <v>0x778Ba6B5ca859F7c72df96Bf13D274e35a78a356</v>
+      </c>
+      <c r="B121" t="str">
+        <v>32.34</v>
+      </c>
+      <c r="C121" t="str">
+        <v>32.34</v>
+      </c>
+      <c r="D121" t="str">
+        <v>33.81</v>
+      </c>
+      <c r="E121" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="str">
+        <v>0x9342fD3f10101019Cf9e6774640957fa1d7A78B2</v>
+      </c>
+      <c r="B122" t="str">
+        <v>810.6</v>
+      </c>
+      <c r="C122" t="str">
+        <v>810.6</v>
+      </c>
+      <c r="D122" t="str">
+        <v>847.19</v>
+      </c>
+      <c r="E122" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="str">
+        <v>0x212172E536d6c24f46D64F57f8FA64E201882146</v>
+      </c>
+      <c r="B123" t="str">
+        <v>28,693.15</v>
+      </c>
+      <c r="C123" t="str">
+        <v>28,693.15</v>
+      </c>
+      <c r="D123" t="str">
+        <v>29,988.26</v>
+      </c>
+      <c r="E123" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="str">
+        <v>0xa5d134A404FBAe6B980D22C2A1be268a1a995F6C</v>
+      </c>
+      <c r="B124" t="str">
+        <v>81.91</v>
+      </c>
+      <c r="C124" t="str">
+        <v>81.91</v>
+      </c>
+      <c r="D124" t="str">
+        <v>85.61</v>
+      </c>
+      <c r="E124" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="str">
+        <v>0x96f194Cf1c9e5eE23B4D96785791F468F6A9C98e</v>
+      </c>
+      <c r="B125" t="str">
+        <v>4,784.06</v>
+      </c>
+      <c r="C125" t="str">
+        <v>4,784.06</v>
+      </c>
+      <c r="D125" t="str">
+        <v>0</v>
+      </c>
+      <c r="E125" t="str">
+        <v>5,000</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="str">
+        <v>0x430cB4360cE341a6Ad0Dfa18b9aD1Ae2cFa9AD18</v>
+      </c>
+      <c r="B126" t="str">
+        <v>1,808.23</v>
+      </c>
+      <c r="C126" t="str">
+        <v>1,808.23</v>
+      </c>
+      <c r="D126" t="str">
+        <v>0</v>
+      </c>
+      <c r="E126" t="str">
+        <v>1,889.85</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="str">
+        <v>0x7a8b381f5E107dc45E3888e7AaBF1E9aB464a1A8</v>
+      </c>
+      <c r="B127" t="str">
+        <v>301.16</v>
+      </c>
+      <c r="C127" t="str">
+        <v>301.16</v>
+      </c>
+      <c r="D127" t="str">
+        <v>314.76</v>
+      </c>
+      <c r="E127" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="str">
+        <v>0x040f62A18EB5D5ca87A08E41A22D004ee7A26380</v>
+      </c>
+      <c r="B128" t="str">
+        <v>69.23</v>
+      </c>
+      <c r="C128" t="str">
+        <v>69.23</v>
+      </c>
+      <c r="D128" t="str">
+        <v>0</v>
+      </c>
+      <c r="E128" t="str">
+        <v>72.36</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="str">
+        <v>0xf85F765B52C7c319287d669D8682eC33eA52Bca9</v>
+      </c>
+      <c r="B129" t="str">
+        <v>394.83</v>
+      </c>
+      <c r="C129" t="str">
+        <v>394.83</v>
+      </c>
+      <c r="D129" t="str">
+        <v>151.9</v>
+      </c>
+      <c r="E129" t="str">
+        <v>260.76</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="str">
+        <v>0x26763e975D773f46E8bA6AF80C09D9C90A07E14D</v>
+      </c>
+      <c r="B130" t="str">
+        <v>145.33</v>
+      </c>
+      <c r="C130" t="str">
+        <v>145.33</v>
+      </c>
+      <c r="D130" t="str">
+        <v>0</v>
+      </c>
+      <c r="E130" t="str">
+        <v>151.9</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="str">
+        <v>0x3010A4E7ce5c99208900c218d0375bfEfE7De269</v>
+      </c>
+      <c r="B131" t="str">
+        <v>2,870.43</v>
+      </c>
+      <c r="C131" t="str">
+        <v>2,870.43</v>
+      </c>
+      <c r="D131" t="str">
+        <v>2,500</v>
+      </c>
+      <c r="E131" t="str">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="str">
+        <v>0xFb55bcB2E843Cc2dA95c48273eA89F167Faf7b93</v>
+      </c>
+      <c r="B132" t="str">
+        <v>2,870.43</v>
+      </c>
+      <c r="C132" t="str">
+        <v>2,870.43</v>
+      </c>
+      <c r="D132" t="str">
+        <v>500</v>
+      </c>
+      <c r="E132" t="str">
+        <v>2,500</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="str">
+        <v>0xA2cfCc9E68d9138ED4eacF9b7E2141D9B41C6eCF</v>
+      </c>
+      <c r="B133" t="str">
+        <v>28.75</v>
+      </c>
+      <c r="C133" t="str">
+        <v>28.75</v>
+      </c>
+      <c r="D133" t="str">
+        <v>30.05</v>
+      </c>
+      <c r="E133" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="str">
+        <v>0x48f5880a56dC2b8e123aB8CddD58521631332e36</v>
+      </c>
+      <c r="B134" t="str">
+        <v>28.75</v>
+      </c>
+      <c r="C134" t="str">
+        <v>28.75</v>
+      </c>
+      <c r="D134" t="str">
+        <v>0</v>
+      </c>
+      <c r="E134" t="str">
+        <v>30.05</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="str">
+        <v>0xDdF9E0547714839685900403611875EbB18C6236</v>
+      </c>
+      <c r="B135" t="str">
+        <v>54.09</v>
+      </c>
+      <c r="C135" t="str">
+        <v>54.09</v>
+      </c>
+      <c r="D135" t="str">
+        <v>0</v>
+      </c>
+      <c r="E135" t="str">
+        <v>56.54</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="str">
+        <v>0x79622cD63ff61A74613fAFB805B7f32D3cf78A95</v>
+      </c>
+      <c r="B136" t="str">
+        <v>26,495.66</v>
+      </c>
+      <c r="C136" t="str">
+        <v>26,495.66</v>
+      </c>
+      <c r="D136" t="str">
+        <v>0</v>
+      </c>
+      <c r="E136" t="str">
+        <v>27,691.58</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="str">
+        <v>0x95814b787287141C80e9917Ee9eC9B2F89275629</v>
+      </c>
+      <c r="B137" t="str">
+        <v>9,495.28</v>
+      </c>
+      <c r="C137" t="str">
+        <v>9,495.28</v>
+      </c>
+      <c r="D137" t="str">
+        <v>9,923.87</v>
+      </c>
+      <c r="E137" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="str">
+        <v>0x70a358970c122dE0ebb3f9c0b8704E71c2f69352</v>
+      </c>
+      <c r="B138" t="str">
+        <v>10.7</v>
+      </c>
+      <c r="C138" t="str">
+        <v>10.7</v>
+      </c>
+      <c r="D138" t="str">
+        <v>0</v>
+      </c>
+      <c r="E138" t="str">
+        <v>11.19</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="str">
+        <v>0xbdAb516d352Adf142207EA2F7749c4a7e0543a55</v>
+      </c>
+      <c r="B139" t="str">
+        <v>2,238.71</v>
+      </c>
+      <c r="C139" t="str">
+        <v>2,238.71</v>
+      </c>
+      <c r="D139" t="str">
+        <v>2,339.76</v>
+      </c>
+      <c r="E139" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="str">
+        <v>0x6BF81D0d4f4e606C3cB09C45f6FA29f8743c72DE</v>
+      </c>
+      <c r="B140" t="str">
+        <v>0</v>
+      </c>
+      <c r="C140" t="str">
+        <v>3,652.3</v>
+      </c>
+      <c r="D140" t="str">
+        <v>0</v>
+      </c>
+      <c r="E140" t="str">
+        <v>3,817.16</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="str">
+        <v>0xf4f611e4f1e8C6E21B54d4A38687C44477cF4eA2</v>
+      </c>
+      <c r="B141" t="str">
+        <v>6.07</v>
+      </c>
+      <c r="C141" t="str">
+        <v>6.07</v>
+      </c>
+      <c r="D141" t="str">
+        <v>6.35</v>
+      </c>
+      <c r="E141" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="str">
+        <v>0x3d1F678EBd71CA033f21D6B1B5B0781a66537447</v>
+      </c>
+      <c r="B142" t="str">
+        <v>1,099.01</v>
+      </c>
+      <c r="C142" t="str">
+        <v>1,099.01</v>
+      </c>
+      <c r="D142" t="str">
+        <v>0</v>
+      </c>
+      <c r="E142" t="str">
+        <v>1,148.62</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="str">
+        <v>0x9fF7d51Cf6a3A12F2Cdd36035827037a35A4B139</v>
+      </c>
+      <c r="B143" t="str">
+        <v>1,237.08</v>
+      </c>
+      <c r="C143" t="str">
+        <v>1,237.08</v>
+      </c>
+      <c r="D143" t="str">
+        <v>0</v>
+      </c>
+      <c r="E143" t="str">
+        <v>1,292.92</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="str">
+        <v>0xeb9Ea287a5BD59731C6fbDEfd9e81dAa4Dc7eB11</v>
+      </c>
+      <c r="B144" t="str">
+        <v>119.5</v>
+      </c>
+      <c r="C144" t="str">
+        <v>119.5</v>
+      </c>
+      <c r="D144" t="str">
+        <v>0</v>
+      </c>
+      <c r="E144" t="str">
+        <v>124.9</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="str">
+        <v>0xd2938A7fCa560A5b6630aaf12d817E5f146cddA4</v>
+      </c>
+      <c r="B145" t="str">
+        <v>707.65</v>
+      </c>
+      <c r="C145" t="str">
+        <v>707.65</v>
+      </c>
+      <c r="D145" t="str">
+        <v>0</v>
+      </c>
+      <c r="E145" t="str">
+        <v>739.6</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="str">
+        <v>0x280a3925f1fAD53B5a263fFc0028Fbab9abE6131</v>
+      </c>
+      <c r="B146" t="str">
+        <v>4,800.32</v>
+      </c>
+      <c r="C146" t="str">
+        <v>4,800.32</v>
+      </c>
+      <c r="D146" t="str">
+        <v>5,016.99</v>
+      </c>
+      <c r="E146" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="str">
+        <v>0xa427746a2606c82afaa69cE757E0705c2c8081a1</v>
+      </c>
+      <c r="B147" t="str">
+        <v>4,800.32</v>
+      </c>
+      <c r="C147" t="str">
+        <v>4,800.32</v>
+      </c>
+      <c r="D147" t="str">
+        <v>0</v>
+      </c>
+      <c r="E147" t="str">
+        <v>5,016.99</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="str">
+        <v>0x8D126B25f7e648938F95A97261C4A4Cf48D0df17</v>
+      </c>
+      <c r="B148" t="str">
+        <v>3,103.75</v>
+      </c>
+      <c r="C148" t="str">
+        <v>3,103.75</v>
+      </c>
+      <c r="D148" t="str">
+        <v>3,243.85</v>
+      </c>
+      <c r="E148" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="str">
+        <v>0xd9a2078c93792cd2f968737092ae7da44eAF64D0</v>
+      </c>
+      <c r="B149" t="str">
+        <v>3,103.75</v>
+      </c>
+      <c r="C149" t="str">
+        <v>3,103.75</v>
+      </c>
+      <c r="D149" t="str">
+        <v>0</v>
+      </c>
+      <c r="E149" t="str">
+        <v>3,243.85</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="str">
+        <v>0xBcb9C22A0b6479E1519fC26a9499FE12AeA0c848</v>
+      </c>
+      <c r="B150" t="str">
+        <v>62.01</v>
+      </c>
+      <c r="C150" t="str">
+        <v>62.01</v>
+      </c>
+      <c r="D150" t="str">
+        <v>64.81</v>
+      </c>
+      <c r="E150" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="str">
+        <v>0xfC8B5e50e7aa48f71F422339e4c0040f7779C714</v>
+      </c>
+      <c r="B151" t="str">
+        <v>2,566.59</v>
+      </c>
+      <c r="C151" t="str">
+        <v>2,566.59</v>
+      </c>
+      <c r="D151" t="str">
+        <v>2,682.44</v>
+      </c>
+      <c r="E151" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="str">
+        <v>0xd9C0e53199290dF3BFB223033f3eb6C16429af0e</v>
+      </c>
+      <c r="B152" t="str">
+        <v>4,106.16</v>
+      </c>
+      <c r="C152" t="str">
+        <v>4,106.16</v>
+      </c>
+      <c r="D152" t="str">
+        <v>0</v>
+      </c>
+      <c r="E152" t="str">
+        <v>4,291.5</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="str">
+        <v>0x4FDC77D8fFDD4F8a3CbFc3De2886DfEE1FD5112f</v>
+      </c>
+      <c r="B153" t="str">
+        <v>0</v>
+      </c>
+      <c r="C153" t="str">
+        <v>308.43</v>
+      </c>
+      <c r="D153" t="str">
+        <v>322.36</v>
+      </c>
+      <c r="E153" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="str">
+        <v>0x260250876501b886EB540553d1f5306FAce6E393</v>
+      </c>
+      <c r="B154" t="str">
+        <v>50.23</v>
+      </c>
+      <c r="C154" t="str">
+        <v>50.23</v>
+      </c>
+      <c r="D154" t="str">
+        <v>52.5</v>
+      </c>
+      <c r="E154" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="str">
+        <v>0x9f65AE97F174c6849297dF848651C520cC145A69</v>
+      </c>
+      <c r="B155" t="str">
+        <v>50.23</v>
+      </c>
+      <c r="C155" t="str">
+        <v>50.23</v>
+      </c>
+      <c r="D155" t="str">
+        <v>0</v>
+      </c>
+      <c r="E155" t="str">
+        <v>52.5</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="str">
+        <v>0xe5C5B9C648a3e66A2A7b8a3f2dA48e76e8309A2C</v>
+      </c>
+      <c r="B156" t="str">
+        <v>1,923.96</v>
+      </c>
+      <c r="C156" t="str">
+        <v>1,923.96</v>
+      </c>
+      <c r="D156" t="str">
+        <v>0</v>
+      </c>
+      <c r="E156" t="str">
+        <v>2,010.81</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="str">
+        <v>0xF9c0f097d88E0284ac932E3090279fDc5bfe1B55</v>
+      </c>
+      <c r="B157" t="str">
+        <v>28,427.29</v>
+      </c>
+      <c r="C157" t="str">
+        <v>28,427.29</v>
+      </c>
+      <c r="D157" t="str">
+        <v>0</v>
+      </c>
+      <c r="E157" t="str">
+        <v>29,710.4</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="str">
+        <v>0x48A7209DD07Bc7409bF3f61820E1Ee9409F462e9</v>
+      </c>
+      <c r="B158" t="str">
+        <v>1,260.55</v>
+      </c>
+      <c r="C158" t="str">
+        <v>1,260.55</v>
+      </c>
+      <c r="D158" t="str">
+        <v>0</v>
+      </c>
+      <c r="E158" t="str">
+        <v>1,317.45</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="str">
+        <v>0xEbbabF54e68354253E41f2D0F1C543FEc5Bcfffa</v>
+      </c>
+      <c r="B159" t="str">
+        <v>202,195.78</v>
+      </c>
+      <c r="C159" t="str">
+        <v>202,195.78</v>
+      </c>
+      <c r="D159" t="str">
+        <v>99,397.31</v>
+      </c>
+      <c r="E159" t="str">
+        <v>111,924.84</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="str">
+        <v>0xd5d071b3A56381308F4B9Fa560AAd7876Df292c7</v>
+      </c>
+      <c r="B160" t="str">
+        <v>190,233.23</v>
+      </c>
+      <c r="C160" t="str">
+        <v>190,233.23</v>
+      </c>
+      <c r="D160" t="str">
+        <v>99,422.34</v>
+      </c>
+      <c r="E160" t="str">
+        <v>99,397.31</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="str">
+        <v>0xF2Aa3A5Df3Af1eD5ff72631A8bcFF0F0AfE060eC</v>
+      </c>
+      <c r="B161" t="str">
+        <v>1,293.35</v>
+      </c>
+      <c r="C161" t="str">
+        <v>1,293.35</v>
+      </c>
+      <c r="D161" t="str">
+        <v>678.6</v>
+      </c>
+      <c r="E161" t="str">
+        <v>673.13</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="str">
+        <v>0xc01bdF2F593bbbFe1e15540c818c57f919466D7B</v>
+      </c>
+      <c r="B162" t="str">
+        <v>1,410.5</v>
+      </c>
+      <c r="C162" t="str">
+        <v>1,410.5</v>
+      </c>
+      <c r="D162" t="str">
+        <v>673.13</v>
+      </c>
+      <c r="E162" t="str">
+        <v>801.04</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="str">
+        <v>0xE3060D70A15f2EdFb390D66e60467Da6F5ECA1C7</v>
+      </c>
+      <c r="B163" t="str">
+        <v>3,672.39</v>
+      </c>
+      <c r="C163" t="str">
+        <v>3,672.39</v>
+      </c>
+      <c r="D163" t="str">
+        <v>580.49</v>
+      </c>
+      <c r="E163" t="str">
+        <v>3,257.66</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="str">
+        <v>0xD7Be7655070f986B3E311EE04cc9aa87Cd11ab5d</v>
+      </c>
+      <c r="B164" t="str">
+        <v>3,672.39</v>
+      </c>
+      <c r="C164" t="str">
+        <v>3,672.39</v>
+      </c>
+      <c r="D164" t="str">
+        <v>3,257.66</v>
+      </c>
+      <c r="E164" t="str">
+        <v>580.49</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="str">
+        <v>0xA678C16Ecca94a90764973FedEbE71d524FAfF84</v>
+      </c>
+      <c r="B165" t="str">
+        <v>5,120.59</v>
+      </c>
+      <c r="C165" t="str">
+        <v>5,120.59</v>
+      </c>
+      <c r="D165" t="str">
+        <v>0</v>
+      </c>
+      <c r="E165" t="str">
+        <v>5,351.72</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="str">
+        <v>0xf2F71fC776df3a2F6Df39D7010468fBce89CF9D8</v>
+      </c>
+      <c r="B166" t="str">
+        <v>124.39</v>
+      </c>
+      <c r="C166" t="str">
+        <v>124.39</v>
+      </c>
+      <c r="D166" t="str">
+        <v>0</v>
+      </c>
+      <c r="E166" t="str">
+        <v>130.01</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="str">
+        <v>0xC44b6fcf320C7A15f288D3792E5BBF7D770e25c4</v>
+      </c>
+      <c r="B167" t="str">
+        <v>31.1</v>
+      </c>
+      <c r="C167" t="str">
+        <v>31.1</v>
+      </c>
+      <c r="D167" t="str">
+        <v>32.51</v>
+      </c>
+      <c r="E167" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="str">
+        <v>0x9C0557216e919eDaCCc56037c66A5fAC1D41D82a</v>
+      </c>
+      <c r="B168" t="str">
+        <v>31.1</v>
+      </c>
+      <c r="C168" t="str">
+        <v>31.1</v>
+      </c>
+      <c r="D168" t="str">
+        <v>0</v>
+      </c>
+      <c r="E168" t="str">
+        <v>32.51</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="str">
+        <v>0x99D5f1d103A892A191aCF6897CE4b65f2F627a28</v>
+      </c>
+      <c r="B169" t="str">
+        <v>310.36</v>
+      </c>
+      <c r="C169" t="str">
+        <v>310.36</v>
+      </c>
+      <c r="D169" t="str">
+        <v>324.37</v>
+      </c>
+      <c r="E169" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="str">
+        <v>0x4E17E118dFfd16659cA02086aA34476fe6350b20</v>
+      </c>
+      <c r="B170" t="str">
+        <v>249.49</v>
+      </c>
+      <c r="C170" t="str">
+        <v>249.49</v>
+      </c>
+      <c r="D170" t="str">
+        <v>260.76</v>
+      </c>
+      <c r="E170" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="str">
+        <v>0x73755c77A68017d6E755Ac0cE9df5EA7c2aF8F75</v>
+      </c>
+      <c r="B171" t="str">
+        <v>0</v>
+      </c>
+      <c r="C171" t="str">
+        <v>478.4</v>
+      </c>
+      <c r="D171" t="str">
+        <v>0</v>
+      </c>
+      <c r="E171" t="str">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="str">
+        <v>0x7aa90dE22D64831e54DA455A90621560f1bC97a2</v>
+      </c>
+      <c r="B172" t="str">
+        <v>188.92</v>
+      </c>
+      <c r="C172" t="str">
+        <v>188.92</v>
+      </c>
+      <c r="D172" t="str">
+        <v>197.45</v>
+      </c>
+      <c r="E172" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="str">
+        <v>0x2373654B6a1564c5BdA4D28dDeF1827D66d7EA2b</v>
+      </c>
+      <c r="B173" t="str">
+        <v>0</v>
+      </c>
+      <c r="C173" t="str">
+        <v>188.92</v>
+      </c>
+      <c r="D173" t="str">
+        <v>0</v>
+      </c>
+      <c r="E173" t="str">
+        <v>197.45</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="str">
+        <v>0x7aD2809008E5DA0c33A72f9144e7970a996D5B6D</v>
+      </c>
+      <c r="B174" t="str">
+        <v>73.93</v>
+      </c>
+      <c r="C174" t="str">
+        <v>73.93</v>
+      </c>
+      <c r="D174" t="str">
+        <v>0</v>
+      </c>
+      <c r="E174" t="str">
+        <v>77.27</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="str">
+        <v>0xA742150Bb2b4e5DfCC4E6df0E577237Fceb797b2</v>
+      </c>
+      <c r="B175" t="str">
+        <v>0</v>
+      </c>
+      <c r="C175" t="str">
+        <v>42.9</v>
+      </c>
+      <c r="D175" t="str">
+        <v>0</v>
+      </c>
+      <c r="E175" t="str">
+        <v>44.84</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="str">
+        <v>0x4CEbE974145E6796dB356F3689082D2d1eEf02Bf</v>
+      </c>
+      <c r="B176" t="str">
+        <v>111.44</v>
+      </c>
+      <c r="C176" t="str">
+        <v>111.44</v>
+      </c>
+      <c r="D176" t="str">
+        <v>116.47</v>
+      </c>
+      <c r="E176" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="str">
+        <v>0x9137e3E86cFf5736277B418E41449CC3428F5317</v>
+      </c>
+      <c r="B177" t="str">
+        <v>111.44</v>
+      </c>
+      <c r="C177" t="str">
+        <v>111.44</v>
+      </c>
+      <c r="D177" t="str">
+        <v>0</v>
+      </c>
+      <c r="E177" t="str">
+        <v>116.47</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="str">
+        <v>0x496e577Baa29fb09B3e281514C56F319b6e0A2C7</v>
+      </c>
+      <c r="B178" t="str">
+        <v>157.81</v>
+      </c>
+      <c r="C178" t="str">
+        <v>157.81</v>
+      </c>
+      <c r="D178" t="str">
+        <v>164.94</v>
+      </c>
+      <c r="E178" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="str">
+        <v>0x9964C7C7EB99E6F70dFef18c90D7526a0C13b46F</v>
+      </c>
+      <c r="B179" t="str">
+        <v>157.81</v>
+      </c>
+      <c r="C179" t="str">
+        <v>157.81</v>
+      </c>
+      <c r="D179" t="str">
+        <v>0</v>
+      </c>
+      <c r="E179" t="str">
+        <v>164.94</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="str">
+        <v>0x942E746C384bec88Dfa6164e8d699858E9988FeB</v>
+      </c>
+      <c r="B180" t="str">
+        <v>627.4</v>
+      </c>
+      <c r="C180" t="str">
+        <v>627.4</v>
+      </c>
+      <c r="D180" t="str">
+        <v>655.72</v>
+      </c>
+      <c r="E180" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="str">
+        <v>0xf0eeE0837e8F4feaC444412991f7005B8dFFa305</v>
+      </c>
+      <c r="B181" t="str">
+        <v>627.4</v>
+      </c>
+      <c r="C181" t="str">
+        <v>627.4</v>
+      </c>
+      <c r="D181" t="str">
+        <v>0</v>
+      </c>
+      <c r="E181" t="str">
+        <v>655.72</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="str">
+        <v>0x212A3caD6d1572C706959d2aeF63071e61914bf2</v>
+      </c>
+      <c r="B182" t="str">
+        <v>603.26</v>
+      </c>
+      <c r="C182" t="str">
+        <v>603.26</v>
+      </c>
+      <c r="D182" t="str">
+        <v>0</v>
+      </c>
+      <c r="E182" t="str">
+        <v>630.49</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="str">
+        <v>0x1A24A8CDa46ACac40606af1D233dAfF9AEe66e2f</v>
+      </c>
+      <c r="B183" t="str">
+        <v>96.76</v>
+      </c>
+      <c r="C183" t="str">
+        <v>96.76</v>
+      </c>
+      <c r="D183" t="str">
+        <v>0</v>
+      </c>
+      <c r="E183" t="str">
+        <v>101.13</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="str">
+        <v>0xFb9Fa9E9276D1631fc4f72c32c19628a8d8a3935</v>
+      </c>
+      <c r="B184" t="str">
+        <v>1,252.19</v>
+      </c>
+      <c r="C184" t="str">
+        <v>1,252.19</v>
+      </c>
+      <c r="D184" t="str">
+        <v>1,308.71</v>
+      </c>
+      <c r="E184" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="str">
+        <v>0xd0bC9CB19A72c6DDE6206d302E049D6E0496a453</v>
+      </c>
+      <c r="B185" t="str">
+        <v>1,252.19</v>
+      </c>
+      <c r="C185" t="str">
+        <v>1,252.19</v>
+      </c>
+      <c r="D185" t="str">
+        <v>0</v>
+      </c>
+      <c r="E185" t="str">
+        <v>1,308.71</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="str">
+        <v>0x0c9168A60476c84DeD650f13837892725D25DeB1</v>
+      </c>
+      <c r="B186" t="str">
+        <v>628.3</v>
+      </c>
+      <c r="C186" t="str">
+        <v>628.3</v>
+      </c>
+      <c r="D186" t="str">
+        <v>0</v>
+      </c>
+      <c r="E186" t="str">
+        <v>656.66</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="str">
+        <v>0x175780bC4d0A1bc28c46C3E71130C092790E7576</v>
+      </c>
+      <c r="B187" t="str">
+        <v>279.33</v>
+      </c>
+      <c r="C187" t="str">
+        <v>279.33</v>
+      </c>
+      <c r="D187" t="str">
+        <v>291.94</v>
+      </c>
+      <c r="E187" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="str">
+        <v>0xB19c1b3cEc4c5bD6DCA220A4f59de9EC681e9211</v>
+      </c>
+      <c r="B188" t="str">
+        <v>0</v>
+      </c>
+      <c r="C188" t="str">
+        <v>279.33</v>
+      </c>
+      <c r="D188" t="str">
+        <v>0</v>
+      </c>
+      <c r="E188" t="str">
+        <v>291.94</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="str">
+        <v>0xD44E29759A73d29F7887702F864406b16612BF5e</v>
+      </c>
+      <c r="B189" t="str">
+        <v>0</v>
+      </c>
+      <c r="C189" t="str">
+        <v>1,525.91</v>
+      </c>
+      <c r="D189" t="str">
+        <v>0</v>
+      </c>
+      <c r="E189" t="str">
+        <v>1,594.79</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="str">
+        <v>0x8EA76c885918FA6f548501b5c4357aff43204CD0</v>
+      </c>
+      <c r="B190" t="str">
+        <v>6.88</v>
+      </c>
+      <c r="C190" t="str">
+        <v>6.88</v>
+      </c>
+      <c r="D190" t="str">
+        <v>7.2</v>
+      </c>
+      <c r="E190" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="str">
+        <v>0xd4e63B2004b55E2aE3c84451951D28dE1C5226Af</v>
+      </c>
+      <c r="B191" t="str">
+        <v>52.57</v>
+      </c>
+      <c r="C191" t="str">
+        <v>52.57</v>
+      </c>
+      <c r="D191" t="str">
+        <v>0</v>
+      </c>
+      <c r="E191" t="str">
+        <v>54.95</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="str">
+        <v>0xB6e85e12331BdEA6fF03b25d3dE68a892C99C5D4</v>
+      </c>
+      <c r="B192" t="str">
+        <v>101.13</v>
+      </c>
+      <c r="C192" t="str">
+        <v>101.13</v>
+      </c>
+      <c r="D192" t="str">
+        <v>0</v>
+      </c>
+      <c r="E192" t="str">
+        <v>105.7</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="str">
+        <v>0x9D89f9451C4B7e04bd58616dbC72e924088AFF21</v>
+      </c>
+      <c r="B193" t="str">
+        <v>143.52</v>
+      </c>
+      <c r="C193" t="str">
+        <v>143.52</v>
+      </c>
+      <c r="D193" t="str">
+        <v>0</v>
+      </c>
+      <c r="E193" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="str">
+        <v>0xfaac07aC0C2769E304c57d6348BeEF832675b225</v>
+      </c>
+      <c r="B194" t="str">
+        <v>433.35</v>
+      </c>
+      <c r="C194" t="str">
+        <v>433.35</v>
+      </c>
+      <c r="D194" t="str">
+        <v>0</v>
+      </c>
+      <c r="E194" t="str">
+        <v>452.91</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="str">
+        <v>0x9f0bE4E742e7d98a8837388b83d508d4A483AECF</v>
+      </c>
+      <c r="B195" t="str">
+        <v>127.05</v>
+      </c>
+      <c r="C195" t="str">
+        <v>127.05</v>
+      </c>
+      <c r="D195" t="str">
+        <v>132.79</v>
+      </c>
+      <c r="E195" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="str">
+        <v>0x0feD39AC6093e042825EfE8862f37dc8425B8f74</v>
+      </c>
+      <c r="B196" t="str">
+        <v>445.27</v>
+      </c>
+      <c r="C196" t="str">
+        <v>445.27</v>
+      </c>
+      <c r="D196" t="str">
+        <v>0</v>
+      </c>
+      <c r="E196" t="str">
+        <v>465.37</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="str">
+        <v>0x9c6E23aC65D33b747B8c56C04db77d836c41Faf5</v>
+      </c>
+      <c r="B197" t="str">
+        <v>126.66</v>
+      </c>
+      <c r="C197" t="str">
+        <v>126.66</v>
+      </c>
+      <c r="D197" t="str">
+        <v>0</v>
+      </c>
+      <c r="E197" t="str">
+        <v>132.38</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="str">
+        <v>0x091D2bf74f675Df1d72eD6E07bCB693D56a4163c</v>
+      </c>
+      <c r="B198" t="str">
+        <v>0</v>
+      </c>
+      <c r="C198" t="str">
+        <v>2,511.96</v>
+      </c>
+      <c r="D198" t="str">
+        <v>2,625.35</v>
+      </c>
+      <c r="E198" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="str">
+        <v>Total</v>
+      </c>
+      <c r="B199" t="str">
+        <v>3,187,685.55</v>
+      </c>
+      <c r="C199" t="str">
+        <v>3,205,127.24</v>
+      </c>
+      <c r="D199" t="str">
+        <v>1,622,298.67</v>
+      </c>
+      <c r="E199" t="str">
+        <v>1,727,497.03</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:E199"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E327"/>

</xml_diff>